<commit_message>
Update to naming of chords within scales.
Names have been shortened to match with convention.  Dominant chords are
now simply X7, e.g. G7 is the 5th chord of C Ionian (Major).
</commit_message>
<xml_diff>
--- a/Shredsheets.xlsx
+++ b/Shredsheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Shredsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557E4630-270A-4602-B7D6-85361FC6928C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1C5ABF-65D0-498B-A549-043966DC2F36}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="197">
   <si>
     <t>Ionian</t>
   </si>
@@ -608,9 +608,6 @@
   </si>
   <si>
     <t>m7 dim</t>
-  </si>
-  <si>
-    <t>M7 dom</t>
   </si>
   <si>
     <t>5 add 7</t>
@@ -1846,6 +1843,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1856,18 +1865,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3044,7 +3041,7 @@
   <dimension ref="B1:AF41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3173,15 +3170,15 @@
       <c r="AF3" s="63"/>
     </row>
     <row r="4" spans="2:32" s="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="132" t="str">
+      <c r="B4" s="128" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B19 = "Ionian (Major)", B10 &amp; " Major", IF(B19 = "Aolian (Minor)", B10 &amp; " Minor", B10 &amp; " " &amp; B19)), "#", "♯"), "b", "♭")</f>
         <v>C Major</v>
       </c>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
       <c r="J4" s="105">
         <f t="shared" ref="J4:P4" si="0">IF(J8 = "", "", IF(J5 = 0, F$1, J5))</f>
         <v>1</v>
@@ -3210,20 +3207,20 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="AE4" s="127" t="s">
+      <c r="AE4" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="AF4" s="128" t="b">
+      <c r="AF4" s="132" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:32" s="64" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
       <c r="J5" s="107">
         <f>IFERROR(HLOOKUP(F$1, Model!$Q$1:$X$17, MATCH($B$19, Model!$Q$2:$Q$20, 0) + 1), F$1)</f>
         <v>0</v>
@@ -3252,16 +3249,16 @@
         <f>IFERROR(HLOOKUP(L$1, Model!$Q$1:$X$17, MATCH($B$19, Model!$Q$2:$Q$20, 0) + 1), L$1)</f>
         <v>0</v>
       </c>
-      <c r="AE5" s="127"/>
-      <c r="AF5" s="128"/>
+      <c r="AE5" s="131"/>
+      <c r="AF5" s="132"/>
     </row>
     <row r="6" spans="2:32" s="64" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="132"/>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
+      <c r="B6" s="128"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
       <c r="J6" s="123" t="str">
         <f>IF(J$4="","", J$8 &amp; IFERROR(HLOOKUP(F$1, Model!$Q$20:$X$36, MATCH($B$19, Model!$Q$2:$Q$20, 0) + 1), F$1))</f>
         <v>CM7</v>
@@ -3280,7 +3277,7 @@
       </c>
       <c r="N6" s="123" t="str">
         <f>IF(N$4="","", N$8 &amp; IFERROR(HLOOKUP(J$1, Model!$Q$20:$X$36, MATCH($B$19, Model!$Q$2:$Q$20, 0) + 1), J$1))</f>
-        <v>GM7 dom</v>
+        <v>G7</v>
       </c>
       <c r="O6" s="123" t="str">
         <f>IF(O$4="","", O$8 &amp; IFERROR(HLOOKUP(K$1, Model!$Q$20:$X$36, MATCH($B$19, Model!$Q$2:$Q$20, 0) + 1), K$1))</f>
@@ -3290,16 +3287,16 @@
         <f>IF(P$4="","", P$8 &amp; IFERROR(HLOOKUP(L$1, Model!$Q$20:$X$36, MATCH($B$19, Model!$Q$2:$Q$20, 0) + 1), L$1))</f>
         <v>Bm7 dim</v>
       </c>
-      <c r="AE6" s="127"/>
-      <c r="AF6" s="128"/>
+      <c r="AE6" s="131"/>
+      <c r="AF6" s="132"/>
     </row>
     <row r="7" spans="2:32" s="65" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="128"/>
       <c r="J7" s="108" t="str">
         <f t="shared" ref="J7:P7" si="1">IF(J4="","",J3)</f>
         <v>Tonic</v>
@@ -3328,20 +3325,20 @@
         <f t="shared" si="1"/>
         <v>Leading Tone</v>
       </c>
-      <c r="AE7" s="127"/>
-      <c r="AF7" s="128"/>
+      <c r="AE7" s="131"/>
+      <c r="AF7" s="132"/>
     </row>
     <row r="8" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
-      <c r="H8" s="133" t="s">
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="133"/>
+      <c r="I8" s="129"/>
       <c r="J8" s="80" t="str">
         <f>Model!J24</f>
         <v>C</v>
@@ -3370,11 +3367,11 @@
         <f>IF(Model!O22=0, "", Model!P24)</f>
         <v>B</v>
       </c>
-      <c r="S8" s="134" t="s">
+      <c r="S8" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="134"/>
-      <c r="U8" s="134"/>
+      <c r="T8" s="130"/>
+      <c r="U8" s="130"/>
       <c r="V8" s="111" t="str">
         <f>IF(Model!J22=1, "h", IF(Model!J22=2, "W", IF(Model!J22=3, "W+h", IF(Model!J22=4, "WW", IF(Model!J22=0, "", Model!J22)))))</f>
         <v>W</v>
@@ -3403,10 +3400,10 @@
         <f>IF(Model!P22=1, "h", IF(Model!P22=2, "W", IF(Model!P22=3, "W+h",IF(Model!P22=4, "WW", IF(Model!P22=0, "", Model!P22)))))</f>
         <v>h</v>
       </c>
-      <c r="AE8" s="130" t="s">
+      <c r="AE8" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="AF8" s="130"/>
+      <c r="AF8" s="134"/>
     </row>
     <row r="9" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="104" t="s">
@@ -3524,7 +3521,7 @@
       </c>
     </row>
     <row r="10" spans="2:32" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="129" t="s">
+      <c r="B10" s="133" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="68" t="s">
@@ -3642,7 +3639,7 @@
       </c>
     </row>
     <row r="11" spans="2:32" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="129"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="68" t="s">
         <v>16</v>
       </c>
@@ -3758,7 +3755,7 @@
       </c>
     </row>
     <row r="12" spans="2:32" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="129"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="68" t="s">
         <v>15</v>
       </c>
@@ -3874,7 +3871,7 @@
       </c>
     </row>
     <row r="13" spans="2:32" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="129"/>
+      <c r="B13" s="133"/>
       <c r="C13" s="68" t="s">
         <v>12</v>
       </c>
@@ -3990,7 +3987,7 @@
       </c>
     </row>
     <row r="14" spans="2:32" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="129"/>
+      <c r="B14" s="133"/>
       <c r="C14" s="68" t="s">
         <v>14</v>
       </c>
@@ -4106,7 +4103,7 @@
       </c>
     </row>
     <row r="15" spans="2:32" s="67" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="127" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="68" t="s">
@@ -4224,7 +4221,7 @@
       </c>
     </row>
     <row r="16" spans="2:32" s="67" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="131"/>
+      <c r="B16" s="127"/>
       <c r="C16" s="69" t="s">
         <v>16</v>
       </c>
@@ -4336,7 +4333,7 @@
       <c r="AF16" s="99"/>
     </row>
     <row r="17" spans="2:32" s="67" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="131"/>
+      <c r="B17" s="127"/>
       <c r="C17" s="69" t="s">
         <v>15</v>
       </c>
@@ -4448,7 +4445,7 @@
       <c r="AF17" s="99"/>
     </row>
     <row r="18" spans="2:32" s="67" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="131"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="69" t="s">
         <v>12</v>
       </c>
@@ -4773,15 +4770,15 @@
       <c r="AF22" s="64"/>
     </row>
     <row r="23" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="132" t="str">
+      <c r="B23" s="128" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B38 = "Ionian (Major)", B29 &amp; " Major", IF(B38 = "Aolian (Minor)", B29 &amp; " Minor", B29 &amp; " " &amp; B38)), "#", "♯"), "b", "♭")</f>
         <v>E Pentatonic Minor</v>
       </c>
-      <c r="C23" s="132"/>
-      <c r="D23" s="132"/>
-      <c r="E23" s="132"/>
-      <c r="F23" s="132"/>
-      <c r="G23" s="132"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128"/>
+      <c r="F23" s="128"/>
+      <c r="G23" s="128"/>
       <c r="H23" s="64"/>
       <c r="I23" s="64"/>
       <c r="J23" s="105">
@@ -4830,12 +4827,12 @@
       <c r="AF23" s="64"/>
     </row>
     <row r="24" spans="2:32" s="63" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="132"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
       <c r="H24" s="64"/>
       <c r="I24" s="64"/>
       <c r="J24" s="79">
@@ -4884,12 +4881,12 @@
       <c r="AF24" s="64"/>
     </row>
     <row r="25" spans="2:32" s="63" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="132"/>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="132"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
       <c r="H25" s="64"/>
       <c r="I25" s="64"/>
       <c r="J25" s="124" t="str">
@@ -4938,12 +4935,12 @@
       <c r="AF25" s="64"/>
     </row>
     <row r="26" spans="2:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="132"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="132"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
       <c r="H26" s="65"/>
       <c r="I26" s="65"/>
       <c r="J26" s="106" t="str">
@@ -4992,16 +4989,16 @@
       <c r="AF26" s="65"/>
     </row>
     <row r="27" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="132"/>
-      <c r="C27" s="132"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132"/>
-      <c r="G27" s="132"/>
-      <c r="H27" s="133" t="s">
+      <c r="B27" s="128"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="133"/>
+      <c r="I27" s="129"/>
       <c r="J27" s="80" t="str">
         <f>Model!J28</f>
         <v>E</v>
@@ -5030,11 +5027,11 @@
         <f>IF(Model!O28=0, "", Model!P28)</f>
         <v>D</v>
       </c>
-      <c r="S27" s="134" t="s">
+      <c r="S27" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="T27" s="134"/>
-      <c r="U27" s="134"/>
+      <c r="T27" s="130"/>
+      <c r="U27" s="130"/>
       <c r="V27" s="111" t="str">
         <f>IF(Model!J26=1, "h", IF(Model!J26=2, "W", IF(Model!J26=3, "W+h", IF(Model!J26=4, "WW", IF(Model!J26=0, "", Model!J22)))))</f>
         <v/>
@@ -5063,10 +5060,10 @@
         <f>IF(Model!P26=1, "h", IF(Model!P26=2, "W", IF(Model!P26=3, "W+h", IF(Model!P26=4, "WW", IF(Model!P26=0, "", Model!P22)))))</f>
         <v>W</v>
       </c>
-      <c r="AE27" s="130" t="s">
+      <c r="AE27" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="AF27" s="130"/>
+      <c r="AF27" s="134"/>
     </row>
     <row r="28" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="104" t="s">
@@ -5187,7 +5184,7 @@
       </c>
     </row>
     <row r="29" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="129" t="s">
+      <c r="B29" s="133" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="68" t="s">
@@ -5306,7 +5303,7 @@
       </c>
     </row>
     <row r="30" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="129"/>
+      <c r="B30" s="133"/>
       <c r="C30" s="68" t="s">
         <v>16</v>
       </c>
@@ -5423,7 +5420,7 @@
       </c>
     </row>
     <row r="31" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="129"/>
+      <c r="B31" s="133"/>
       <c r="C31" s="68" t="s">
         <v>15</v>
       </c>
@@ -5540,7 +5537,7 @@
       </c>
     </row>
     <row r="32" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="129"/>
+      <c r="B32" s="133"/>
       <c r="C32" s="68" t="s">
         <v>12</v>
       </c>
@@ -5657,7 +5654,7 @@
       </c>
     </row>
     <row r="33" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="129"/>
+      <c r="B33" s="133"/>
       <c r="C33" s="68" t="s">
         <v>14</v>
       </c>
@@ -5774,7 +5771,7 @@
       </c>
     </row>
     <row r="34" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="131" t="s">
+      <c r="B34" s="127" t="s">
         <v>60</v>
       </c>
       <c r="C34" s="68" t="s">
@@ -5893,7 +5890,7 @@
       </c>
     </row>
     <row r="35" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="131"/>
+      <c r="B35" s="127"/>
       <c r="C35" s="69" t="s">
         <v>16</v>
       </c>
@@ -6006,7 +6003,7 @@
       <c r="AF35" s="103"/>
     </row>
     <row r="36" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="131"/>
+      <c r="B36" s="127"/>
       <c r="C36" s="69" t="s">
         <v>15</v>
       </c>
@@ -6119,7 +6116,7 @@
       <c r="AF36" s="103"/>
     </row>
     <row r="37" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="131"/>
+      <c r="B37" s="127"/>
       <c r="C37" s="69" t="s">
         <v>12</v>
       </c>
@@ -6452,6 +6449,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE4:AE7"/>
+    <mergeCell ref="AF4:AF7"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AE27:AF27"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B23:G27"/>
     <mergeCell ref="H27:I27"/>
@@ -6460,12 +6463,6 @@
     <mergeCell ref="S8:U8"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="B4:G8"/>
-    <mergeCell ref="AE4:AE7"/>
-    <mergeCell ref="AF4:AF7"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AE27:AF27"/>
   </mergeCells>
   <conditionalFormatting sqref="AF4 AF10:AF19">
     <cfRule type="expression" dxfId="76" priority="526">
@@ -6772,8 +6769,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BO57"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -9132,8 +9129,8 @@
       <c r="W21" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="X21" s="117" t="s">
-        <v>188</v>
+      <c r="X21" s="117">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:66" x14ac:dyDescent="0.25">
@@ -9191,7 +9188,7 @@
         <v>184</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="V22" s="6" t="s">
         <v>185</v>
@@ -9258,8 +9255,8 @@
         <v>185</v>
       </c>
       <c r="U23" s="64"/>
-      <c r="V23" s="64" t="s">
-        <v>188</v>
+      <c r="V23" s="64">
+        <v>7</v>
       </c>
       <c r="W23" s="64"/>
       <c r="X23" s="118" t="s">
@@ -9325,8 +9322,8 @@
         <v>185</v>
       </c>
       <c r="W24" s="6"/>
-      <c r="X24" s="117" t="s">
-        <v>188</v>
+      <c r="X24" s="117">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:66" x14ac:dyDescent="0.25">
@@ -9377,19 +9374,19 @@
         <v>175</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S25" s="6"/>
       <c r="T25" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U25" s="6"/>
       <c r="V25" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="W25" s="6"/>
       <c r="X25" s="117" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="2:66" x14ac:dyDescent="0.25">
@@ -9439,14 +9436,14 @@
       <c r="Q26" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="R26" s="64" t="s">
-        <v>188</v>
+      <c r="R26" s="64">
+        <v>7</v>
       </c>
       <c r="S26" s="6" t="s">
         <v>185</v>
       </c>
       <c r="T26" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U26" s="64" t="s">
         <v>186</v>
@@ -9517,8 +9514,8 @@
       <c r="T27" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="U27" s="64" t="s">
-        <v>188</v>
+      <c r="U27" s="64">
+        <v>7</v>
       </c>
       <c r="V27" s="64" t="s">
         <v>185</v>
@@ -9578,25 +9575,25 @@
         <v>58</v>
       </c>
       <c r="R28" s="64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S28" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="T28" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="T28" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="U28" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="V28" s="6" t="s">
-        <v>188</v>
+      <c r="V28" s="6">
+        <v>7</v>
       </c>
       <c r="W28" s="6" t="s">
         <v>186</v>
       </c>
       <c r="X28" s="117" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="2:66" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -9627,8 +9624,8 @@
       <c r="U29" s="64" t="s">
         <v>186</v>
       </c>
-      <c r="V29" s="64" t="s">
-        <v>188</v>
+      <c r="V29" s="64">
+        <v>7</v>
       </c>
       <c r="W29" s="64" t="s">
         <v>185</v>
@@ -9676,8 +9673,8 @@
       <c r="V30" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="W30" s="6" t="s">
-        <v>188</v>
+      <c r="W30" s="6">
+        <v>7</v>
       </c>
       <c r="X30" s="117" t="s">
         <v>185</v>
@@ -9703,8 +9700,8 @@
       <c r="R31" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="S31" s="64" t="s">
-        <v>188</v>
+      <c r="S31" s="64">
+        <v>7</v>
       </c>
       <c r="T31" s="64" t="s">
         <v>185</v>
@@ -9742,25 +9739,25 @@
         <v>57</v>
       </c>
       <c r="R32" s="64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S32" s="64" t="s">
         <v>185</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="U32" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="V32" s="64" t="s">
-        <v>188</v>
+        <v>193</v>
+      </c>
+      <c r="U32" s="64">
+        <v>7</v>
+      </c>
+      <c r="V32" s="64">
+        <v>7</v>
       </c>
       <c r="W32" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="X32" s="118" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.35">
@@ -9782,8 +9779,8 @@
       <c r="Q33" s="116" t="s">
         <v>21</v>
       </c>
-      <c r="R33" s="64" t="s">
-        <v>188</v>
+      <c r="R33" s="64">
+        <v>7</v>
       </c>
       <c r="S33" s="64" t="s">
         <v>185</v>
@@ -9827,10 +9824,10 @@
         <v>184</v>
       </c>
       <c r="S34" s="64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T34" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U34" s="6"/>
       <c r="V34" s="6">
@@ -9868,7 +9865,7 @@
         <v>184</v>
       </c>
       <c r="U35" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="V35" s="6">
         <v>5</v>
@@ -9903,8 +9900,8 @@
       <c r="S36" s="120" t="s">
         <v>186</v>
       </c>
-      <c r="T36" s="121" t="s">
-        <v>188</v>
+      <c r="T36" s="121">
+        <v>7</v>
       </c>
       <c r="U36" s="121" t="s">
         <v>185</v>

</xml_diff>

<commit_message>
Small fix to Shredsheets Text Logo, which is still awful!  Fixed a formatting error to the open position on the first fret board.
</commit_message>
<xml_diff>
--- a/Shredsheets.xlsx
+++ b/Shredsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Shredsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFF0691-8CF4-43CB-A24A-EE05FBAC4B9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3990C60E-FFA1-4E6B-AA1B-6E8E30ABC4C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26460" windowHeight="19635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1965" windowWidth="26460" windowHeight="19635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fretboards" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="197">
   <si>
     <t>Ionian</t>
   </si>
@@ -632,6 +632,9 @@
   </si>
   <si>
     <t>Degree Coloring</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1793,42 +1796,54 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1839,25 +1854,235 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="141">
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF642C76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8CFF19"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB567F5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4DA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3788CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF642C76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8CFF19"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB567F5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4DA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3788CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF642C76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8CFF19"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB567F5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4DA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3788CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3172,10 +3397,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B1:AF41"/>
+  <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3191,7 +3416,7 @@
     <col min="33" max="16384" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" s="59" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="59" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E1" s="59">
         <v>0</v>
       </c>
@@ -3269,10 +3494,10 @@
       </c>
       <c r="AE1" s="86"/>
     </row>
-    <row r="2" spans="2:32" s="59" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" s="59" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AE2" s="86"/>
     </row>
-    <row r="3" spans="2:32" s="60" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="60" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
@@ -3303,161 +3528,164 @@
       <c r="AE3" s="86"/>
       <c r="AF3" s="59"/>
     </row>
-    <row r="4" spans="2:32" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="128" t="str">
+    <row r="4" spans="1:32" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="133" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B19 = "Ionian (Major)", B10 &amp; " Major", IF(B19 = "Aolian (Minor)", B10 &amp; " Minor", B10 &amp; " " &amp; B19)), "#", "♯"), "b", "♭")</f>
-        <v>C Major</v>
-      </c>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="K4" s="123">
+        <v>C Lydian</v>
+      </c>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="K4" s="130">
         <f>IF(J8 = "", "", IF(K5 = 0, F$1, K5))</f>
         <v>1</v>
       </c>
-      <c r="L4" s="123"/>
-      <c r="M4" s="123">
+      <c r="L4" s="130"/>
+      <c r="M4" s="130">
         <f>IF(K8 = "", "", IF(M5 = 0, G$1, M5))</f>
         <v>2</v>
       </c>
-      <c r="N4" s="123"/>
-      <c r="O4" s="123">
+      <c r="N4" s="130"/>
+      <c r="O4" s="130">
         <f>IF(L8 = "", "", IF(O5 = 0, H$1, O5))</f>
         <v>3</v>
       </c>
-      <c r="P4" s="123"/>
-      <c r="Q4" s="123">
+      <c r="P4" s="130"/>
+      <c r="Q4" s="130" t="str">
         <f>IF(M8 = "", "", IF(Q5 = 0, I$1, Q5))</f>
-        <v>4</v>
-      </c>
-      <c r="R4" s="123"/>
-      <c r="S4" s="123">
+        <v>♯4</v>
+      </c>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130">
         <f>IF(N8 = "", "", IF(S5 = 0, J$1, S5))</f>
         <v>5</v>
       </c>
-      <c r="T4" s="123"/>
-      <c r="U4" s="123">
+      <c r="T4" s="130"/>
+      <c r="U4" s="130">
         <f>IF(O8 = "", "", IF(U5 = 0, K$1, U5))</f>
         <v>6</v>
       </c>
-      <c r="V4" s="123"/>
-      <c r="W4" s="123">
+      <c r="V4" s="130"/>
+      <c r="W4" s="130">
         <f>IF(P8 = "", "", IF(W5 = 0, L$1, W5))</f>
         <v>7</v>
       </c>
-      <c r="X4" s="123"/>
-      <c r="Z4" s="131" t="s">
+      <c r="X4" s="130"/>
+      <c r="Z4" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="141" t="b">
+      <c r="AA4" s="125"/>
+      <c r="AB4" s="126" t="b">
         <v>0</v>
       </c>
-      <c r="AC4" s="141"/>
+      <c r="AC4" s="126"/>
     </row>
-    <row r="5" spans="2:32" s="60" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="K5" s="125">
+    <row r="5" spans="1:32" s="60" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="133"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="K5" s="131">
         <f>IFERROR(HLOOKUP(F$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), F$1)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125">
+      <c r="L5" s="131"/>
+      <c r="M5" s="131">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), G$1)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="125"/>
-      <c r="O5" s="125">
+      <c r="N5" s="131"/>
+      <c r="O5" s="131">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), H$1)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="125"/>
-      <c r="Q5" s="125">
+      <c r="P5" s="131"/>
+      <c r="Q5" s="131" t="str">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), I$1)</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="125"/>
-      <c r="S5" s="125">
+        <v>♯4</v>
+      </c>
+      <c r="R5" s="131"/>
+      <c r="S5" s="131">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), J$1)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="125"/>
-      <c r="U5" s="125">
+      <c r="T5" s="131"/>
+      <c r="U5" s="131">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), K$1)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="125"/>
-      <c r="W5" s="125">
+      <c r="V5" s="131"/>
+      <c r="W5" s="131">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), L$1)</f>
         <v>0</v>
       </c>
-      <c r="X5" s="125"/>
-      <c r="Z5" s="131"/>
-      <c r="AA5" s="131"/>
-      <c r="AB5" s="141"/>
-      <c r="AC5" s="141"/>
+      <c r="X5" s="131"/>
+      <c r="Z5" s="125"/>
+      <c r="AA5" s="125"/>
+      <c r="AB5" s="126"/>
+      <c r="AC5" s="126"/>
     </row>
-    <row r="6" spans="2:32" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="128"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="K6" s="126" t="str">
+    <row r="6" spans="1:32" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="133"/>
+      <c r="C6" s="133"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
+      <c r="K6" s="129" t="str">
         <f>IF(K$4="","", J$8 &amp; IFERROR(HLOOKUP(F$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), F$1))</f>
         <v>CM7</v>
       </c>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126" t="str">
+      <c r="L6" s="129"/>
+      <c r="M6" s="129" t="str">
         <f>IF(M$4="","", K$8 &amp; IFERROR(HLOOKUP(G$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), G$1))</f>
-        <v>Dm7</v>
-      </c>
-      <c r="N6" s="126"/>
-      <c r="O6" s="126" t="str">
+        <v>D7</v>
+      </c>
+      <c r="N6" s="129"/>
+      <c r="O6" s="129" t="str">
         <f>IF(O$4="","", L$8 &amp; IFERROR(HLOOKUP(H$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), H$1))</f>
         <v>Em7</v>
       </c>
-      <c r="P6" s="126"/>
-      <c r="Q6" s="126" t="str">
+      <c r="P6" s="129"/>
+      <c r="Q6" s="129" t="str">
         <f>IF(Q$4="","", M$8 &amp; IFERROR(HLOOKUP(I$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), I$1))</f>
-        <v>FM7</v>
-      </c>
-      <c r="R6" s="126"/>
-      <c r="S6" s="126" t="str">
+        <v>F♯m7ø</v>
+      </c>
+      <c r="R6" s="129"/>
+      <c r="S6" s="129" t="str">
         <f>IF(S$4="","", N$8 &amp; IFERROR(HLOOKUP(J$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), J$1))</f>
-        <v>G7</v>
-      </c>
-      <c r="T6" s="126"/>
-      <c r="U6" s="126" t="str">
+        <v>GM7</v>
+      </c>
+      <c r="T6" s="129"/>
+      <c r="U6" s="129" t="str">
         <f>IF(U$4="","", O$8 &amp; IFERROR(HLOOKUP(K$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), K$1))</f>
         <v>Am7</v>
       </c>
-      <c r="V6" s="126"/>
-      <c r="W6" s="126" t="str">
+      <c r="V6" s="129"/>
+      <c r="W6" s="129" t="str">
         <f>IF(W$4="","", P$8 &amp; IFERROR(HLOOKUP(L$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), L$1))</f>
-        <v>Bm7ø</v>
-      </c>
-      <c r="X6" s="126"/>
-      <c r="Z6" s="131"/>
-      <c r="AA6" s="131"/>
-      <c r="AB6" s="141"/>
-      <c r="AC6" s="141"/>
+        <v>Bm7</v>
+      </c>
+      <c r="X6" s="129"/>
+      <c r="Z6" s="125"/>
+      <c r="AA6" s="125"/>
+      <c r="AB6" s="126"/>
+      <c r="AC6" s="126"/>
     </row>
-    <row r="7" spans="2:32" s="61" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="128"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
+    <row r="7" spans="1:32" s="61" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
       <c r="J7" s="95"/>
       <c r="K7" s="95"/>
       <c r="L7" s="95"/>
@@ -3465,22 +3693,22 @@
       <c r="N7" s="95"/>
       <c r="O7" s="95"/>
       <c r="P7" s="95"/>
-      <c r="Z7" s="131"/>
-      <c r="AA7" s="131"/>
-      <c r="AB7" s="141"/>
-      <c r="AC7" s="141"/>
+      <c r="Z7" s="125"/>
+      <c r="AA7" s="125"/>
+      <c r="AB7" s="126"/>
+      <c r="AC7" s="126"/>
     </row>
-    <row r="8" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="128"/>
-      <c r="C8" s="128"/>
-      <c r="D8" s="128"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="129" t="s">
+    <row r="8" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="134" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="129"/>
+      <c r="I8" s="134"/>
       <c r="J8" s="73" t="str">
         <f>Model!I24</f>
         <v>C</v>
@@ -3495,7 +3723,7 @@
       </c>
       <c r="M8" s="76" t="str">
         <f>IF(Model!K22=0, "", Model!L24)</f>
-        <v>F</v>
+        <v>F♯</v>
       </c>
       <c r="N8" s="77" t="str">
         <f>IF(Model!L22=0, "", Model!M24)</f>
@@ -3509,11 +3737,11 @@
         <f>IF(Model!N22=0, "", Model!O24)</f>
         <v>B</v>
       </c>
-      <c r="S8" s="130" t="s">
+      <c r="S8" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="130"/>
-      <c r="U8" s="130"/>
+      <c r="T8" s="135"/>
+      <c r="U8" s="135"/>
       <c r="V8" s="98" t="str">
         <f>IF(Model!I22=1, "h", IF(Model!I22=2, "W", IF(Model!I22=3, "W+h", IF(Model!I22=4, "WW", IF(Model!I22=0, "", Model!I22)))))</f>
         <v>W</v>
@@ -3524,11 +3752,11 @@
       </c>
       <c r="X8" s="81" t="str">
         <f>IF(Model!K22=1, "h", IF(Model!K22=2, "W", IF(Model!K22=3, "W+h", IF(Model!K22=4, "WW", IF(Model!K22=0, "", Model!K22)))))</f>
-        <v>h</v>
+        <v>W</v>
       </c>
       <c r="Y8" s="82" t="str">
         <f>IF(Model!L22=1, "h", IF(Model!L22=2, "W", IF(Model!L22=3, "W+h",IF(Model!L22=4, "WW", IF(Model!L22=0, "", Model!L22)))))</f>
-        <v>W</v>
+        <v>h</v>
       </c>
       <c r="Z8" s="83" t="str">
         <f>IF(Model!M22=1, "h", IF(Model!M22=2, "W", IF(Model!M22=3, "W+h",IF(Model!M22=4, "WW", IF(Model!M22=0, "", Model!M22)))))</f>
@@ -3542,12 +3770,12 @@
         <f>IF(Model!O22=1, "h", IF(Model!O22=2, "W", IF(Model!O22=3, "W+h",IF(Model!O22=4, "WW", IF(Model!O22=0, "", Model!O22)))))</f>
         <v>h</v>
       </c>
-      <c r="AE8" s="133" t="s">
+      <c r="AE8" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="AF8" s="133"/>
+      <c r="AF8" s="128"/>
     </row>
-    <row r="9" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="93" t="s">
         <v>13</v>
       </c>
@@ -3555,104 +3783,104 @@
         <v>17</v>
       </c>
       <c r="D9" s="37"/>
-      <c r="E9" s="138">
-        <f>IF($AB$4, 24-E$1, E$1)</f>
+      <c r="E9" s="122">
+        <f t="shared" ref="E9:AC9" si="0">IF($AB$4, 24-E$1, E$1)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="140">
-        <f>IF($AB$4, 24-F$1, F$1)</f>
+      <c r="F9" s="124">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G9" s="50">
-        <f>IF($AB$4, 24-G$1, G$1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H9" s="48">
-        <f>IF($AB$4, 24-H$1, H$1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I9" s="50">
-        <f>IF($AB$4, 24-I$1, I$1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J9" s="48">
-        <f>IF($AB$4, 24-J$1, J$1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K9" s="50">
-        <f>IF($AB$4, 24-K$1, K$1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L9" s="48">
-        <f>IF($AB$4, 24-L$1, L$1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M9" s="50">
-        <f>IF($AB$4, 24-M$1, M$1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="N9" s="48">
-        <f>IF($AB$4, 24-N$1, N$1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="O9" s="50">
-        <f>IF($AB$4, 24-O$1, O$1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="P9" s="50">
-        <f>IF($AB$4, 24-P$1, P$1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="Q9" s="49">
-        <f>IF($AB$4, 24-Q$1, Q$1)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="R9" s="50">
-        <f>IF($AB$4, 24-R$1, R$1)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="S9" s="50">
-        <f>IF($AB$4, 24-S$1, S$1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="T9" s="48">
-        <f>IF($AB$4, 24-T$1, T$1)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="U9" s="50">
-        <f>IF($AB$4, 24-U$1, U$1)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="V9" s="48">
-        <f>IF($AB$4, 24-V$1, V$1)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="W9" s="50">
-        <f>IF($AB$4, 24-W$1, W$1)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="X9" s="48">
-        <f>IF($AB$4, 24-X$1, X$1)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="Y9" s="50">
-        <f>IF($AB$4, 24-Y$1, Y$1)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="Z9" s="48">
-        <f>IF($AB$4, 24-Z$1, Z$1)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="AA9" s="50">
-        <f>IF($AB$4, 24-AA$1, AA$1)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="AB9" s="50">
-        <f>IF($AB$4, 24-AB$1, AB$1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="AC9" s="55">
-        <f>IF($AB$4, 24-AC$1, AC$1)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="AE9" s="96" t="s">
@@ -3662,8 +3890,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="132" t="s">
+    <row r="10" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="127" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="64" t="s">
@@ -3673,17 +3901,17 @@
         <f>VLOOKUP(UPPER(Fretboards!C10), Model!$B$2:$D$41, 3)</f>
         <v>4</v>
       </c>
-      <c r="E10" s="118" t="str">
-        <f>IFERROR(HLOOKUP(MATCH($D10+E$9, Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
+      <c r="E10" s="58" t="str">
+        <f>IFERROR(HLOOKUP(MATCH(MOD($D10+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>E : 3</v>
       </c>
       <c r="F10" s="119" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="G10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="H10" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3727,11 +3955,11 @@
       </c>
       <c r="R10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="S10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="T10" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3781,8 +4009,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="132"/>
+    <row r="11" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="127"/>
       <c r="C11" s="64" t="s">
         <v>16</v>
       </c>
@@ -3790,7 +4018,7 @@
         <f>VLOOKUP(UPPER(Fretboards!C11), Model!$B$2:$D$41, 3)</f>
         <v>11</v>
       </c>
-      <c r="E11" s="118" t="str">
+      <c r="E11" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>B : 7</v>
       </c>
@@ -3816,11 +4044,11 @@
       </c>
       <c r="K11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="L11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="M11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3864,11 +4092,11 @@
       </c>
       <c r="W11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="X11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="Y11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3898,8 +4126,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="132"/>
+    <row r="12" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="127"/>
       <c r="C12" s="64" t="s">
         <v>15</v>
       </c>
@@ -3907,7 +4135,7 @@
         <f>VLOOKUP(UPPER(Fretboards!C12), Model!$B$2:$D$41, 3)</f>
         <v>7</v>
       </c>
-      <c r="E12" s="118" t="str">
+      <c r="E12" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>G : 5</v>
       </c>
@@ -3949,11 +4177,11 @@
       </c>
       <c r="O12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="P12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="Q12" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3997,11 +4225,11 @@
       </c>
       <c r="AA12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="AB12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="AC12" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4015,8 +4243,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="132"/>
+    <row r="13" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="127"/>
       <c r="C13" s="64" t="s">
         <v>12</v>
       </c>
@@ -4024,7 +4252,7 @@
         <f>VLOOKUP(UPPER(Fretboards!C13), Model!$B$2:$D$41, 3)</f>
         <v>2</v>
       </c>
-      <c r="E13" s="118" t="str">
+      <c r="E13" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>D : 2</v>
       </c>
@@ -4038,11 +4266,11 @@
       </c>
       <c r="H13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="I13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="J13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4086,11 +4314,11 @@
       </c>
       <c r="T13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="U13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="V13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4129,11 +4357,11 @@
       </c>
       <c r="AF13" s="120" t="b">
         <f>HLOOKUP(I$1, Model!$I$40:$O$56, MATCH($B$19, Model!$H$40:$H$56, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="132"/>
+    <row r="14" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="127"/>
       <c r="C14" s="64" t="s">
         <v>14</v>
       </c>
@@ -4141,7 +4369,7 @@
         <f>VLOOKUP(UPPER(Fretboards!C14), Model!$B$2:$D$41, 3)</f>
         <v>9</v>
       </c>
-      <c r="E14" s="118" t="str">
+      <c r="E14" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>A : 6</v>
       </c>
@@ -4175,11 +4403,11 @@
       </c>
       <c r="M14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="N14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="O14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4223,11 +4451,11 @@
       </c>
       <c r="Y14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="Z14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="AA14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4246,11 +4474,11 @@
       </c>
       <c r="AF14" s="120" t="b">
         <f>HLOOKUP(J$1, Model!$I$40:$O$56, MATCH($B$19, Model!$H$40:$H$56, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="127" t="s">
+    <row r="15" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="132" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="64" t="s">
@@ -4260,17 +4488,17 @@
         <f>VLOOKUP(UPPER(Fretboards!C15), Model!$B$2:$D$41, 3)</f>
         <v>4</v>
       </c>
-      <c r="E15" s="118" t="str">
+      <c r="E15" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>E : 3</v>
       </c>
       <c r="F15" s="119" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="G15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="H15" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4314,11 +4542,11 @@
       </c>
       <c r="R15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="S15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F♯ : ♯4</v>
       </c>
       <c r="T15" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4365,11 +4593,11 @@
       </c>
       <c r="AF15" s="120" t="b">
         <f>HLOOKUP(K$1, Model!$I$40:$O$56, MATCH($B$19, Model!$H$40:$H$56, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="127"/>
+    <row r="16" spans="1:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="132"/>
       <c r="C16" s="64" t="s">
         <v>16</v>
       </c>
@@ -4377,7 +4605,7 @@
         <f>VLOOKUP(UPPER(Fretboards!C16), Model!$B$2:$D$41, 3)</f>
         <v>11</v>
       </c>
-      <c r="E16" s="118" t="str">
+      <c r="E16" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D16+E$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v>B : 7</v>
       </c>
@@ -4403,11 +4631,11 @@
       </c>
       <c r="K16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D16+K$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="L16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D16+L$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F♯ : 4</v>
       </c>
       <c r="M16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D16+M$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4451,11 +4679,11 @@
       </c>
       <c r="W16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D16+W$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="X16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D16+X$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F♯ : 4</v>
       </c>
       <c r="Y16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D16+Y$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4481,7 +4709,7 @@
       <c r="AF16" s="121"/>
     </row>
     <row r="17" spans="2:32" s="63" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="127"/>
+      <c r="B17" s="132"/>
       <c r="C17" s="64" t="s">
         <v>15</v>
       </c>
@@ -4489,7 +4717,7 @@
         <f>VLOOKUP(UPPER(Fretboards!C17), Model!$B$2:$D$41, 3)</f>
         <v>7</v>
       </c>
-      <c r="E17" s="118" t="str">
+      <c r="E17" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D17+E$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v>G : 5</v>
       </c>
@@ -4531,11 +4759,11 @@
       </c>
       <c r="O17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D17+O$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="P17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D17+P$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F♯ : 4</v>
       </c>
       <c r="Q17" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D17+Q$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4579,11 +4807,11 @@
       </c>
       <c r="AA17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D17+AA$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="AB17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D17+AB$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F♯ : 4</v>
       </c>
       <c r="AC17" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D17+AC$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4593,7 +4821,7 @@
       <c r="AF17" s="121"/>
     </row>
     <row r="18" spans="2:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="127"/>
+      <c r="B18" s="132"/>
       <c r="C18" s="64" t="s">
         <v>12</v>
       </c>
@@ -4601,7 +4829,7 @@
         <f>VLOOKUP(UPPER(Fretboards!C18), Model!$B$2:$D$41, 3)</f>
         <v>2</v>
       </c>
-      <c r="E18" s="118" t="str">
+      <c r="E18" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D18+E$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v>D : 2</v>
       </c>
@@ -4615,11 +4843,11 @@
       </c>
       <c r="H18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D18+H$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="I18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D18+I$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F♯ : 4</v>
       </c>
       <c r="J18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D18+J$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4663,11 +4891,11 @@
       </c>
       <c r="T18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D18+T$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="U18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D18+U$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F♯ : 4</v>
       </c>
       <c r="V18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$28, 5) &amp; " : " &amp; MATCH(MOD($D18+V$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4706,108 +4934,108 @@
     </row>
     <row r="19" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="67" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="C19" s="65"/>
       <c r="D19" s="1"/>
       <c r="E19" s="51">
-        <f>IF($AB$4, 24-E$1, E$1)</f>
+        <f t="shared" ref="E19:AC19" si="1">IF($AB$4, 24-E$1, E$1)</f>
         <v>0</v>
       </c>
       <c r="F19" s="50">
-        <f>IF($AB$4, 24-F$1, F$1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G19" s="50">
-        <f>IF($AB$4, 24-G$1, G$1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H19" s="48">
-        <f>IF($AB$4, 24-H$1, H$1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I19" s="50">
-        <f>IF($AB$4, 24-I$1, I$1)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J19" s="48">
-        <f>IF($AB$4, 24-J$1, J$1)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K19" s="50">
-        <f>IF($AB$4, 24-K$1, K$1)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L19" s="48">
-        <f>IF($AB$4, 24-L$1, L$1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="M19" s="50">
-        <f>IF($AB$4, 24-M$1, M$1)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="N19" s="48">
-        <f>IF($AB$4, 24-N$1, N$1)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="O19" s="50">
-        <f>IF($AB$4, 24-O$1, O$1)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="P19" s="50">
-        <f>IF($AB$4, 24-P$1, P$1)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="Q19" s="49">
-        <f>IF($AB$4, 24-Q$1, Q$1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="R19" s="50">
-        <f>IF($AB$4, 24-R$1, R$1)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="S19" s="50">
-        <f>IF($AB$4, 24-S$1, S$1)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="T19" s="48">
-        <f>IF($AB$4, 24-T$1, T$1)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="U19" s="50">
-        <f>IF($AB$4, 24-U$1, U$1)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="V19" s="48">
-        <f>IF($AB$4, 24-V$1, V$1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="W19" s="50">
-        <f>IF($AB$4, 24-W$1, W$1)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="X19" s="48">
-        <f>IF($AB$4, 24-X$1, X$1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="Y19" s="50">
-        <f>IF($AB$4, 24-Y$1, Y$1)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="Z19" s="48">
-        <f>IF($AB$4, 24-Z$1, Z$1)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="AA19" s="50">
-        <f>IF($AB$4, 24-AA$1, AA$1)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="AB19" s="50">
-        <f>IF($AB$4, 24-AB$1, AB$1)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="AC19" s="55">
-        <f>IF($AB$4, 24-AC$1, AC$1)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="AE19" s="88" t="s">
@@ -4815,7 +5043,7 @@
       </c>
       <c r="AF19" s="120" t="b">
         <f>HLOOKUP(L$1, Model!$I$40:$O$56, MATCH($B$19, Model!$H$40:$H$56, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.3">
@@ -4904,50 +5132,50 @@
       <c r="AF22" s="60"/>
     </row>
     <row r="23" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="128" t="str">
+      <c r="B23" s="133" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B38 = "Ionian (Major)", B29 &amp; " Major", IF(B38 = "Aolian (Minor)", B29 &amp; " Minor", B29 &amp; " " &amp; B38)), "#", "♯"), "b", "♭")</f>
         <v>E Pentatonic Minor</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="K23" s="123">
+      <c r="C23" s="133"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="133"/>
+      <c r="K23" s="130">
         <f>IF(J27 = "", "", IF(K24 = 0, F$1, K24))</f>
         <v>1</v>
       </c>
-      <c r="L23" s="123"/>
-      <c r="M23" s="123" t="str">
+      <c r="L23" s="130"/>
+      <c r="M23" s="130" t="str">
         <f>IF(K27 = "", "", IF(M24 = 0, G$1, M24))</f>
         <v/>
       </c>
-      <c r="N23" s="123"/>
-      <c r="O23" s="123" t="str">
+      <c r="N23" s="130"/>
+      <c r="O23" s="130" t="str">
         <f>IF(L27 = "", "", IF(O24 = 0, H$1, O24))</f>
         <v>♭3</v>
       </c>
-      <c r="P23" s="123"/>
-      <c r="Q23" s="123">
+      <c r="P23" s="130"/>
+      <c r="Q23" s="130">
         <f>IF(M27 = "", "", IF(Q24 = 0, I$1, Q24))</f>
         <v>4</v>
       </c>
-      <c r="R23" s="123"/>
-      <c r="S23" s="123">
+      <c r="R23" s="130"/>
+      <c r="S23" s="130">
         <f>IF(N27 = "", "", IF(S24 = 0, J$1, S24))</f>
         <v>5</v>
       </c>
-      <c r="T23" s="123"/>
-      <c r="U23" s="123" t="str">
+      <c r="T23" s="130"/>
+      <c r="U23" s="130" t="str">
         <f>IF(O27 = "", "", IF(U24 = 0, K$1, U24))</f>
         <v/>
       </c>
-      <c r="V23" s="123"/>
-      <c r="W23" s="123" t="str">
+      <c r="V23" s="130"/>
+      <c r="W23" s="130" t="str">
         <f>IF(P27 = "", "", IF(W24 = 0, L$1, W24))</f>
         <v>♭7</v>
       </c>
-      <c r="X23" s="123"/>
+      <c r="X23" s="130"/>
       <c r="Y23" s="60"/>
       <c r="Z23" s="60"/>
       <c r="AA23" s="60"/>
@@ -4958,47 +5186,47 @@
       <c r="AF23" s="60"/>
     </row>
     <row r="24" spans="2:32" s="59" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="128"/>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="128"/>
-      <c r="G24" s="128"/>
-      <c r="K24" s="124">
+      <c r="B24" s="133"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
+      <c r="G24" s="133"/>
+      <c r="K24" s="136">
         <f>IFERROR(HLOOKUP(F$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), F$1)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="124"/>
-      <c r="M24" s="124">
+      <c r="L24" s="136"/>
+      <c r="M24" s="136">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), G$1)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="124"/>
-      <c r="O24" s="124" t="str">
+      <c r="N24" s="136"/>
+      <c r="O24" s="136" t="str">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), H$1)</f>
         <v>♭3</v>
       </c>
-      <c r="P24" s="124"/>
-      <c r="Q24" s="124">
+      <c r="P24" s="136"/>
+      <c r="Q24" s="136">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), I$1)</f>
         <v>0</v>
       </c>
-      <c r="R24" s="124"/>
-      <c r="S24" s="124">
+      <c r="R24" s="136"/>
+      <c r="S24" s="136">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), J$1)</f>
         <v>0</v>
       </c>
-      <c r="T24" s="124"/>
-      <c r="U24" s="124">
+      <c r="T24" s="136"/>
+      <c r="U24" s="136">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), K$1)</f>
         <v>0</v>
       </c>
-      <c r="V24" s="124"/>
-      <c r="W24" s="124" t="str">
+      <c r="V24" s="136"/>
+      <c r="W24" s="136" t="str">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), L$1)</f>
         <v>♭7</v>
       </c>
-      <c r="X24" s="124"/>
+      <c r="X24" s="136"/>
       <c r="Y24" s="60"/>
       <c r="Z24" s="60"/>
       <c r="AA24" s="60"/>
@@ -5009,47 +5237,47 @@
       <c r="AF24" s="60"/>
     </row>
     <row r="25" spans="2:32" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="128"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="128"/>
-      <c r="E25" s="128"/>
-      <c r="F25" s="128"/>
-      <c r="G25" s="128"/>
-      <c r="K25" s="122" t="str">
+      <c r="B25" s="133"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="133"/>
+      <c r="K25" s="137" t="str">
         <f>IF(K$23="","", J$27 &amp; IFERROR(HLOOKUP(F$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), F$1))</f>
         <v>Em7</v>
       </c>
-      <c r="L25" s="122"/>
-      <c r="M25" s="122" t="str">
+      <c r="L25" s="137"/>
+      <c r="M25" s="137" t="str">
         <f>IF(M$23="","", K$27 &amp; IFERROR(HLOOKUP(G$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), G$1))</f>
         <v/>
       </c>
-      <c r="N25" s="122"/>
-      <c r="O25" s="122" t="str">
+      <c r="N25" s="137"/>
+      <c r="O25" s="137" t="str">
         <f>IF(O$23="","", L$27 &amp; IFERROR(HLOOKUP(H$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), H$1))</f>
         <v>GM</v>
       </c>
-      <c r="P25" s="122"/>
-      <c r="Q25" s="122" t="str">
+      <c r="P25" s="137"/>
+      <c r="Q25" s="137" t="str">
         <f>IF(Q$23="","", M$27 &amp; IFERROR(HLOOKUP(I$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), I$1))</f>
         <v>A5 ♭7</v>
       </c>
-      <c r="R25" s="122"/>
-      <c r="S25" s="122" t="str">
+      <c r="R25" s="137"/>
+      <c r="S25" s="137" t="str">
         <f>IF(S$23="","", N$27 &amp; IFERROR(HLOOKUP(J$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), J$1))</f>
         <v>B5</v>
       </c>
-      <c r="T25" s="122"/>
-      <c r="U25" s="122" t="str">
+      <c r="T25" s="137"/>
+      <c r="U25" s="137" t="str">
         <f>IF(U$23="","", O$27 &amp; IFERROR(HLOOKUP(K$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), K$1))</f>
         <v/>
       </c>
-      <c r="V25" s="122"/>
-      <c r="W25" s="122" t="str">
+      <c r="V25" s="137"/>
+      <c r="W25" s="137" t="str">
         <f>IF(W$23="","", P$27 &amp; IFERROR(HLOOKUP(L$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), L$1))</f>
         <v>D5</v>
       </c>
-      <c r="X25" s="122"/>
+      <c r="X25" s="137"/>
       <c r="Y25" s="60"/>
       <c r="Z25" s="60"/>
       <c r="AA25" s="60"/>
@@ -5060,12 +5288,12 @@
       <c r="AF25" s="60"/>
     </row>
     <row r="26" spans="2:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="128"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="128"/>
+      <c r="B26" s="133"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="133"/>
+      <c r="G26" s="133"/>
       <c r="H26" s="61"/>
       <c r="I26" s="61"/>
       <c r="J26" s="94"/>
@@ -5093,16 +5321,16 @@
       <c r="AF26" s="61"/>
     </row>
     <row r="27" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="128"/>
-      <c r="C27" s="128"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="128"/>
-      <c r="H27" s="129" t="s">
+      <c r="B27" s="133"/>
+      <c r="C27" s="133"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="133"/>
+      <c r="G27" s="133"/>
+      <c r="H27" s="134" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="129"/>
+      <c r="I27" s="134"/>
       <c r="J27" s="73" t="str">
         <f>Model!I28</f>
         <v>E</v>
@@ -5131,11 +5359,11 @@
         <f>IF(Model!N28=0, "", Model!O28)</f>
         <v>D</v>
       </c>
-      <c r="S27" s="130" t="s">
+      <c r="S27" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="T27" s="130"/>
-      <c r="U27" s="130"/>
+      <c r="T27" s="135"/>
+      <c r="U27" s="135"/>
       <c r="V27" s="98" t="str">
         <f>IF(Model!I26=1, "h", IF(Model!I26=2, "W", IF(Model!I26=3, "W+h", IF(Model!I26=4, "WW", IF(Model!I26=0, "", Model!I22)))))</f>
         <v/>
@@ -5164,10 +5392,10 @@
         <f>IF(Model!O26=1, "h", IF(Model!O26=2, "W", IF(Model!O26=3, "W+h", IF(Model!O26=4, "WW", IF(Model!O26=0, "", Model!O22)))))</f>
         <v>W</v>
       </c>
-      <c r="AE27" s="133" t="s">
+      <c r="AE27" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="AF27" s="133"/>
+      <c r="AF27" s="128"/>
     </row>
     <row r="28" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="93" t="s">
@@ -5180,104 +5408,104 @@
         <f>VLOOKUP(UPPER(Fretboards!C28), Model!$B$2:$D$41, 3)</f>
         <v>5</v>
       </c>
-      <c r="E28" s="138">
-        <f>IF($AB$4, 24-E$1, E$1)</f>
+      <c r="E28" s="122">
+        <f t="shared" ref="E28:AC28" si="2">IF($AB$4, 24-E$1, E$1)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="139">
-        <f>IF($AB$4, 24-F$1, F$1)</f>
+      <c r="F28" s="123">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G28" s="47">
-        <f>IF($AB$4, 24-G$1, G$1)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H28" s="48">
-        <f>IF($AB$4, 24-H$1, H$1)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I28" s="47">
-        <f>IF($AB$4, 24-I$1, I$1)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J28" s="48">
-        <f>IF($AB$4, 24-J$1, J$1)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K28" s="47">
-        <f>IF($AB$4, 24-K$1, K$1)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L28" s="48">
-        <f>IF($AB$4, 24-L$1, L$1)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="M28" s="47">
-        <f>IF($AB$4, 24-M$1, M$1)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="N28" s="48">
-        <f>IF($AB$4, 24-N$1, N$1)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="O28" s="47">
-        <f>IF($AB$4, 24-O$1, O$1)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="P28" s="47">
-        <f>IF($AB$4, 24-P$1, P$1)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="Q28" s="53">
-        <f>IF($AB$4, 24-Q$1, Q$1)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="R28" s="47">
-        <f>IF($AB$4, 24-R$1, R$1)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="S28" s="47">
-        <f>IF($AB$4, 24-S$1, S$1)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="T28" s="48">
-        <f>IF($AB$4, 24-T$1, T$1)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="U28" s="47">
-        <f>IF($AB$4, 24-U$1, U$1)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="V28" s="48">
-        <f>IF($AB$4, 24-V$1, V$1)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="W28" s="47">
-        <f>IF($AB$4, 24-W$1, W$1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="X28" s="48">
-        <f>IF($AB$4, 24-X$1, X$1)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="Y28" s="47">
-        <f>IF($AB$4, 24-Y$1, Y$1)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="Z28" s="48">
-        <f>IF($AB$4, 24-Z$1, Z$1)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="AA28" s="47">
-        <f>IF($AB$4, 24-AA$1, AA$1)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="AB28" s="47">
-        <f>IF($AB$4, 24-AB$1, AB$1)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="AC28" s="54">
-        <f>IF($AB$4, 24-AC$1, AC$1)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="AE28" s="96" t="s">
@@ -5288,7 +5516,7 @@
       </c>
     </row>
     <row r="29" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="132" t="s">
+      <c r="B29" s="127" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="64" t="s">
@@ -5408,7 +5636,7 @@
       </c>
     </row>
     <row r="30" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="132"/>
+      <c r="B30" s="127"/>
       <c r="C30" s="64" t="s">
         <v>16</v>
       </c>
@@ -5526,7 +5754,7 @@
       </c>
     </row>
     <row r="31" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="132"/>
+      <c r="B31" s="127"/>
       <c r="C31" s="64" t="s">
         <v>15</v>
       </c>
@@ -5644,7 +5872,7 @@
       </c>
     </row>
     <row r="32" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="132"/>
+      <c r="B32" s="127"/>
       <c r="C32" s="64" t="s">
         <v>12</v>
       </c>
@@ -5762,7 +5990,7 @@
       </c>
     </row>
     <row r="33" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="132"/>
+      <c r="B33" s="127"/>
       <c r="C33" s="64" t="s">
         <v>14</v>
       </c>
@@ -5880,7 +6108,7 @@
       </c>
     </row>
     <row r="34" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="127" t="s">
+      <c r="B34" s="132" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="64" t="s">
@@ -6000,7 +6228,7 @@
       </c>
     </row>
     <row r="35" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="127"/>
+      <c r="B35" s="132"/>
       <c r="C35" s="64" t="s">
         <v>16</v>
       </c>
@@ -6050,7 +6278,7 @@
       </c>
       <c r="O35" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D35+O$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D35+O$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 4</v>
+        <v>A : ♯4</v>
       </c>
       <c r="P35" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D35+P$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D35+P$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -6098,7 +6326,7 @@
       </c>
       <c r="AA35" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D35+AA$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D35+AA$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 4</v>
+        <v>A : ♯4</v>
       </c>
       <c r="AB35" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D35+AB$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D35+AB$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -6113,7 +6341,7 @@
       <c r="AF35" s="121"/>
     </row>
     <row r="36" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="127"/>
+      <c r="B36" s="132"/>
       <c r="C36" s="64" t="s">
         <v>15</v>
       </c>
@@ -6131,7 +6359,7 @@
       </c>
       <c r="G36" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D36+G$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D36+G$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 4</v>
+        <v>A : ♯4</v>
       </c>
       <c r="H36" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D36+H$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D36+H$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -6179,7 +6407,7 @@
       </c>
       <c r="S36" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D36+S$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D36+S$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 4</v>
+        <v>A : ♯4</v>
       </c>
       <c r="T36" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D36+T$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D36+T$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -6226,7 +6454,7 @@
       <c r="AF36" s="121"/>
     </row>
     <row r="37" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="127"/>
+      <c r="B37" s="132"/>
       <c r="C37" s="64" t="s">
         <v>12</v>
       </c>
@@ -6264,7 +6492,7 @@
       </c>
       <c r="L37" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D37+L$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D37+L$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 4</v>
+        <v>A : ♯4</v>
       </c>
       <c r="M37" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D37+M$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D37+M$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -6312,7 +6540,7 @@
       </c>
       <c r="X37" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D37+X$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D37+X$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 4</v>
+        <v>A : ♯4</v>
       </c>
       <c r="Y37" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D37+Y$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$28, 9) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D37+Y$28, 12), Model!$I$27:$O$27, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -6345,103 +6573,103 @@
       <c r="C38" s="65"/>
       <c r="D38" s="1"/>
       <c r="E38" s="52">
-        <f>IF($AB$4, 24-E$1, E$1)</f>
+        <f t="shared" ref="E38:AC38" si="3">IF($AB$4, 24-E$1, E$1)</f>
         <v>0</v>
       </c>
       <c r="F38" s="47">
-        <f>IF($AB$4, 24-F$1, F$1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G38" s="47">
-        <f>IF($AB$4, 24-G$1, G$1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H38" s="48">
-        <f>IF($AB$4, 24-H$1, H$1)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I38" s="47">
-        <f>IF($AB$4, 24-I$1, I$1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J38" s="48">
-        <f>IF($AB$4, 24-J$1, J$1)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="K38" s="47">
-        <f>IF($AB$4, 24-K$1, K$1)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L38" s="48">
-        <f>IF($AB$4, 24-L$1, L$1)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="M38" s="47">
-        <f>IF($AB$4, 24-M$1, M$1)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N38" s="48">
-        <f>IF($AB$4, 24-N$1, N$1)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O38" s="47">
-        <f>IF($AB$4, 24-O$1, O$1)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="P38" s="47">
-        <f>IF($AB$4, 24-P$1, P$1)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="Q38" s="53">
-        <f>IF($AB$4, 24-Q$1, Q$1)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="R38" s="47">
-        <f>IF($AB$4, 24-R$1, R$1)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="S38" s="47">
-        <f>IF($AB$4, 24-S$1, S$1)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="T38" s="48">
-        <f>IF($AB$4, 24-T$1, T$1)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="U38" s="47">
-        <f>IF($AB$4, 24-U$1, U$1)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="V38" s="48">
-        <f>IF($AB$4, 24-V$1, V$1)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="W38" s="47">
-        <f>IF($AB$4, 24-W$1, W$1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="X38" s="48">
-        <f>IF($AB$4, 24-X$1, X$1)</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="Y38" s="47">
-        <f>IF($AB$4, 24-Y$1, Y$1)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="Z38" s="48">
-        <f>IF($AB$4, 24-Z$1, Z$1)</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="AA38" s="47">
-        <f>IF($AB$4, 24-AA$1, AA$1)</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="AB38" s="47">
-        <f>IF($AB$4, 24-AB$1, AB$1)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="AC38" s="54">
-        <f>IF($AB$4, 24-AC$1, AC$1)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="AE38" s="88" t="s">
@@ -6485,6 +6713,46 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B23:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B4:G8"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
     <mergeCell ref="Z4:AA7"/>
     <mergeCell ref="AB4:AC7"/>
     <mergeCell ref="B10:B14"/>
@@ -6501,468 +6769,451 @@
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="U5:V5"/>
     <mergeCell ref="U6:V6"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B23:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B4:G8"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U25:V25"/>
   </mergeCells>
   <conditionalFormatting sqref="AB4 AF10:AF19">
-    <cfRule type="expression" dxfId="119" priority="541">
+    <cfRule type="expression" dxfId="140" priority="548">
       <formula>AND($AF$15=TRUE, SEARCH("6", AB4))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="542">
+    <cfRule type="expression" dxfId="139" priority="549">
       <formula>AND($AF$10=TRUE, SEARCH("1", AB4))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="543">
+    <cfRule type="expression" dxfId="138" priority="550">
       <formula>AND($AF$11=TRUE, SEARCH("2", AB4))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="544">
+    <cfRule type="expression" dxfId="137" priority="551">
       <formula>AND($AF$12=TRUE, SEARCH("3", AB4))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="545">
+    <cfRule type="expression" dxfId="136" priority="552">
       <formula>AND($AF$13=TRUE, SEARCH("4", AB4))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="546">
+    <cfRule type="expression" dxfId="135" priority="553">
       <formula>AND($AF$14=TRUE, SEARCH("5", AB4))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="547">
+    <cfRule type="expression" dxfId="134" priority="554">
       <formula>AND($AF$19=TRUE, SEARCH("7", AB4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:AA8">
-    <cfRule type="containsText" dxfId="112" priority="164" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="133" priority="171" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",W8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF3">
-    <cfRule type="expression" dxfId="111" priority="100">
+    <cfRule type="expression" dxfId="132" priority="107">
       <formula>AND($AF$15=TRUE, SEARCH("6", AF3))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="101">
+    <cfRule type="expression" dxfId="131" priority="108">
       <formula>AND($AF$10=TRUE, SEARCH("1", AF3))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="102">
+    <cfRule type="expression" dxfId="130" priority="109">
       <formula>AND($AF$11=TRUE, SEARCH("2", AF3))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="103">
+    <cfRule type="expression" dxfId="129" priority="110">
       <formula>AND($AF$12=TRUE, SEARCH("3", AF3))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="104">
+    <cfRule type="expression" dxfId="128" priority="111">
       <formula>AND($AF$13=TRUE, SEARCH("4", AF3))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="105">
+    <cfRule type="expression" dxfId="127" priority="112">
       <formula>AND($AF$14=TRUE, SEARCH("5", AF3))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="106">
+    <cfRule type="expression" dxfId="126" priority="113">
       <formula>AND($AF$19=TRUE, SEARCH("7", AF3))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:AC18">
-    <cfRule type="expression" dxfId="104" priority="86">
+    <cfRule type="expression" dxfId="125" priority="93">
       <formula>AND($AF$10, SEARCH("1", G10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="87">
+    <cfRule type="expression" dxfId="124" priority="94">
       <formula>AND($AF$11, SEARCH("2", G10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="88">
+    <cfRule type="expression" dxfId="123" priority="95">
       <formula>AND($AF$12, SEARCH("3", G10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="89">
+    <cfRule type="expression" dxfId="122" priority="96">
       <formula>AND($AF$13, SEARCH("4", G10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="90">
+    <cfRule type="expression" dxfId="121" priority="97">
       <formula>AND($AF$14, SEARCH("5", G10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="91">
+    <cfRule type="expression" dxfId="120" priority="98">
       <formula>AND($AF$15, SEARCH("6", G10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="92">
+    <cfRule type="expression" dxfId="119" priority="99">
       <formula>AND($AF$19, SEARCH("7", G10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE29:AE34 AE38">
-    <cfRule type="expression" dxfId="97" priority="72">
+    <cfRule type="expression" dxfId="118" priority="79">
       <formula>AND($AF$29, SEARCH("1", AE29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="73">
+    <cfRule type="expression" dxfId="117" priority="80">
       <formula>AND($AF$30, SEARCH("2", AE29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="74">
+    <cfRule type="expression" dxfId="116" priority="81">
       <formula>AND($AF$31, SEARCH("3", AE29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="75">
+    <cfRule type="expression" dxfId="115" priority="82">
       <formula>AND($AF$32, SEARCH("4", AE29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="76">
+    <cfRule type="expression" dxfId="114" priority="83">
       <formula>AND($AF$33, SEARCH("5", AE29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="77">
+    <cfRule type="expression" dxfId="113" priority="84">
       <formula>AND($AF$34, SEARCH("6", AE29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="78">
+    <cfRule type="expression" dxfId="112" priority="85">
       <formula>AND($AF$38, SEARCH("7", AE29))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:AC37">
-    <cfRule type="expression" dxfId="90" priority="93">
+    <cfRule type="expression" dxfId="111" priority="100">
       <formula>AND($AF$29, SEARCH("1", E29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="94">
+    <cfRule type="expression" dxfId="110" priority="101">
       <formula>AND($AF$30, SEARCH("2", E29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="95">
+    <cfRule type="expression" dxfId="109" priority="102">
       <formula>AND($AF$31, SEARCH("3", E29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="96">
+    <cfRule type="expression" dxfId="108" priority="103">
       <formula>AND($AF$32, SEARCH("4", E29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="97">
+    <cfRule type="expression" dxfId="107" priority="104">
       <formula>AND($AF$33, SEARCH("5", E29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="98">
+    <cfRule type="expression" dxfId="106" priority="105">
       <formula>AND($AF$34, SEARCH("6", E29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="99">
+    <cfRule type="expression" dxfId="105" priority="106">
       <formula>AND($AF$38, SEARCH("7", E29))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE10:AE15 AE19">
-    <cfRule type="expression" dxfId="83" priority="51">
+    <cfRule type="expression" dxfId="104" priority="58">
       <formula>AND($AF$10, SEARCH("1", AE10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="52">
+    <cfRule type="expression" dxfId="103" priority="59">
       <formula>AND($AF$11, SEARCH("2", AE10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="53">
+    <cfRule type="expression" dxfId="102" priority="60">
       <formula>AND($AF$12, SEARCH("3", AE10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="54">
+    <cfRule type="expression" dxfId="101" priority="61">
       <formula>AND($AF$13, SEARCH("4", AE10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="55">
+    <cfRule type="expression" dxfId="100" priority="62">
       <formula>AND($AF$14, SEARCH("5", AE10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="56">
+    <cfRule type="expression" dxfId="99" priority="63">
       <formula>AND($AF$15, SEARCH("6", AE10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="57">
+    <cfRule type="expression" dxfId="98" priority="64">
       <formula>AND($AF$19, SEARCH("7", AE10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8">
-    <cfRule type="containsText" dxfId="76" priority="47" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="97" priority="54" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",V8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB8">
-    <cfRule type="containsText" dxfId="75" priority="46" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="96" priority="53" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AB8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V27">
-    <cfRule type="containsText" dxfId="74" priority="38" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="95" priority="45" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",V27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W27">
-    <cfRule type="containsText" dxfId="73" priority="37" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="94" priority="44" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",W27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X27">
-    <cfRule type="containsText" dxfId="72" priority="36" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="93" priority="43" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",X27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y27">
-    <cfRule type="containsText" dxfId="71" priority="35" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="92" priority="42" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Y27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z27">
-    <cfRule type="containsText" dxfId="70" priority="34" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="91" priority="41" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Z27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA27">
-    <cfRule type="containsText" dxfId="69" priority="33" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="90" priority="40" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AA27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB27">
-    <cfRule type="containsText" dxfId="68" priority="32" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="89" priority="39" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AB27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:P18">
-    <cfRule type="containsBlanks" dxfId="67" priority="551">
+    <cfRule type="containsBlanks" dxfId="88" priority="558">
       <formula>LEN(TRIM(G10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:P37">
-    <cfRule type="containsBlanks" dxfId="66" priority="552">
+    <cfRule type="containsBlanks" dxfId="87" priority="559">
       <formula>LEN(TRIM(F29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:AB18">
-    <cfRule type="containsBlanks" dxfId="65" priority="553">
+    <cfRule type="containsBlanks" dxfId="86" priority="560">
       <formula>LEN(TRIM(R10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R29:AB37">
-    <cfRule type="containsBlanks" dxfId="64" priority="16">
+    <cfRule type="containsBlanks" dxfId="85" priority="23">
       <formula>LEN(TRIM(R29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8 M27">
-    <cfRule type="expression" dxfId="63" priority="589">
+    <cfRule type="expression" dxfId="84" priority="596">
       <formula>FIND(7,Q4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="590">
+    <cfRule type="expression" dxfId="83" priority="597">
       <formula>FIND(6, Q4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="591">
+    <cfRule type="expression" dxfId="82" priority="598">
       <formula>FIND(5,Q4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="592">
+    <cfRule type="expression" dxfId="81" priority="599">
       <formula>FIND(4,Q4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="593">
+    <cfRule type="expression" dxfId="80" priority="600">
       <formula>FIND(3, Q4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="594">
+    <cfRule type="expression" dxfId="79" priority="601">
       <formula>FIND(2, Q4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="595">
+    <cfRule type="expression" dxfId="78" priority="602">
       <formula>FIND(1, Q4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8 L27">
-    <cfRule type="expression" dxfId="56" priority="603">
+    <cfRule type="expression" dxfId="77" priority="610">
       <formula>FIND(7,O4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="604">
+    <cfRule type="expression" dxfId="76" priority="611">
       <formula>FIND(6, O4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="605">
+    <cfRule type="expression" dxfId="75" priority="612">
       <formula>FIND(5,O4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="606">
+    <cfRule type="expression" dxfId="74" priority="613">
       <formula>FIND(4,O4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="607">
+    <cfRule type="expression" dxfId="73" priority="614">
       <formula>FIND(3, O4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="608">
+    <cfRule type="expression" dxfId="72" priority="615">
       <formula>FIND(2, O4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="609">
+    <cfRule type="expression" dxfId="71" priority="616">
       <formula>FIND(1, O4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8 K27">
-    <cfRule type="expression" dxfId="49" priority="617">
+    <cfRule type="expression" dxfId="70" priority="624">
       <formula>FIND(7,M4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="618">
+    <cfRule type="expression" dxfId="69" priority="625">
       <formula>FIND(6, M4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="619">
+    <cfRule type="expression" dxfId="68" priority="626">
       <formula>FIND(5,M4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="620">
+    <cfRule type="expression" dxfId="67" priority="627">
       <formula>FIND(4,M4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="621">
+    <cfRule type="expression" dxfId="66" priority="628">
       <formula>FIND(3, M4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="622">
+    <cfRule type="expression" dxfId="65" priority="629">
       <formula>FIND(2, M4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="623">
+    <cfRule type="expression" dxfId="64" priority="630">
       <formula>FIND(1, M4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8 J27">
-    <cfRule type="expression" dxfId="42" priority="631">
+    <cfRule type="expression" dxfId="63" priority="638">
       <formula>FIND(7,K4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="632">
+    <cfRule type="expression" dxfId="62" priority="639">
       <formula>FIND(6, K4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="633">
+    <cfRule type="expression" dxfId="61" priority="640">
       <formula>FIND(5,K4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="634">
+    <cfRule type="expression" dxfId="60" priority="641">
       <formula>FIND(4,K4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="635">
+    <cfRule type="expression" dxfId="59" priority="642">
       <formula>FIND(3, K4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="636">
+    <cfRule type="expression" dxfId="58" priority="643">
       <formula>FIND(2, K4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="637">
+    <cfRule type="expression" dxfId="57" priority="644">
       <formula>FIND(1, K4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8 P27">
-    <cfRule type="expression" dxfId="35" priority="638">
+    <cfRule type="expression" dxfId="56" priority="645">
       <formula>FIND(7,W4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="639">
+    <cfRule type="expression" dxfId="55" priority="646">
       <formula>FIND(6, W4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="640">
+    <cfRule type="expression" dxfId="54" priority="647">
       <formula>FIND(5,W4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="641">
+    <cfRule type="expression" dxfId="53" priority="648">
       <formula>FIND(4,W4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="642">
+    <cfRule type="expression" dxfId="52" priority="649">
       <formula>FIND(3, W4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="643">
+    <cfRule type="expression" dxfId="51" priority="650">
       <formula>FIND(2, W4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="644">
+    <cfRule type="expression" dxfId="50" priority="651">
       <formula>FIND(1, W4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8 O27">
-    <cfRule type="expression" dxfId="28" priority="645">
+    <cfRule type="expression" dxfId="49" priority="652">
       <formula>FIND(7,U4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="646">
+    <cfRule type="expression" dxfId="48" priority="653">
       <formula>FIND(6, U4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="647">
+    <cfRule type="expression" dxfId="47" priority="654">
       <formula>FIND(5,U4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="648">
+    <cfRule type="expression" dxfId="46" priority="655">
       <formula>FIND(4,U4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="649">
+    <cfRule type="expression" dxfId="45" priority="656">
       <formula>FIND(3, U4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="650">
+    <cfRule type="expression" dxfId="44" priority="657">
       <formula>FIND(2, U4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="651">
+    <cfRule type="expression" dxfId="43" priority="658">
       <formula>FIND(1, U4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8 N27">
-    <cfRule type="expression" dxfId="21" priority="652">
+    <cfRule type="expression" dxfId="42" priority="659">
       <formula>FIND(7,S4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="653">
+    <cfRule type="expression" dxfId="41" priority="660">
       <formula>FIND(6, S4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="654">
+    <cfRule type="expression" dxfId="40" priority="661">
       <formula>FIND(5,S4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="655">
+    <cfRule type="expression" dxfId="39" priority="662">
       <formula>FIND(4,S4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="656">
+    <cfRule type="expression" dxfId="38" priority="663">
       <formula>FIND(3, S4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="657">
+    <cfRule type="expression" dxfId="37" priority="664">
       <formula>FIND(2, S4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="658">
+    <cfRule type="expression" dxfId="36" priority="665">
       <formula>FIND(1, S4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF29:AF38">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="35" priority="16">
       <formula>AND($AF$15=TRUE, SEARCH("6", AF29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="34" priority="17">
       <formula>AND($AF$10=TRUE, SEARCH("1", AF29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="33" priority="18">
       <formula>AND($AF$11=TRUE, SEARCH("2", AF29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="32" priority="19">
       <formula>AND($AF$12=TRUE, SEARCH("3", AF29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="31" priority="20">
       <formula>AND($AF$13=TRUE, SEARCH("4", AF29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="14">
+    <cfRule type="expression" dxfId="30" priority="21">
       <formula>AND($AF$14=TRUE, SEARCH("5", AF29))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="15">
+    <cfRule type="expression" dxfId="29" priority="22">
       <formula>AND($AF$19=TRUE, SEARCH("7", AF29))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:F18">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>AND($AF$29, SEARCH("1", E10))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>AND($AF$30, SEARCH("2", E10))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>AND($AF$31, SEARCH("3", E10))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>AND($AF$32, SEARCH("4", E10))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>AND($AF$33, SEARCH("5", E10))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>AND($AF$34, SEARCH("6", E10))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
-      <formula>AND($AF$38, SEARCH("7", E10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:F18">
-    <cfRule type="containsBlanks" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
+      <formula>AND($AF$29, SEARCH("1", F10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="9">
+      <formula>AND($AF$30, SEARCH("2", F10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="10">
+      <formula>AND($AF$31, SEARCH("3", F10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="11">
+      <formula>AND($AF$32, SEARCH("4", F10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="12">
+      <formula>AND($AF$33, SEARCH("5", F10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="13">
+      <formula>AND($AF$34, SEARCH("6", F10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="14">
+      <formula>AND($AF$38, SEARCH("7", F10))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F18">
+    <cfRule type="containsBlanks" dxfId="21" priority="15">
       <formula>LEN(TRIM(F10))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <conditionalFormatting sqref="E10:E18">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>AND($AF$10, SEARCH("1", E10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>AND($AF$11, SEARCH("2", E10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>AND($AF$12, SEARCH("3", E10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>AND($AF$13, SEARCH("4", E10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>AND($AF$14, SEARCH("5", E10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>AND($AF$15, SEARCH("6", E10))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>AND($AF$19, SEARCH("7", E10))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 B29" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Cb,C,C#,Db,D,D#,Eb,E,E#,Fb,F,F#,Gb,G,G#,Ab,A,A#,Bb,B,B#"</formula1>
     </dataValidation>
@@ -6975,8 +7226,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C15 C29:C34" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Cb,C,C#,Db,D,D#,Eb,e,E,E#,Fb,F,F#,Gb,G,G#,Ab,A,A#,Bb,B,B#"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B38 B19" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>"Ionian (Major),Dorian,Phrygian,Lydian,Mixolydian,Aolian (Minor),Locrian,Pentatonic Minor,Pentatonic Major,Harmonic Minor,Melodic Minor,Blues,Major Chord Tones,Minor Chord Tones,Diminished,Dominant"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B38" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>"Ionian (Major),Dorian,Phrygian,Lydian,Mixolydian,Aolian (Minor),Locrian,Pentatonic Minor,Pentatonic Major,Harmonic Minor,Melodic Minor,Blues,Major Chord Tones,Minor Chord Tones,Diminished"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{63CD6973-FBAC-467C-9C35-B07B23726C70}">
+      <formula1>"Ionian (Major),Dorian,Phrygian,Lydian,Mixolydian,Aolian (Minor),Locrian,Pentatonic Minor,Pentatonic Major,Harmonic Minor,Melodic Minor,Blues,Major Chord Tones,Minor Chord Tones,Diminished"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6989,8 +7243,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BN57"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -7025,10 +7279,10 @@
         <v>94</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="136" t="s">
+      <c r="F1" s="140" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="137"/>
+      <c r="G1" s="141"/>
       <c r="H1" s="112" t="s">
         <v>22</v>
       </c>
@@ -7304,10 +7558,10 @@
       <c r="D3" s="11">
         <v>10</v>
       </c>
-      <c r="F3" s="134" t="s">
+      <c r="F3" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="135"/>
+      <c r="G3" s="139"/>
       <c r="H3" s="14" t="s">
         <v>59</v>
       </c>
@@ -7437,7 +7691,7 @@
       </c>
       <c r="G4" s="9" t="str">
         <f>Fretboards!B19</f>
-        <v>Ionian (Major)</v>
+        <v>Lydian</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>171</v>
@@ -7552,10 +7806,10 @@
       <c r="D5" s="11">
         <v>8</v>
       </c>
-      <c r="F5" s="134" t="s">
+      <c r="F5" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="135"/>
+      <c r="G5" s="139"/>
       <c r="H5" s="14" t="s">
         <v>172</v>
       </c>
@@ -7814,42 +8068,22 @@
       <c r="D7" s="11">
         <v>11</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="9">
-        <v>2</v>
-      </c>
-      <c r="J7" s="9">
-        <v>2</v>
-      </c>
-      <c r="K7" s="9">
-        <v>1</v>
-      </c>
-      <c r="L7" s="9">
-        <v>2</v>
-      </c>
-      <c r="M7" s="9">
-        <v>2</v>
-      </c>
-      <c r="N7" s="9">
-        <v>1</v>
-      </c>
-      <c r="O7" s="114">
-        <v>2</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="114"/>
+      <c r="P7" s="9"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
-      <c r="W7" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="W7" s="6"/>
       <c r="X7" s="41">
         <v>6</v>
       </c>
@@ -9247,9 +9481,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>♯4</v>
       </c>
       <c r="M21" s="9">
         <f t="shared" si="0"/>
@@ -9311,11 +9545,11 @@
       </c>
       <c r="K22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!K20 + 1, FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!L20 + 1, FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!M20 + 1, FALSE)</f>
@@ -9379,7 +9613,7 @@
       </c>
       <c r="L23" s="9">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M23" s="9">
         <f t="shared" si="1"/>
@@ -9439,7 +9673,7 @@
       </c>
       <c r="L24" s="9" t="str">
         <f>IF(K22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + L20 - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:K22) + 1))</f>
-        <v>F</v>
+        <v>F♯</v>
       </c>
       <c r="M24" s="9" t="str">
         <f>IF(L22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + M20 - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:L22) + 1))</f>
@@ -9573,30 +9807,14 @@
         <f>VLOOKUP($G$6, Model!$H$2:$O$17, Model!O20 + 1, FALSE)</f>
         <v>2</v>
       </c>
-      <c r="P26" s="103" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q26" s="60">
-        <v>7</v>
-      </c>
-      <c r="R26" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="S26" s="60" t="s">
-        <v>187</v>
-      </c>
-      <c r="T26" s="60" t="s">
-        <v>184</v>
-      </c>
-      <c r="U26" s="60" t="s">
-        <v>183</v>
-      </c>
-      <c r="V26" s="60" t="s">
-        <v>183</v>
-      </c>
-      <c r="W26" s="105" t="s">
-        <v>184</v>
-      </c>
+      <c r="P26" s="103"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="60"/>
+      <c r="T26" s="60"/>
+      <c r="U26" s="60"/>
+      <c r="V26" s="60"/>
+      <c r="W26" s="105"/>
     </row>
     <row r="27" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
@@ -10143,7 +10361,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O43" s="114" t="b">
         <v>1</v>
@@ -10166,7 +10384,7 @@
         <v>1</v>
       </c>
       <c r="M44" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N44" s="9" t="b">
         <v>0</v>
@@ -10539,30 +10757,14 @@
       <c r="V55" s="8"/>
     </row>
     <row r="56" spans="8:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H56" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="L56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="M56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="N56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="O56" s="115" t="b">
-        <v>1</v>
-      </c>
+      <c r="H56" s="15"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="115"/>
       <c r="P56" s="8"/>
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>

</xml_diff>

<commit_message>
Fixed augmented chord names
</commit_message>
<xml_diff>
--- a/Shredsheets.xlsx
+++ b/Shredsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Shredsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71A45CF-767A-4BB6-AA3F-A08146B45853}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E701B99-6D30-494E-BC68-A8E03B29FAEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11970" yWindow="2475" windowWidth="26460" windowHeight="19635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12315" yWindow="1740" windowWidth="26460" windowHeight="19635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fretboards" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="204">
   <si>
     <t>Ionian</t>
   </si>
@@ -647,6 +647,15 @@
   </si>
   <si>
     <t>♯2</t>
+  </si>
+  <si>
+    <t>4♭♭7</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>+M7</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1768,14 +1777,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1817,45 +1821,48 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1868,1075 +1875,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="254">
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CC068"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81B2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF813997"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CC068"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81B2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CC068"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81B2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="127">
     <dxf>
       <font>
         <color theme="0" tint="-4.9989318521683403E-2"/>
@@ -4328,7 +3278,7 @@
   <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="Q25" sqref="Q25:R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -4460,23 +3410,23 @@
       <c r="A4" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="131" t="str">
+      <c r="B4" s="129" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B19 = "Ionian (Major)", B10 &amp; " Major", IF(B19 = "Aolian (Minor)", B10 &amp; " Minor", B10 &amp; " " &amp; B19)), "#", "♯"), "b", "♭")</f>
-        <v>C Major</v>
-      </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+        <v>C Augmented</v>
+      </c>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
       <c r="K4" s="126">
         <f>IF(J8 = "", "", IF(K5 = 0, F$1, K5))</f>
         <v>1</v>
       </c>
       <c r="L4" s="126"/>
-      <c r="M4" s="126">
+      <c r="M4" s="126" t="str">
         <f>IF(K8 = "", "", IF(M5 = 0, G$1, M5))</f>
-        <v>2</v>
+        <v>♯2</v>
       </c>
       <c r="N4" s="126"/>
       <c r="O4" s="126">
@@ -4484,9 +3434,9 @@
         <v>3</v>
       </c>
       <c r="P4" s="126"/>
-      <c r="Q4" s="126">
+      <c r="Q4" s="126" t="str">
         <f>IF(M8 = "", "", IF(Q5 = 0, I$1, Q5))</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="R4" s="126"/>
       <c r="S4" s="126">
@@ -4494,9 +3444,9 @@
         <v>5</v>
       </c>
       <c r="T4" s="126"/>
-      <c r="U4" s="126">
+      <c r="U4" s="126" t="str">
         <f>IF(O8 = "", "", IF(U5 = 0, K$1, U5))</f>
-        <v>6</v>
+        <v>♯5</v>
       </c>
       <c r="V4" s="126"/>
       <c r="W4" s="126">
@@ -4504,116 +3454,116 @@
         <v>7</v>
       </c>
       <c r="X4" s="126"/>
-      <c r="Z4" s="134" t="s">
+      <c r="Z4" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="AA4" s="134"/>
-      <c r="AB4" s="135" t="b">
+      <c r="AA4" s="121"/>
+      <c r="AB4" s="122" t="b">
         <v>0</v>
       </c>
-      <c r="AC4" s="135"/>
+      <c r="AC4" s="122"/>
     </row>
     <row r="5" spans="1:32" s="60" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="K5" s="128">
+      <c r="B5" s="129"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="K5" s="127">
         <f>IFERROR(HLOOKUP(F$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), F$1)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="128"/>
-      <c r="M5" s="128">
+      <c r="L5" s="127"/>
+      <c r="M5" s="127" t="str">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), G$1)</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="128"/>
-      <c r="O5" s="128">
+        <v>♯2</v>
+      </c>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), H$1)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="128"/>
-      <c r="Q5" s="128">
+      <c r="P5" s="127"/>
+      <c r="Q5" s="127">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), I$1)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="128"/>
-      <c r="S5" s="128">
+      <c r="R5" s="127"/>
+      <c r="S5" s="127">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), J$1)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="128"/>
-      <c r="U5" s="128">
+      <c r="T5" s="127"/>
+      <c r="U5" s="127" t="str">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), K$1)</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="128"/>
-      <c r="W5" s="128">
+        <v>♯5</v>
+      </c>
+      <c r="V5" s="127"/>
+      <c r="W5" s="127">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), L$1)</f>
         <v>0</v>
       </c>
-      <c r="X5" s="128"/>
-      <c r="Z5" s="134"/>
-      <c r="AA5" s="134"/>
-      <c r="AB5" s="135"/>
-      <c r="AC5" s="135"/>
+      <c r="X5" s="127"/>
+      <c r="Z5" s="121"/>
+      <c r="AA5" s="121"/>
+      <c r="AB5" s="122"/>
+      <c r="AC5" s="122"/>
     </row>
     <row r="6" spans="1:32" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="131"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="K6" s="129" t="str">
+      <c r="B6" s="129"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="K6" s="125" t="str">
         <f>IF(K$4="","", J$8 &amp; IFERROR(HLOOKUP(F$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), F$1))</f>
-        <v>CM7</v>
-      </c>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129" t="str">
+        <v>C+M7</v>
+      </c>
+      <c r="L6" s="125"/>
+      <c r="M6" s="125" t="str">
         <f>IF(M$4="","", K$8 &amp; IFERROR(HLOOKUP(G$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), G$1))</f>
-        <v>Dm7</v>
-      </c>
-      <c r="N6" s="129"/>
-      <c r="O6" s="129" t="str">
+        <v>D♯4♭♭7</v>
+      </c>
+      <c r="N6" s="125"/>
+      <c r="O6" s="125" t="str">
         <f>IF(O$4="","", L$8 &amp; IFERROR(HLOOKUP(H$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), H$1))</f>
-        <v>Em7</v>
-      </c>
-      <c r="P6" s="129"/>
-      <c r="Q6" s="129" t="str">
+        <v>EM7</v>
+      </c>
+      <c r="P6" s="125"/>
+      <c r="Q6" s="125" t="str">
         <f>IF(Q$4="","", M$8 &amp; IFERROR(HLOOKUP(I$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), I$1))</f>
-        <v>FM7</v>
-      </c>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129" t="str">
+        <v/>
+      </c>
+      <c r="R6" s="125"/>
+      <c r="S6" s="125" t="str">
         <f>IF(S$4="","", N$8 &amp; IFERROR(HLOOKUP(J$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), J$1))</f>
-        <v>G7</v>
-      </c>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129" t="str">
+        <v>G+</v>
+      </c>
+      <c r="T6" s="125"/>
+      <c r="U6" s="125" t="str">
         <f>IF(U$4="","", O$8 &amp; IFERROR(HLOOKUP(K$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), K$1))</f>
-        <v>Am7</v>
-      </c>
-      <c r="V6" s="129"/>
-      <c r="W6" s="129" t="str">
+        <v>G♯m</v>
+      </c>
+      <c r="V6" s="125"/>
+      <c r="W6" s="125" t="str">
         <f>IF(W$4="","", P$8 &amp; IFERROR(HLOOKUP(L$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), L$1))</f>
-        <v>Bm7ø</v>
-      </c>
-      <c r="X6" s="129"/>
-      <c r="Z6" s="134"/>
-      <c r="AA6" s="134"/>
-      <c r="AB6" s="135"/>
-      <c r="AC6" s="135"/>
+        <v>B6</v>
+      </c>
+      <c r="X6" s="125"/>
+      <c r="Z6" s="121"/>
+      <c r="AA6" s="121"/>
+      <c r="AB6" s="122"/>
+      <c r="AC6" s="122"/>
     </row>
     <row r="7" spans="1:32" s="61" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="131"/>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
-      <c r="F7" s="131"/>
-      <c r="G7" s="131"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
       <c r="J7" s="95"/>
       <c r="K7" s="95"/>
       <c r="L7" s="95"/>
@@ -4621,29 +3571,29 @@
       <c r="N7" s="95"/>
       <c r="O7" s="95"/>
       <c r="P7" s="95"/>
-      <c r="Z7" s="134"/>
-      <c r="AA7" s="134"/>
-      <c r="AB7" s="135"/>
-      <c r="AC7" s="135"/>
+      <c r="Z7" s="121"/>
+      <c r="AA7" s="121"/>
+      <c r="AB7" s="122"/>
+      <c r="AC7" s="122"/>
     </row>
     <row r="8" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="132" t="s">
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="132"/>
+      <c r="I8" s="130"/>
       <c r="J8" s="73" t="str">
         <f>Model!I24</f>
         <v>C</v>
       </c>
       <c r="K8" s="74" t="str">
         <f>IF(Model!I22=0, "", Model!J24)</f>
-        <v>D</v>
+        <v>D♯</v>
       </c>
       <c r="L8" s="75" t="str">
         <f>IF(Model!J22=0, "", Model!K24)</f>
@@ -4651,7 +3601,7 @@
       </c>
       <c r="M8" s="76" t="str">
         <f>IF(Model!K22=0, "", Model!L24)</f>
-        <v>F</v>
+        <v/>
       </c>
       <c r="N8" s="77" t="str">
         <f>IF(Model!L22=0, "", Model!M24)</f>
@@ -4659,49 +3609,49 @@
       </c>
       <c r="O8" s="78" t="str">
         <f>IF(Model!M22=0, "", Model!N24)</f>
-        <v>A</v>
+        <v>G♯</v>
       </c>
       <c r="P8" s="79" t="str">
         <f>IF(Model!N22=0, "", Model!O24)</f>
         <v>B</v>
       </c>
-      <c r="S8" s="133" t="s">
+      <c r="S8" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
+      <c r="T8" s="131"/>
+      <c r="U8" s="131"/>
       <c r="V8" s="98" t="str">
         <f>IF(Model!I22=1, "h", IF(Model!I22=2, "W", IF(Model!I22=3, "W+h", IF(Model!I22=4, "WW", IF(Model!I22=0, "", Model!I22)))))</f>
-        <v>W</v>
+        <v>W+h</v>
       </c>
       <c r="W8" s="80" t="str">
         <f>IF(Model!J22=1, "h", IF(Model!J22=2, "W", IF(Model!J22=3, "W+h", IF(Model!J22=4, "WW", IF(Model!J22=0, "", Model!J22)))))</f>
-        <v>W</v>
+        <v>h</v>
       </c>
       <c r="X8" s="81" t="str">
         <f>IF(Model!K22=1, "h", IF(Model!K22=2, "W", IF(Model!K22=3, "W+h", IF(Model!K22=4, "WW", IF(Model!K22=0, "", Model!K22)))))</f>
-        <v>h</v>
+        <v/>
       </c>
       <c r="Y8" s="82" t="str">
         <f>IF(Model!L22=1, "h", IF(Model!L22=2, "W", IF(Model!L22=3, "W+h",IF(Model!L22=4, "WW", IF(Model!L22=0, "", Model!L22)))))</f>
-        <v>W</v>
+        <v>W+h</v>
       </c>
       <c r="Z8" s="83" t="str">
         <f>IF(Model!M22=1, "h", IF(Model!M22=2, "W", IF(Model!M22=3, "W+h",IF(Model!M22=4, "WW", IF(Model!M22=0, "", Model!M22)))))</f>
-        <v>W</v>
+        <v>h</v>
       </c>
       <c r="AA8" s="84" t="str">
         <f>IF(Model!N22=1, "h", IF(Model!N22=2, "W", IF(Model!N22=3, "W+h", IF(Model!N22=4, "WW", IF(Model!N22=0, "", Model!N22)))))</f>
-        <v>W</v>
+        <v>W+h</v>
       </c>
       <c r="AB8" s="85" t="str">
         <f>IF(Model!O22=1, "h", IF(Model!O22=2, "W", IF(Model!O22=3, "W+h",IF(Model!O22=4, "WW", IF(Model!O22=0, "", Model!O22)))))</f>
         <v>h</v>
       </c>
-      <c r="AE8" s="137" t="s">
+      <c r="AE8" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="AF8" s="137"/>
+      <c r="AF8" s="124"/>
     </row>
     <row r="9" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="93" t="s">
@@ -4711,11 +3661,11 @@
         <v>17</v>
       </c>
       <c r="D9" s="37"/>
-      <c r="E9" s="122">
+      <c r="E9" s="117">
         <f t="shared" ref="E9:AC9" si="0">IF($AB$4, 24-E$1, E$1)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="124">
+      <c r="F9" s="119">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4819,7 +3769,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="136" t="s">
+      <c r="B10" s="123" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="64" t="s">
@@ -4833,9 +3783,9 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>E : 3</v>
       </c>
-      <c r="F10" s="119" t="str">
+      <c r="F10" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="G10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4847,11 +3797,11 @@
       </c>
       <c r="I10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="J10" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="K10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4871,11 +3821,11 @@
       </c>
       <c r="O10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="P10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="Q10" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4883,7 +3833,7 @@
       </c>
       <c r="R10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="S10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4895,11 +3845,11 @@
       </c>
       <c r="U10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="V10" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="W10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4919,11 +3869,11 @@
       </c>
       <c r="AA10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="AB10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="AC10" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4932,13 +3882,13 @@
       <c r="AE10" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="AF10" s="120" t="b">
+      <c r="AF10" s="115" t="b">
         <f>HLOOKUP(F$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="136"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="64" t="s">
         <v>16</v>
       </c>
@@ -4950,7 +3900,7 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>B : 7</v>
       </c>
-      <c r="F11" s="119" t="str">
+      <c r="F11" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>C : 1</v>
       </c>
@@ -4960,11 +3910,11 @@
       </c>
       <c r="H11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="I11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="J11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4972,7 +3922,7 @@
       </c>
       <c r="K11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="L11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4984,11 +3934,11 @@
       </c>
       <c r="N11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="O11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="P11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5008,11 +3958,11 @@
       </c>
       <c r="T11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="U11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="V11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5020,7 +3970,7 @@
       </c>
       <c r="W11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="X11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5032,11 +3982,11 @@
       </c>
       <c r="Z11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="AA11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="AB11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5049,13 +3999,13 @@
       <c r="AE11" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="AF11" s="120" t="b">
+      <c r="AF11" s="115" t="b">
         <f>HLOOKUP(G$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="136"/>
+      <c r="B12" s="123"/>
       <c r="C12" s="64" t="s">
         <v>15</v>
       </c>
@@ -5067,13 +4017,13 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>G : 5</v>
       </c>
-      <c r="F12" s="119" t="str">
+      <c r="F12" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="G12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="H12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5093,11 +4043,11 @@
       </c>
       <c r="L12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="M12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="N12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5105,7 +4055,7 @@
       </c>
       <c r="O12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="P12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5117,11 +4067,11 @@
       </c>
       <c r="R12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="S12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="T12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5141,11 +4091,11 @@
       </c>
       <c r="X12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="Y12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="Z12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5153,7 +4103,7 @@
       </c>
       <c r="AA12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="AB12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5166,13 +4116,13 @@
       <c r="AE12" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="AF12" s="120" t="b">
+      <c r="AF12" s="115" t="b">
         <f>HLOOKUP(H$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="136"/>
+      <c r="B13" s="123"/>
       <c r="C13" s="64" t="s">
         <v>12</v>
       </c>
@@ -5182,11 +4132,11 @@
       </c>
       <c r="E13" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
-      </c>
-      <c r="F13" s="119" t="str">
+        <v/>
+      </c>
+      <c r="F13" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="G13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5194,7 +4144,7 @@
       </c>
       <c r="H13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="I13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5206,11 +4156,11 @@
       </c>
       <c r="K13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="L13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="M13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5230,11 +4180,11 @@
       </c>
       <c r="Q13" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="R13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="S13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5242,7 +4192,7 @@
       </c>
       <c r="T13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="U13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5254,11 +4204,11 @@
       </c>
       <c r="W13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="X13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="Y13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5278,18 +4228,18 @@
       </c>
       <c r="AC13" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="AE13" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="AF13" s="120" t="b">
+      <c r="AF13" s="115" t="b">
         <f>HLOOKUP(I$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="136"/>
+      <c r="B14" s="123"/>
       <c r="C14" s="64" t="s">
         <v>14</v>
       </c>
@@ -5299,9 +4249,9 @@
       </c>
       <c r="E14" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
-      </c>
-      <c r="F14" s="119" t="str">
+        <v/>
+      </c>
+      <c r="F14" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v/>
       </c>
@@ -5319,11 +4269,11 @@
       </c>
       <c r="J14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="K14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="L14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5331,7 +4281,7 @@
       </c>
       <c r="M14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="N14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5343,11 +4293,11 @@
       </c>
       <c r="P14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="Q14" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="R14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5367,11 +4317,11 @@
       </c>
       <c r="V14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="W14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="X14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5379,7 +4329,7 @@
       </c>
       <c r="Y14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="Z14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5391,22 +4341,22 @@
       </c>
       <c r="AB14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="AC14" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="AE14" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="AF14" s="120" t="b">
+      <c r="AF14" s="115" t="b">
         <f>HLOOKUP(J$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="128" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="64" t="s">
@@ -5420,9 +4370,9 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
         <v>E : 3</v>
       </c>
-      <c r="F15" s="119" t="str">
+      <c r="F15" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="G15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5434,11 +4384,11 @@
       </c>
       <c r="I15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="J15" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="K15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5458,11 +4408,11 @@
       </c>
       <c r="O15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="P15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="Q15" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5470,7 +4420,7 @@
       </c>
       <c r="R15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="S15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5482,11 +4432,11 @@
       </c>
       <c r="U15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>G♯ : ♯5</v>
       </c>
       <c r="V15" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="W15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5506,11 +4456,11 @@
       </c>
       <c r="AA15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="AB15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D♯ : ♯2</v>
       </c>
       <c r="AC15" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -5519,13 +4469,13 @@
       <c r="AE15" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="AF15" s="120" t="b">
+      <c r="AF15" s="115" t="b">
         <f>HLOOKUP(K$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="130"/>
+      <c r="B16" s="128"/>
       <c r="C16" s="64" t="s">
         <v>16</v>
       </c>
@@ -5537,7 +4487,7 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+E$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v>B : 7</v>
       </c>
-      <c r="F16" s="119" t="str">
+      <c r="F16" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+F$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v>C : 1</v>
       </c>
@@ -5547,11 +4497,11 @@
       </c>
       <c r="H16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+H$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="I16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+I$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D♯ : 2</v>
       </c>
       <c r="J16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+J$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5559,7 +4509,7 @@
       </c>
       <c r="K16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+K$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="L16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+L$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5571,11 +4521,11 @@
       </c>
       <c r="N16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+N$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>G♯ : 6</v>
       </c>
       <c r="O16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+O$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="P16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+P$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5595,11 +4545,11 @@
       </c>
       <c r="T16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+T$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="U16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+U$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D♯ : 2</v>
       </c>
       <c r="V16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+V$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5607,7 +4557,7 @@
       </c>
       <c r="W16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+W$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="X16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+X$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5619,11 +4569,11 @@
       </c>
       <c r="Z16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+Z$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>G♯ : 6</v>
       </c>
       <c r="AA16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+AA$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="AB16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+AB$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5634,10 +4584,10 @@
         <v>B : 7</v>
       </c>
       <c r="AE16" s="90"/>
-      <c r="AF16" s="121"/>
+      <c r="AF16" s="116"/>
     </row>
     <row r="17" spans="2:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="130"/>
+      <c r="B17" s="128"/>
       <c r="C17" s="64" t="s">
         <v>32</v>
       </c>
@@ -5649,17 +4599,17 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+E$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v/>
       </c>
-      <c r="F17" s="119" t="str">
+      <c r="F17" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+F$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v>G : 5</v>
       </c>
       <c r="G17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+G$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>G♯ : 6</v>
       </c>
       <c r="H17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+H$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="I17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+I$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5679,11 +4629,11 @@
       </c>
       <c r="M17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+M$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="N17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+N$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D♯ : 2</v>
       </c>
       <c r="O17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+O$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5691,7 +4641,7 @@
       </c>
       <c r="P17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+P$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="Q17" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+Q$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5703,11 +4653,11 @@
       </c>
       <c r="S17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+S$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>G♯ : 6</v>
       </c>
       <c r="T17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+T$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="U17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+U$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5727,11 +4677,11 @@
       </c>
       <c r="Y17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+Y$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="Z17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+Z$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D♯ : 2</v>
       </c>
       <c r="AA17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+AA$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5739,17 +4689,17 @@
       </c>
       <c r="AB17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+AB$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="AC17" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+AC$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v/>
       </c>
       <c r="AE17" s="91"/>
-      <c r="AF17" s="121"/>
+      <c r="AF17" s="116"/>
     </row>
     <row r="18" spans="2:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="130"/>
+      <c r="B18" s="128"/>
       <c r="C18" s="64" t="s">
         <v>30</v>
       </c>
@@ -5761,13 +4711,13 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+E$9, 12), Model!$I$23:$O$23, 0), "")</f>
         <v/>
       </c>
-      <c r="F18" s="119" t="str">
+      <c r="F18" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+F$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="G18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+G$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D♯ : 2</v>
       </c>
       <c r="H18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+H$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5775,7 +4725,7 @@
       </c>
       <c r="I18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+I$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="J18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+J$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5787,11 +4737,11 @@
       </c>
       <c r="L18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+L$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>G♯ : 6</v>
       </c>
       <c r="M18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+M$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="N18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+N$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5811,11 +4761,11 @@
       </c>
       <c r="R18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+R$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="S18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+S$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D♯ : 2</v>
       </c>
       <c r="T18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+T$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5823,7 +4773,7 @@
       </c>
       <c r="U18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+U$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>F : 4</v>
+        <v/>
       </c>
       <c r="V18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+V$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5835,11 +4785,11 @@
       </c>
       <c r="X18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+X$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>G♯ : 6</v>
       </c>
       <c r="Y18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+Y$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="Z18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+Z$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -5858,11 +4808,11 @@
         <v/>
       </c>
       <c r="AE18" s="92"/>
-      <c r="AF18" s="121"/>
+      <c r="AF18" s="116"/>
     </row>
     <row r="19" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="67" t="s">
-        <v>170</v>
+        <v>197</v>
       </c>
       <c r="C19" s="65"/>
       <c r="D19" s="1"/>
@@ -5969,7 +4919,7 @@
       <c r="AE19" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="AF19" s="120" t="b">
+      <c r="AF19" s="115" t="b">
         <f>HLOOKUP(L$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
         <v>1</v>
       </c>
@@ -6060,15 +5010,15 @@
       <c r="AF22" s="60"/>
     </row>
     <row r="23" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="131" t="str">
+      <c r="B23" s="129" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B38 = "Ionian (Major)", B29 &amp; " Major", IF(B38 = "Aolian (Minor)", B29 &amp; " Minor", B29 &amp; " " &amp; B38)), "#", "♯"), "b", "♭")</f>
         <v>E Pentatonic Minor</v>
       </c>
-      <c r="C23" s="131"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="131"/>
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="129"/>
       <c r="K23" s="126">
         <f>IF(J27 = "", "", IF(K24 = 0, F$1, K24))</f>
         <v>1</v>
@@ -6114,47 +5064,47 @@
       <c r="AF23" s="60"/>
     </row>
     <row r="24" spans="2:32" s="59" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="131"/>
-      <c r="K24" s="127">
+      <c r="B24" s="129"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="129"/>
+      <c r="K24" s="132">
         <f>IFERROR(HLOOKUP(F$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), F$1)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127">
+      <c r="L24" s="132"/>
+      <c r="M24" s="132">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), G$1)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="127"/>
-      <c r="O24" s="127" t="str">
+      <c r="N24" s="132"/>
+      <c r="O24" s="132" t="str">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), H$1)</f>
         <v>♭3</v>
       </c>
-      <c r="P24" s="127"/>
-      <c r="Q24" s="127">
+      <c r="P24" s="132"/>
+      <c r="Q24" s="132">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), I$1)</f>
         <v>0</v>
       </c>
-      <c r="R24" s="127"/>
-      <c r="S24" s="127">
+      <c r="R24" s="132"/>
+      <c r="S24" s="132">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), J$1)</f>
         <v>0</v>
       </c>
-      <c r="T24" s="127"/>
-      <c r="U24" s="127">
+      <c r="T24" s="132"/>
+      <c r="U24" s="132">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), K$1)</f>
         <v>0</v>
       </c>
-      <c r="V24" s="127"/>
-      <c r="W24" s="127" t="str">
+      <c r="V24" s="132"/>
+      <c r="W24" s="132" t="str">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), L$1)</f>
         <v>♭7</v>
       </c>
-      <c r="X24" s="127"/>
+      <c r="X24" s="132"/>
       <c r="Y24" s="60"/>
       <c r="Z24" s="60"/>
       <c r="AA24" s="60"/>
@@ -6165,47 +5115,47 @@
       <c r="AF24" s="60"/>
     </row>
     <row r="25" spans="2:32" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="131"/>
-      <c r="C25" s="131"/>
-      <c r="D25" s="131"/>
-      <c r="E25" s="131"/>
-      <c r="F25" s="131"/>
-      <c r="G25" s="131"/>
-      <c r="K25" s="125" t="str">
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="129"/>
+      <c r="K25" s="133" t="str">
         <f>IF(K$23="","", J$27 &amp; IFERROR(HLOOKUP(F$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), F$1))</f>
         <v>Em7</v>
       </c>
-      <c r="L25" s="125"/>
-      <c r="M25" s="125" t="str">
+      <c r="L25" s="133"/>
+      <c r="M25" s="133" t="str">
         <f>IF(M$23="","", K$27 &amp; IFERROR(HLOOKUP(G$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), G$1))</f>
         <v/>
       </c>
-      <c r="N25" s="125"/>
-      <c r="O25" s="125" t="str">
+      <c r="N25" s="133"/>
+      <c r="O25" s="133" t="str">
         <f>IF(O$23="","", L$27 &amp; IFERROR(HLOOKUP(H$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), H$1))</f>
         <v>GM</v>
       </c>
-      <c r="P25" s="125"/>
-      <c r="Q25" s="125" t="str">
+      <c r="P25" s="133"/>
+      <c r="Q25" s="133" t="str">
         <f>IF(Q$23="","", M$27 &amp; IFERROR(HLOOKUP(I$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), I$1))</f>
         <v>A5 ♭7</v>
       </c>
-      <c r="R25" s="125"/>
-      <c r="S25" s="125" t="str">
+      <c r="R25" s="133"/>
+      <c r="S25" s="133" t="str">
         <f>IF(S$23="","", N$27 &amp; IFERROR(HLOOKUP(J$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), J$1))</f>
         <v>B5</v>
       </c>
-      <c r="T25" s="125"/>
-      <c r="U25" s="125" t="str">
+      <c r="T25" s="133"/>
+      <c r="U25" s="133" t="str">
         <f>IF(U$23="","", O$27 &amp; IFERROR(HLOOKUP(K$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), K$1))</f>
         <v/>
       </c>
-      <c r="V25" s="125"/>
-      <c r="W25" s="125" t="str">
+      <c r="V25" s="133"/>
+      <c r="W25" s="133" t="str">
         <f>IF(W$23="","", P$27 &amp; IFERROR(HLOOKUP(L$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), L$1))</f>
         <v>D5</v>
       </c>
-      <c r="X25" s="125"/>
+      <c r="X25" s="133"/>
       <c r="Y25" s="60"/>
       <c r="Z25" s="60"/>
       <c r="AA25" s="60"/>
@@ -6216,12 +5166,12 @@
       <c r="AF25" s="60"/>
     </row>
     <row r="26" spans="2:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="131"/>
-      <c r="C26" s="131"/>
-      <c r="D26" s="131"/>
-      <c r="E26" s="131"/>
-      <c r="F26" s="131"/>
-      <c r="G26" s="131"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
       <c r="H26" s="61"/>
       <c r="I26" s="61"/>
       <c r="J26" s="94"/>
@@ -6249,16 +5199,16 @@
       <c r="AF26" s="61"/>
     </row>
     <row r="27" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="131"/>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="132" t="s">
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="129"/>
+      <c r="F27" s="129"/>
+      <c r="G27" s="129"/>
+      <c r="H27" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="132"/>
+      <c r="I27" s="130"/>
       <c r="J27" s="73" t="str">
         <f>Model!I29</f>
         <v>E</v>
@@ -6287,11 +5237,11 @@
         <f>IF(Model!N29=0, "", Model!O29)</f>
         <v>D</v>
       </c>
-      <c r="S27" s="133" t="s">
+      <c r="S27" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="T27" s="133"/>
-      <c r="U27" s="133"/>
+      <c r="T27" s="131"/>
+      <c r="U27" s="131"/>
       <c r="V27" s="98" t="str">
         <f>IF(Model!I27=1, "h", IF(Model!I27=2, "W", IF(Model!I27=3, "W+h", IF(Model!I27=4, "WW", IF(Model!I27=0, "", Model!I22)))))</f>
         <v/>
@@ -6320,10 +5270,10 @@
         <f>IF(Model!O27=1, "h", IF(Model!O27=2, "W", IF(Model!O27=3, "W+h", IF(Model!O27=4, "WW", IF(Model!O27=0, "", Model!O22)))))</f>
         <v>W</v>
       </c>
-      <c r="AE27" s="137" t="s">
+      <c r="AE27" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="AF27" s="137"/>
+      <c r="AF27" s="124"/>
     </row>
     <row r="28" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="93" t="s">
@@ -6333,11 +5283,11 @@
         <v>17</v>
       </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="122">
+      <c r="E28" s="117">
         <f t="shared" ref="E28:AC28" si="2">IF($AB$4, 24-E$1, E$1)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="123">
+      <c r="F28" s="118">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -6441,7 +5391,7 @@
       </c>
     </row>
     <row r="29" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="136" t="s">
+      <c r="B29" s="123" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="64" t="s">
@@ -6451,11 +5401,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C29), Model!$B$2:$D$41, 3)</f>
         <v>4</v>
       </c>
-      <c r="E29" s="118" t="str">
+      <c r="E29" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D29+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D29+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>E : 1</v>
       </c>
-      <c r="F29" s="119" t="str">
+      <c r="F29" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D29+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D29+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
@@ -6555,13 +5505,13 @@
       <c r="AE29" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="AF29" s="120" t="b">
+      <c r="AF29" s="115" t="b">
         <f>HLOOKUP(F$1, Model!$I$41:$O$57, MATCH($B$38, Model!$H$41:$H$57, 0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="136"/>
+      <c r="B30" s="123"/>
       <c r="C30" s="64" t="s">
         <v>16</v>
       </c>
@@ -6569,11 +5519,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C30), Model!$B$2:$D$41, 3)</f>
         <v>11</v>
       </c>
-      <c r="E30" s="118" t="str">
+      <c r="E30" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D30+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D30+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>B : 5</v>
       </c>
-      <c r="F30" s="119" t="str">
+      <c r="F30" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D30+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D30+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
@@ -6673,13 +5623,13 @@
       <c r="AE30" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="AF30" s="120" t="b">
+      <c r="AF30" s="115" t="b">
         <f>HLOOKUP(G$1, Model!$I$41:$O$57, MATCH($B$38, Model!$H$41:$H$57, 0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="136"/>
+      <c r="B31" s="123"/>
       <c r="C31" s="64" t="s">
         <v>15</v>
       </c>
@@ -6687,11 +5637,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C31), Model!$B$2:$D$41, 3)</f>
         <v>7</v>
       </c>
-      <c r="E31" s="118" t="str">
+      <c r="E31" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D31+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D31+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>G : 3</v>
       </c>
-      <c r="F31" s="119" t="str">
+      <c r="F31" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D31+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D31+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
@@ -6791,13 +5741,13 @@
       <c r="AE31" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="AF31" s="120" t="b">
+      <c r="AF31" s="115" t="b">
         <f>HLOOKUP(H$1, Model!$I$41:$O$57, MATCH($B$38, Model!$H$41:$H$57, 0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="136"/>
+      <c r="B32" s="123"/>
       <c r="C32" s="64" t="s">
         <v>12</v>
       </c>
@@ -6805,11 +5755,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C32), Model!$B$2:$D$41, 3)</f>
         <v>2</v>
       </c>
-      <c r="E32" s="118" t="str">
+      <c r="E32" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D32+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D32+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>D : 7</v>
       </c>
-      <c r="F32" s="119" t="str">
+      <c r="F32" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D32+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D32+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
@@ -6909,13 +5859,13 @@
       <c r="AE32" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="AF32" s="120" t="b">
+      <c r="AF32" s="115" t="b">
         <f>HLOOKUP(I$1, Model!$I$41:$O$57, MATCH($B$38, Model!$H$41:$H$57, 0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="136"/>
+      <c r="B33" s="123"/>
       <c r="C33" s="64" t="s">
         <v>14</v>
       </c>
@@ -6923,11 +5873,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C33), Model!$B$2:$D$41, 3)</f>
         <v>9</v>
       </c>
-      <c r="E33" s="118" t="str">
+      <c r="E33" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D33+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D33+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>A : 4</v>
       </c>
-      <c r="F33" s="119" t="str">
+      <c r="F33" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D33+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D33+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
@@ -7027,13 +5977,13 @@
       <c r="AE33" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="AF33" s="120" t="b">
+      <c r="AF33" s="115" t="b">
         <f>HLOOKUP(J$1, Model!$I$41:$O$57, MATCH($B$38, Model!$H$41:$H$57, 0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="130" t="s">
+      <c r="B34" s="128" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="64" t="s">
@@ -7043,11 +5993,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C34), Model!$B$2:$D$41, 3)</f>
         <v>4</v>
       </c>
-      <c r="E34" s="118" t="str">
+      <c r="E34" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D34+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D34+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>E : 1</v>
       </c>
-      <c r="F34" s="119" t="str">
+      <c r="F34" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D34+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D34+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
@@ -7147,13 +6097,13 @@
       <c r="AE34" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="AF34" s="120" t="b">
+      <c r="AF34" s="115" t="b">
         <f>HLOOKUP(K$1, Model!$I$41:$O$57, MATCH($B$38, Model!$H$41:$H$57, 0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="130"/>
+      <c r="B35" s="128"/>
       <c r="C35" s="64" t="s">
         <v>16</v>
       </c>
@@ -7161,11 +6111,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C35), Model!$B$2:$D$41, 3)</f>
         <v>11</v>
       </c>
-      <c r="E35" s="118" t="str">
+      <c r="E35" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D35+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D35+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>B : 5</v>
       </c>
-      <c r="F35" s="119" t="str">
+      <c r="F35" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D35+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D35+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
@@ -7263,10 +6213,10 @@
       </c>
       <c r="AD35" s="63"/>
       <c r="AE35" s="90"/>
-      <c r="AF35" s="121"/>
+      <c r="AF35" s="116"/>
     </row>
     <row r="36" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="130"/>
+      <c r="B36" s="128"/>
       <c r="C36" s="64" t="s">
         <v>32</v>
       </c>
@@ -7274,11 +6224,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C36), Model!$B$2:$D$41, 3)</f>
         <v>6</v>
       </c>
-      <c r="E36" s="118" t="str">
+      <c r="E36" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D36+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D36+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
-      <c r="F36" s="119" t="str">
+      <c r="F36" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D36+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D36+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>G : 3</v>
       </c>
@@ -7376,10 +6326,10 @@
       </c>
       <c r="AD36" s="63"/>
       <c r="AE36" s="91"/>
-      <c r="AF36" s="121"/>
+      <c r="AF36" s="116"/>
     </row>
     <row r="37" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="130"/>
+      <c r="B37" s="128"/>
       <c r="C37" s="64" t="s">
         <v>30</v>
       </c>
@@ -7387,11 +6337,11 @@
         <f>VLOOKUP(UPPER(Fretboards!C37), Model!$B$2:$D$41, 3)</f>
         <v>1</v>
       </c>
-      <c r="E37" s="118" t="str">
+      <c r="E37" s="113" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D37+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D37+E$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v/>
       </c>
-      <c r="F37" s="119" t="str">
+      <c r="F37" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D37+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$29, 10) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D37+F$28, 12), Model!$I$28:$O$28, 0), Model!$I$20:$O$26, 6), "")</f>
         <v>D : 7</v>
       </c>
@@ -7489,7 +6439,7 @@
       </c>
       <c r="AD37" s="63"/>
       <c r="AE37" s="92"/>
-      <c r="AF37" s="121"/>
+      <c r="AF37" s="116"/>
     </row>
     <row r="38" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="67" t="s">
@@ -7600,7 +6550,7 @@
       <c r="AE38" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="AF38" s="120" t="b">
+      <c r="AF38" s="115" t="b">
         <f>HLOOKUP(L$1, Model!$I$41:$O$57, MATCH($B$38, Model!$H$41:$H$57, 0))</f>
         <v>1</v>
       </c>
@@ -7634,10 +6584,50 @@
       <c r="AC39" s="68"/>
     </row>
     <row r="41" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B41" s="110"/>
+      <c r="B41" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B23:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B4:G8"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
     <mergeCell ref="Z4:AA7"/>
     <mergeCell ref="AB4:AC7"/>
     <mergeCell ref="B10:B14"/>
@@ -7654,46 +6644,6 @@
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="U5:V5"/>
     <mergeCell ref="U6:V6"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B23:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B4:G8"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U25:V25"/>
   </mergeCells>
   <conditionalFormatting sqref="AB4 AF10:AF19">
     <cfRule type="expression" dxfId="126" priority="548">
@@ -8166,7 +7116,7 @@
   <dimension ref="A1:BN58"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28:O28"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -8201,11 +7151,11 @@
         <v>94</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="140" t="s">
+      <c r="F1" s="136" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="141"/>
-      <c r="H1" s="112" t="s">
+      <c r="G1" s="137"/>
+      <c r="H1" s="107" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="17"/>
@@ -8214,7 +7164,7 @@
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
-      <c r="O1" s="113"/>
+      <c r="O1" s="108"/>
       <c r="P1" s="99" t="s">
         <v>60</v>
       </c>
@@ -8367,7 +7317,7 @@
       <c r="N2" s="9">
         <v>2</v>
       </c>
-      <c r="O2" s="114">
+      <c r="O2" s="109">
         <v>2</v>
       </c>
       <c r="P2" s="9" t="s">
@@ -8480,10 +7430,10 @@
       <c r="D3" s="11">
         <v>10</v>
       </c>
-      <c r="F3" s="138" t="s">
+      <c r="F3" s="134" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="139"/>
+      <c r="G3" s="135"/>
       <c r="H3" s="14" t="s">
         <v>59</v>
       </c>
@@ -8505,7 +7455,7 @@
       <c r="N3" s="9">
         <v>3</v>
       </c>
-      <c r="O3" s="114">
+      <c r="O3" s="109">
         <v>1</v>
       </c>
       <c r="P3" s="9" t="s">
@@ -8613,7 +7563,7 @@
       </c>
       <c r="G4" s="9" t="str">
         <f>Fretboards!B19</f>
-        <v>Ionian (Major)</v>
+        <v>Augmented</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>171</v>
@@ -8636,7 +7586,7 @@
       <c r="N4" s="9">
         <v>4</v>
       </c>
-      <c r="O4" s="114">
+      <c r="O4" s="109">
         <v>1</v>
       </c>
       <c r="P4" s="9" t="s">
@@ -8728,10 +7678,10 @@
       <c r="D5" s="11">
         <v>8</v>
       </c>
-      <c r="F5" s="138" t="s">
+      <c r="F5" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="139"/>
+      <c r="G5" s="135"/>
       <c r="H5" s="14" t="s">
         <v>172</v>
       </c>
@@ -8753,7 +7703,7 @@
       <c r="N5" s="9">
         <v>3</v>
       </c>
-      <c r="O5" s="114">
+      <c r="O5" s="109">
         <v>2</v>
       </c>
       <c r="P5" s="9" t="s">
@@ -8876,7 +7826,7 @@
       <c r="N6" s="9">
         <v>3</v>
       </c>
-      <c r="O6" s="114">
+      <c r="O6" s="109">
         <v>2</v>
       </c>
       <c r="P6" s="9" t="s">
@@ -9011,7 +7961,7 @@
       <c r="N7" s="9">
         <v>3</v>
       </c>
-      <c r="O7" s="114">
+      <c r="O7" s="109">
         <v>1</v>
       </c>
       <c r="P7" s="9" t="s">
@@ -9128,7 +8078,7 @@
       <c r="N8" s="9">
         <v>1</v>
       </c>
-      <c r="O8" s="114">
+      <c r="O8" s="109">
         <v>2</v>
       </c>
       <c r="P8" s="9" t="s">
@@ -9246,7 +8196,7 @@
       <c r="N9" s="9">
         <v>3</v>
       </c>
-      <c r="O9" s="114">
+      <c r="O9" s="109">
         <v>1</v>
       </c>
       <c r="P9" s="9" t="s">
@@ -9380,7 +8330,7 @@
       <c r="N10" s="9">
         <v>2</v>
       </c>
-      <c r="O10" s="114">
+      <c r="O10" s="109">
         <v>1</v>
       </c>
       <c r="P10" s="9" t="s">
@@ -9510,7 +8460,7 @@
       <c r="N11" s="9">
         <v>2</v>
       </c>
-      <c r="O11" s="114">
+      <c r="O11" s="109">
         <v>2</v>
       </c>
       <c r="P11" s="9" t="s">
@@ -9638,7 +8588,7 @@
       <c r="N12" s="9">
         <v>2</v>
       </c>
-      <c r="O12" s="114">
+      <c r="O12" s="109">
         <v>1</v>
       </c>
       <c r="P12" s="9" t="s">
@@ -9768,7 +8718,7 @@
       <c r="N13" s="9">
         <v>2</v>
       </c>
-      <c r="O13" s="114">
+      <c r="O13" s="109">
         <v>1</v>
       </c>
       <c r="P13" s="9" t="s">
@@ -9909,7 +8859,7 @@
       <c r="N14" s="9">
         <v>1</v>
       </c>
-      <c r="O14" s="114">
+      <c r="O14" s="109">
         <v>2</v>
       </c>
       <c r="P14" s="9" t="s">
@@ -10039,7 +8989,7 @@
       <c r="N15" s="9">
         <v>0</v>
       </c>
-      <c r="O15" s="114">
+      <c r="O15" s="109">
         <v>2</v>
       </c>
       <c r="P15" s="9" t="s">
@@ -10169,7 +9119,7 @@
       <c r="N16" s="9">
         <v>3</v>
       </c>
-      <c r="O16" s="114">
+      <c r="O16" s="109">
         <v>2</v>
       </c>
       <c r="P16" s="9" t="s">
@@ -10258,7 +9208,7 @@
       <c r="N17" s="16">
         <v>2</v>
       </c>
-      <c r="O17" s="115">
+      <c r="O17" s="110">
         <v>2</v>
       </c>
       <c r="P17" s="16" t="s">
@@ -10417,9 +9367,9 @@
         <f>IF(VLOOKUP($G$4,$P$2:$W$17, 1+I20, FALSE) = 0, I20, VLOOKUP($G$4,$P$2:$W$17, 1+I20, FALSE))</f>
         <v>1</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="9" t="str">
         <f t="shared" ref="J21:O21" si="0">IF(VLOOKUP($G$4,$P$2:$W$17, 1+J20, FALSE) = 0, J20, VLOOKUP($G$4,$P$2:$W$17, 1+J20, FALSE))</f>
-        <v>2</v>
+        <v>♯2</v>
       </c>
       <c r="K21" s="9">
         <f t="shared" si="0"/>
@@ -10433,9 +9383,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>♯5</v>
       </c>
       <c r="O21" s="9">
         <f t="shared" si="0"/>
@@ -10444,25 +9394,25 @@
       <c r="P21" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="Q21" s="6" t="s">
+      <c r="Q21" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="R21" s="6" t="s">
+      <c r="R21" s="139" t="s">
         <v>194</v>
       </c>
-      <c r="S21" s="6" t="s">
+      <c r="S21" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="T21" s="60" t="s">
+      <c r="T21" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="U21" s="60" t="s">
+      <c r="U21" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="V21" s="6" t="s">
+      <c r="V21" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="W21" s="104">
+      <c r="W21" s="140">
         <v>7</v>
       </c>
     </row>
@@ -10481,27 +9431,27 @@
       </c>
       <c r="I22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!I20 + 1, FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!J20 + 1, FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!K20 + 1, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!L20 + 1, FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!M20 + 1, FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!N20 + 1, FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!O20 + 1, FALSE)</f>
@@ -10510,23 +9460,23 @@
       <c r="P22" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="Q22" s="6" t="s">
+      <c r="Q22" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6" t="s">
+      <c r="R22" s="139"/>
+      <c r="S22" s="139" t="s">
         <v>182</v>
       </c>
-      <c r="T22" s="6" t="s">
+      <c r="T22" s="139" t="s">
         <v>189</v>
       </c>
-      <c r="U22" s="6" t="s">
+      <c r="U22" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="V22" s="6" t="s">
+      <c r="V22" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="W22" s="104" t="s">
+      <c r="W22" s="140" t="s">
         <v>183</v>
       </c>
     </row>
@@ -10549,15 +9499,15 @@
       </c>
       <c r="J23" s="9">
         <f t="shared" ref="J23:O23" si="1">IFERROR(VLOOKUP(SUBSTITUTE(SUBSTITUTE(J24, "♭", "b"), "♯","#"), $B$2:$D$41, 3, FALSE), "")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K23" s="9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="M23" s="9">
         <f t="shared" si="1"/>
@@ -10565,7 +9515,7 @@
       </c>
       <c r="N23" s="9">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O23" s="9">
         <f t="shared" si="1"/>
@@ -10574,19 +9524,19 @@
       <c r="P23" s="103" t="s">
         <v>171</v>
       </c>
-      <c r="Q23" s="6" t="s">
+      <c r="Q23" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="R23" s="6"/>
-      <c r="S23" s="60" t="s">
+      <c r="R23" s="139"/>
+      <c r="S23" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="T23" s="60"/>
-      <c r="U23" s="60">
+      <c r="T23" s="138"/>
+      <c r="U23" s="138">
         <v>7</v>
       </c>
-      <c r="V23" s="60"/>
-      <c r="W23" s="105" t="s">
+      <c r="V23" s="138"/>
+      <c r="W23" s="141" t="s">
         <v>194</v>
       </c>
     </row>
@@ -10609,7 +9559,7 @@
       </c>
       <c r="J24" s="9" t="str">
         <f>IF(I22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(J21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:I22) + 1))</f>
-        <v>D</v>
+        <v>D♯</v>
       </c>
       <c r="K24" s="9" t="str">
         <f>IF(J22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(K21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:J22) + 1))</f>
@@ -10617,7 +9567,7 @@
       </c>
       <c r="L24" s="9" t="str">
         <f>IF(K22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(L21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:K22) + 1))</f>
-        <v>F</v>
+        <v/>
       </c>
       <c r="M24" s="9" t="str">
         <f>IF(L22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(M21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:L22) + 1))</f>
@@ -10625,7 +9575,7 @@
       </c>
       <c r="N24" s="9" t="str">
         <f>IF(M22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(N21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:M22) + 1))</f>
-        <v>A</v>
+        <v>G♯</v>
       </c>
       <c r="O24" s="9" t="str">
         <f>IF(N22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(O21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:N22) + 1))</f>
@@ -10634,19 +9584,19 @@
       <c r="P24" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="Q24" s="6" t="s">
+      <c r="Q24" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6" t="s">
+      <c r="R24" s="139"/>
+      <c r="S24" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60" t="s">
+      <c r="T24" s="138"/>
+      <c r="U24" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="V24" s="6"/>
-      <c r="W24" s="104">
+      <c r="V24" s="139"/>
+      <c r="W24" s="140">
         <v>7</v>
       </c>
     </row>
@@ -10687,19 +9637,19 @@
       <c r="P25" s="103" t="s">
         <v>173</v>
       </c>
-      <c r="Q25" s="6" t="s">
+      <c r="Q25" s="139" t="s">
         <v>186</v>
       </c>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6" t="s">
+      <c r="R25" s="139"/>
+      <c r="S25" s="139" t="s">
         <v>186</v>
       </c>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6" t="s">
+      <c r="T25" s="139"/>
+      <c r="U25" s="139" t="s">
         <v>186</v>
       </c>
-      <c r="V25" s="6"/>
-      <c r="W25" s="104" t="s">
+      <c r="V25" s="139"/>
+      <c r="W25" s="140" t="s">
         <v>186</v>
       </c>
     </row>
@@ -10717,45 +9667,55 @@
         <v>60</v>
       </c>
       <c r="I26" s="9">
-        <f>IF(VLOOKUP($G$6,$P$2:$W$19, 1+I20, FALSE) = 0, I20, VLOOKUP($G$6,$P$2:$W$19, 1+I20, FALSE))</f>
+        <f t="shared" ref="I26:O26" si="2">IF(VLOOKUP($G$6,$P$2:$W$19, 1+I20, FALSE) = 0, I20, VLOOKUP($G$6,$P$2:$W$19, 1+I20, FALSE))</f>
         <v>1</v>
       </c>
       <c r="J26" s="9">
-        <f>IF(VLOOKUP($G$6,$P$2:$W$19, 1+J20, FALSE) = 0, J20, VLOOKUP($G$6,$P$2:$W$19, 1+J20, FALSE))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K26" s="9" t="str">
-        <f>IF(VLOOKUP($G$6,$P$2:$W$19, 1+K20, FALSE) = 0, K20, VLOOKUP($G$6,$P$2:$W$19, 1+K20, FALSE))</f>
+        <f t="shared" si="2"/>
         <v>♭3</v>
       </c>
       <c r="L26" s="9">
-        <f>IF(VLOOKUP($G$6,$P$2:$W$19, 1+L20, FALSE) = 0, L20, VLOOKUP($G$6,$P$2:$W$19, 1+L20, FALSE))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M26" s="9">
-        <f>IF(VLOOKUP($G$6,$P$2:$W$19, 1+M20, FALSE) = 0, M20, VLOOKUP($G$6,$P$2:$W$19, 1+M20, FALSE))</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="N26" s="9">
-        <f>IF(VLOOKUP($G$6,$P$2:$W$19, 1+N20, FALSE) = 0, N20, VLOOKUP($G$6,$P$2:$W$19, 1+N20, FALSE))</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="O26" s="9" t="str">
-        <f>IF(VLOOKUP($G$6,$P$2:$W$19, 1+O20, FALSE) = 0, O20, VLOOKUP($G$6,$P$2:$W$19, 1+O20, FALSE))</f>
+        <f t="shared" si="2"/>
         <v>♭7</v>
       </c>
       <c r="P26" s="103" t="s">
         <v>197</v>
       </c>
-      <c r="Q26" s="60" t="s">
+      <c r="Q26" s="138" t="s">
+        <v>203</v>
+      </c>
+      <c r="R26" s="139" t="s">
+        <v>201</v>
+      </c>
+      <c r="S26" s="139" t="s">
+        <v>184</v>
+      </c>
+      <c r="T26" s="138"/>
+      <c r="U26" s="138" t="s">
         <v>198</v>
       </c>
-      <c r="R26" s="6"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="60"/>
-      <c r="V26" s="60"/>
-      <c r="W26" s="105"/>
+      <c r="V26" s="138" t="s">
+        <v>202</v>
+      </c>
+      <c r="W26" s="141">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
@@ -10801,25 +9761,25 @@
       <c r="P27" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="Q27" s="6" t="s">
+      <c r="Q27" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="R27" s="6" t="s">
+      <c r="R27" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="S27" s="6" t="s">
+      <c r="S27" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="T27" s="60">
+      <c r="T27" s="138">
         <v>7</v>
       </c>
-      <c r="U27" s="60" t="s">
+      <c r="U27" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="V27" s="60" t="s">
+      <c r="V27" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="W27" s="104" t="s">
+      <c r="W27" s="140" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10836,56 +9796,56 @@
       <c r="H28" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="142">
+      <c r="I28" s="120">
         <f>IFERROR(VLOOKUP(SUBSTITUTE(SUBSTITUTE(I29, "♭", "b"), "♯","#"), $B$2:$D$41, 3, FALSE), "")</f>
         <v>4</v>
       </c>
-      <c r="J28" s="142" t="str">
-        <f t="shared" ref="J28:O28" si="2">IFERROR(VLOOKUP(SUBSTITUTE(SUBSTITUTE(J29, "♭", "b"), "♯","#"), $B$2:$D$41, 3, FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="K28" s="142">
-        <f t="shared" si="2"/>
+      <c r="J28" s="120" t="str">
+        <f t="shared" ref="J28:O28" si="3">IFERROR(VLOOKUP(SUBSTITUTE(SUBSTITUTE(J29, "♭", "b"), "♯","#"), $B$2:$D$41, 3, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="K28" s="120">
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="L28" s="142">
-        <f t="shared" si="2"/>
+      <c r="L28" s="120">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="M28" s="142">
-        <f t="shared" si="2"/>
+      <c r="M28" s="120">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="N28" s="142" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O28" s="142">
-        <f t="shared" si="2"/>
+      <c r="N28" s="120" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O28" s="120">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P28" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="Q28" s="60" t="s">
+      <c r="Q28" s="138" t="s">
         <v>193</v>
       </c>
-      <c r="R28" s="6" t="s">
+      <c r="R28" s="139" t="s">
         <v>187</v>
       </c>
-      <c r="S28" s="6" t="s">
+      <c r="S28" s="139" t="s">
         <v>188</v>
       </c>
-      <c r="T28" s="6" t="s">
+      <c r="T28" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="U28" s="6">
+      <c r="U28" s="139">
         <v>7</v>
       </c>
-      <c r="V28" s="6" t="s">
+      <c r="V28" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="W28" s="104" t="s">
+      <c r="W28" s="140" t="s">
         <v>186</v>
       </c>
     </row>
@@ -10933,25 +9893,25 @@
       <c r="P29" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="Q29" s="6" t="s">
+      <c r="Q29" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="R29" s="6" t="s">
+      <c r="R29" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="S29" s="60" t="s">
+      <c r="S29" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="T29" s="60" t="s">
+      <c r="T29" s="138" t="s">
         <v>184</v>
       </c>
-      <c r="U29" s="60">
+      <c r="U29" s="138">
         <v>7</v>
       </c>
-      <c r="V29" s="60" t="s">
+      <c r="V29" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="W29" s="105" t="s">
+      <c r="W29" s="141" t="s">
         <v>194</v>
       </c>
     </row>
@@ -10968,25 +9928,25 @@
       <c r="P30" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="Q30" s="139" t="s">
         <v>194</v>
       </c>
-      <c r="R30" s="6" t="s">
+      <c r="R30" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="S30" s="60" t="s">
+      <c r="S30" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="T30" s="60" t="s">
+      <c r="T30" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="U30" s="6" t="s">
+      <c r="U30" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="V30" s="6">
+      <c r="V30" s="139">
         <v>7</v>
       </c>
-      <c r="W30" s="104" t="s">
+      <c r="W30" s="140" t="s">
         <v>183</v>
       </c>
     </row>
@@ -11011,25 +9971,25 @@
       <c r="P31" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="Q31" s="6" t="s">
+      <c r="Q31" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="R31" s="60">
+      <c r="R31" s="138">
         <v>7</v>
       </c>
-      <c r="S31" s="60" t="s">
+      <c r="S31" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="T31" s="60" t="s">
+      <c r="T31" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="U31" s="6" t="s">
+      <c r="U31" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="V31" s="6" t="s">
+      <c r="V31" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="W31" s="105" t="s">
+      <c r="W31" s="141" t="s">
         <v>183</v>
       </c>
     </row>
@@ -11047,25 +10007,25 @@
       <c r="P32" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="Q32" s="60" t="s">
+      <c r="Q32" s="138" t="s">
         <v>193</v>
       </c>
-      <c r="R32" s="60" t="s">
+      <c r="R32" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="S32" s="6" t="s">
+      <c r="S32" s="139" t="s">
         <v>190</v>
       </c>
-      <c r="T32" s="60">
+      <c r="T32" s="138">
         <v>7</v>
       </c>
-      <c r="U32" s="60">
+      <c r="U32" s="138">
         <v>7</v>
       </c>
-      <c r="V32" s="60" t="s">
+      <c r="V32" s="138" t="s">
         <v>187</v>
       </c>
-      <c r="W32" s="105" t="s">
+      <c r="W32" s="141" t="s">
         <v>187</v>
       </c>
     </row>
@@ -11079,29 +10039,29 @@
       <c r="D33" s="11">
         <v>7</v>
       </c>
-      <c r="H33" s="111"/>
+      <c r="H33" s="106"/>
       <c r="P33" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="Q33" s="60">
+      <c r="Q33" s="138">
         <v>7</v>
       </c>
-      <c r="R33" s="60" t="s">
+      <c r="R33" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="S33" s="60" t="s">
+      <c r="S33" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="T33" s="6" t="s">
+      <c r="T33" s="139" t="s">
         <v>184</v>
       </c>
-      <c r="U33" s="6" t="s">
+      <c r="U33" s="139" t="s">
         <v>183</v>
       </c>
-      <c r="V33" s="60" t="s">
+      <c r="V33" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="W33" s="104" t="s">
+      <c r="W33" s="140" t="s">
         <v>184</v>
       </c>
     </row>
@@ -11115,27 +10075,27 @@
       <c r="D34" s="11">
         <v>8</v>
       </c>
-      <c r="H34" s="111"/>
+      <c r="H34" s="106"/>
       <c r="P34" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="Q34" s="60" t="s">
+      <c r="Q34" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="R34" s="60" t="s">
+      <c r="R34" s="138" t="s">
         <v>185</v>
       </c>
-      <c r="S34" s="60" t="s">
+      <c r="S34" s="138" t="s">
         <v>191</v>
       </c>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6">
+      <c r="T34" s="139"/>
+      <c r="U34" s="139">
         <v>5</v>
       </c>
-      <c r="V34" s="60" t="s">
+      <c r="V34" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="W34" s="104"/>
+      <c r="W34" s="140"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B35" s="9" t="s">
@@ -11147,25 +10107,25 @@
       <c r="D35" s="11">
         <v>9</v>
       </c>
-      <c r="H35" s="111"/>
+      <c r="H35" s="106"/>
       <c r="P35" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="Q35" s="60" t="s">
+      <c r="Q35" s="138" t="s">
         <v>183</v>
       </c>
-      <c r="R35" s="6"/>
-      <c r="S35" s="6" t="s">
+      <c r="R35" s="139"/>
+      <c r="S35" s="139" t="s">
         <v>182</v>
       </c>
-      <c r="T35" s="60" t="s">
+      <c r="T35" s="138" t="s">
         <v>192</v>
       </c>
-      <c r="U35" s="6">
+      <c r="U35" s="139">
         <v>5</v>
       </c>
-      <c r="V35" s="6"/>
-      <c r="W35" s="104">
+      <c r="V35" s="139"/>
+      <c r="W35" s="140">
         <v>5</v>
       </c>
     </row>
@@ -11179,29 +10139,29 @@
       <c r="D36" s="11">
         <v>6</v>
       </c>
-      <c r="H36" s="111"/>
-      <c r="P36" s="106" t="s">
+      <c r="H36" s="106"/>
+      <c r="P36" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="Q36" s="107" t="s">
+      <c r="Q36" s="142" t="s">
         <v>183</v>
       </c>
-      <c r="R36" s="107" t="s">
+      <c r="R36" s="142" t="s">
         <v>184</v>
       </c>
-      <c r="S36" s="108">
+      <c r="S36" s="143">
         <v>7</v>
       </c>
-      <c r="T36" s="108" t="s">
+      <c r="T36" s="143" t="s">
         <v>183</v>
       </c>
-      <c r="U36" s="108" t="s">
+      <c r="U36" s="143" t="s">
         <v>194</v>
       </c>
-      <c r="V36" s="107" t="s">
+      <c r="V36" s="142" t="s">
         <v>184</v>
       </c>
-      <c r="W36" s="109" t="s">
+      <c r="W36" s="144" t="s">
         <v>183</v>
       </c>
     </row>
@@ -11215,17 +10175,17 @@
       <c r="D37" s="11">
         <v>5</v>
       </c>
-      <c r="H37" s="111"/>
+      <c r="H37" s="106"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.35">
       <c r="D38" s="11"/>
-      <c r="H38" s="111"/>
+      <c r="H38" s="106"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="11"/>
-      <c r="H39" s="111"/>
+      <c r="H39" s="106"/>
     </row>
     <row r="40" spans="2:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="9"/>
@@ -11236,7 +10196,7 @@
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="13"/>
-      <c r="H41" s="116" t="s">
+      <c r="H41" s="111" t="s">
         <v>195</v>
       </c>
       <c r="I41" s="99">
@@ -11257,7 +10217,7 @@
       <c r="N41" s="99">
         <v>6</v>
       </c>
-      <c r="O41" s="117">
+      <c r="O41" s="112">
         <v>7</v>
       </c>
     </row>
@@ -11285,7 +10245,7 @@
       <c r="N42" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O42" s="114" t="b">
+      <c r="O42" s="109" t="b">
         <v>1</v>
       </c>
     </row>
@@ -11311,7 +10271,7 @@
       <c r="N43" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O43" s="114" t="b">
+      <c r="O43" s="109" t="b">
         <v>1</v>
       </c>
     </row>
@@ -11337,7 +10297,7 @@
       <c r="N44" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O44" s="114" t="b">
+      <c r="O44" s="109" t="b">
         <v>1</v>
       </c>
     </row>
@@ -11363,7 +10323,7 @@
       <c r="N45" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O45" s="114" t="b">
+      <c r="O45" s="109" t="b">
         <v>0</v>
       </c>
       <c r="P45" s="8"/>
@@ -11396,7 +10356,7 @@
       <c r="N46" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O46" s="114" t="b">
+      <c r="O46" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P46" s="8"/>
@@ -11429,7 +10389,7 @@
       <c r="N47" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O47" s="114" t="b">
+      <c r="O47" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P47" s="8"/>
@@ -11462,7 +10422,7 @@
       <c r="N48" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O48" s="114" t="b">
+      <c r="O48" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P48" s="8"/>
@@ -11495,7 +10455,7 @@
       <c r="N49" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O49" s="114" t="b">
+      <c r="O49" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P49" s="8"/>
@@ -11528,7 +10488,7 @@
       <c r="N50" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O50" s="114" t="b">
+      <c r="O50" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P50" s="8"/>
@@ -11561,7 +10521,7 @@
       <c r="N51" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O51" s="114" t="b">
+      <c r="O51" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P51" s="8"/>
@@ -11594,7 +10554,7 @@
       <c r="N52" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O52" s="114" t="b">
+      <c r="O52" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P52" s="8"/>
@@ -11627,7 +10587,7 @@
       <c r="N53" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O53" s="114" t="b">
+      <c r="O53" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P53" s="8"/>
@@ -11660,7 +10620,7 @@
       <c r="N54" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O54" s="114" t="b">
+      <c r="O54" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P54" s="8"/>
@@ -11693,7 +10653,7 @@
       <c r="N55" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O55" s="114" t="b">
+      <c r="O55" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P55" s="8"/>
@@ -11726,7 +10686,7 @@
       <c r="N56" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O56" s="114" t="b">
+      <c r="O56" s="109" t="b">
         <v>1</v>
       </c>
       <c r="P56" s="8"/>
@@ -11759,7 +10719,7 @@
       <c r="N57" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="O57" s="115" t="b">
+      <c r="O57" s="110" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Restored Ionian default 1st fret board, and removed headings / formula bar
</commit_message>
<xml_diff>
--- a/Shredsheets.xlsx
+++ b/Shredsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Shredsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E701B99-6D30-494E-BC68-A8E03B29FAEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6809AE7C-AE3C-4643-AB6F-96D51BB16E08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12315" yWindow="1740" windowWidth="26460" windowHeight="19635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1365" windowWidth="26460" windowHeight="19635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fretboards" sheetId="1" r:id="rId1"/>
@@ -1824,57 +1824,6 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1882,6 +1831,57 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3277,8 +3277,8 @@
   </sheetPr>
   <dimension ref="A1:AF41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25:R25"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3410,160 +3410,160 @@
       <c r="A4" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="129" t="str">
+      <c r="B4" s="134" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B19 = "Ionian (Major)", B10 &amp; " Major", IF(B19 = "Aolian (Minor)", B10 &amp; " Minor", B10 &amp; " " &amp; B19)), "#", "♯"), "b", "♭")</f>
-        <v>C Augmented</v>
-      </c>
-      <c r="C4" s="129"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="K4" s="126">
+        <v>C Major</v>
+      </c>
+      <c r="C4" s="134"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="K4" s="129">
         <f>IF(J8 = "", "", IF(K5 = 0, F$1, K5))</f>
         <v>1</v>
       </c>
-      <c r="L4" s="126"/>
-      <c r="M4" s="126" t="str">
+      <c r="L4" s="129"/>
+      <c r="M4" s="129">
         <f>IF(K8 = "", "", IF(M5 = 0, G$1, M5))</f>
-        <v>♯2</v>
-      </c>
-      <c r="N4" s="126"/>
-      <c r="O4" s="126">
+        <v>2</v>
+      </c>
+      <c r="N4" s="129"/>
+      <c r="O4" s="129">
         <f>IF(L8 = "", "", IF(O5 = 0, H$1, O5))</f>
         <v>3</v>
       </c>
-      <c r="P4" s="126"/>
-      <c r="Q4" s="126" t="str">
+      <c r="P4" s="129"/>
+      <c r="Q4" s="129">
         <f>IF(M8 = "", "", IF(Q5 = 0, I$1, Q5))</f>
-        <v/>
-      </c>
-      <c r="R4" s="126"/>
-      <c r="S4" s="126">
+        <v>4</v>
+      </c>
+      <c r="R4" s="129"/>
+      <c r="S4" s="129">
         <f>IF(N8 = "", "", IF(S5 = 0, J$1, S5))</f>
         <v>5</v>
       </c>
-      <c r="T4" s="126"/>
-      <c r="U4" s="126" t="str">
+      <c r="T4" s="129"/>
+      <c r="U4" s="129">
         <f>IF(O8 = "", "", IF(U5 = 0, K$1, U5))</f>
-        <v>♯5</v>
-      </c>
-      <c r="V4" s="126"/>
-      <c r="W4" s="126">
+        <v>6</v>
+      </c>
+      <c r="V4" s="129"/>
+      <c r="W4" s="129">
         <f>IF(P8 = "", "", IF(W5 = 0, L$1, W5))</f>
         <v>7</v>
       </c>
-      <c r="X4" s="126"/>
-      <c r="Z4" s="121" t="s">
+      <c r="X4" s="129"/>
+      <c r="Z4" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="AA4" s="121"/>
-      <c r="AB4" s="122" t="b">
+      <c r="AA4" s="137"/>
+      <c r="AB4" s="138" t="b">
         <v>0</v>
       </c>
-      <c r="AC4" s="122"/>
+      <c r="AC4" s="138"/>
     </row>
     <row r="5" spans="1:32" s="60" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="129"/>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
-      <c r="K5" s="127">
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="K5" s="131">
         <f>IFERROR(HLOOKUP(F$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), F$1)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="127"/>
-      <c r="M5" s="127" t="str">
+      <c r="L5" s="131"/>
+      <c r="M5" s="131">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), G$1)</f>
-        <v>♯2</v>
-      </c>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127">
+        <v>0</v>
+      </c>
+      <c r="N5" s="131"/>
+      <c r="O5" s="131">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), H$1)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="127"/>
-      <c r="Q5" s="127">
+      <c r="P5" s="131"/>
+      <c r="Q5" s="131">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), I$1)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="127"/>
-      <c r="S5" s="127">
+      <c r="R5" s="131"/>
+      <c r="S5" s="131">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), J$1)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="127"/>
-      <c r="U5" s="127" t="str">
+      <c r="T5" s="131"/>
+      <c r="U5" s="131">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), K$1)</f>
-        <v>♯5</v>
-      </c>
-      <c r="V5" s="127"/>
-      <c r="W5" s="127">
+        <v>0</v>
+      </c>
+      <c r="V5" s="131"/>
+      <c r="W5" s="131">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$1:$W$17, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), L$1)</f>
         <v>0</v>
       </c>
-      <c r="X5" s="127"/>
-      <c r="Z5" s="121"/>
-      <c r="AA5" s="121"/>
-      <c r="AB5" s="122"/>
-      <c r="AC5" s="122"/>
+      <c r="X5" s="131"/>
+      <c r="Z5" s="137"/>
+      <c r="AA5" s="137"/>
+      <c r="AB5" s="138"/>
+      <c r="AC5" s="138"/>
     </row>
     <row r="6" spans="1:32" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="K6" s="125" t="str">
+      <c r="B6" s="134"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="K6" s="132" t="str">
         <f>IF(K$4="","", J$8 &amp; IFERROR(HLOOKUP(F$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), F$1))</f>
-        <v>C+M7</v>
-      </c>
-      <c r="L6" s="125"/>
-      <c r="M6" s="125" t="str">
+        <v>CM7</v>
+      </c>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132" t="str">
         <f>IF(M$4="","", K$8 &amp; IFERROR(HLOOKUP(G$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), G$1))</f>
-        <v>D♯4♭♭7</v>
-      </c>
-      <c r="N6" s="125"/>
-      <c r="O6" s="125" t="str">
+        <v>Dm7</v>
+      </c>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132" t="str">
         <f>IF(O$4="","", L$8 &amp; IFERROR(HLOOKUP(H$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), H$1))</f>
-        <v>EM7</v>
-      </c>
-      <c r="P6" s="125"/>
-      <c r="Q6" s="125" t="str">
+        <v>Em7</v>
+      </c>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132" t="str">
         <f>IF(Q$4="","", M$8 &amp; IFERROR(HLOOKUP(I$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), I$1))</f>
-        <v/>
-      </c>
-      <c r="R6" s="125"/>
-      <c r="S6" s="125" t="str">
+        <v>FM7</v>
+      </c>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132" t="str">
         <f>IF(S$4="","", N$8 &amp; IFERROR(HLOOKUP(J$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), J$1))</f>
-        <v>G+</v>
-      </c>
-      <c r="T6" s="125"/>
-      <c r="U6" s="125" t="str">
+        <v>G7</v>
+      </c>
+      <c r="T6" s="132"/>
+      <c r="U6" s="132" t="str">
         <f>IF(U$4="","", O$8 &amp; IFERROR(HLOOKUP(K$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), K$1))</f>
-        <v>G♯m</v>
-      </c>
-      <c r="V6" s="125"/>
-      <c r="W6" s="125" t="str">
+        <v>Am7</v>
+      </c>
+      <c r="V6" s="132"/>
+      <c r="W6" s="132" t="str">
         <f>IF(W$4="","", P$8 &amp; IFERROR(HLOOKUP(L$1, Model!$P$20:$W$36, MATCH($B$19, Model!$P$2:$P$20, 0) + 1), L$1))</f>
-        <v>B6</v>
-      </c>
-      <c r="X6" s="125"/>
-      <c r="Z6" s="121"/>
-      <c r="AA6" s="121"/>
-      <c r="AB6" s="122"/>
-      <c r="AC6" s="122"/>
+        <v>Bm7ø</v>
+      </c>
+      <c r="X6" s="132"/>
+      <c r="Z6" s="137"/>
+      <c r="AA6" s="137"/>
+      <c r="AB6" s="138"/>
+      <c r="AC6" s="138"/>
     </row>
     <row r="7" spans="1:32" s="61" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
       <c r="J7" s="95"/>
       <c r="K7" s="95"/>
       <c r="L7" s="95"/>
@@ -3571,29 +3571,29 @@
       <c r="N7" s="95"/>
       <c r="O7" s="95"/>
       <c r="P7" s="95"/>
-      <c r="Z7" s="121"/>
-      <c r="AA7" s="121"/>
-      <c r="AB7" s="122"/>
-      <c r="AC7" s="122"/>
+      <c r="Z7" s="137"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="138"/>
+      <c r="AC7" s="138"/>
     </row>
     <row r="8" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="129"/>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
-      <c r="H8" s="130" t="s">
+      <c r="B8" s="134"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="130"/>
+      <c r="I8" s="135"/>
       <c r="J8" s="73" t="str">
         <f>Model!I24</f>
         <v>C</v>
       </c>
       <c r="K8" s="74" t="str">
         <f>IF(Model!I22=0, "", Model!J24)</f>
-        <v>D♯</v>
+        <v>D</v>
       </c>
       <c r="L8" s="75" t="str">
         <f>IF(Model!J22=0, "", Model!K24)</f>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="M8" s="76" t="str">
         <f>IF(Model!K22=0, "", Model!L24)</f>
-        <v/>
+        <v>F</v>
       </c>
       <c r="N8" s="77" t="str">
         <f>IF(Model!L22=0, "", Model!M24)</f>
@@ -3609,49 +3609,49 @@
       </c>
       <c r="O8" s="78" t="str">
         <f>IF(Model!M22=0, "", Model!N24)</f>
-        <v>G♯</v>
+        <v>A</v>
       </c>
       <c r="P8" s="79" t="str">
         <f>IF(Model!N22=0, "", Model!O24)</f>
         <v>B</v>
       </c>
-      <c r="S8" s="131" t="s">
+      <c r="S8" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
+      <c r="T8" s="136"/>
+      <c r="U8" s="136"/>
       <c r="V8" s="98" t="str">
         <f>IF(Model!I22=1, "h", IF(Model!I22=2, "W", IF(Model!I22=3, "W+h", IF(Model!I22=4, "WW", IF(Model!I22=0, "", Model!I22)))))</f>
-        <v>W+h</v>
+        <v>W</v>
       </c>
       <c r="W8" s="80" t="str">
         <f>IF(Model!J22=1, "h", IF(Model!J22=2, "W", IF(Model!J22=3, "W+h", IF(Model!J22=4, "WW", IF(Model!J22=0, "", Model!J22)))))</f>
-        <v>h</v>
+        <v>W</v>
       </c>
       <c r="X8" s="81" t="str">
         <f>IF(Model!K22=1, "h", IF(Model!K22=2, "W", IF(Model!K22=3, "W+h", IF(Model!K22=4, "WW", IF(Model!K22=0, "", Model!K22)))))</f>
-        <v/>
+        <v>h</v>
       </c>
       <c r="Y8" s="82" t="str">
         <f>IF(Model!L22=1, "h", IF(Model!L22=2, "W", IF(Model!L22=3, "W+h",IF(Model!L22=4, "WW", IF(Model!L22=0, "", Model!L22)))))</f>
-        <v>W+h</v>
+        <v>W</v>
       </c>
       <c r="Z8" s="83" t="str">
         <f>IF(Model!M22=1, "h", IF(Model!M22=2, "W", IF(Model!M22=3, "W+h",IF(Model!M22=4, "WW", IF(Model!M22=0, "", Model!M22)))))</f>
-        <v>h</v>
+        <v>W</v>
       </c>
       <c r="AA8" s="84" t="str">
         <f>IF(Model!N22=1, "h", IF(Model!N22=2, "W", IF(Model!N22=3, "W+h", IF(Model!N22=4, "WW", IF(Model!N22=0, "", Model!N22)))))</f>
-        <v>W+h</v>
+        <v>W</v>
       </c>
       <c r="AB8" s="85" t="str">
         <f>IF(Model!O22=1, "h", IF(Model!O22=2, "W", IF(Model!O22=3, "W+h",IF(Model!O22=4, "WW", IF(Model!O22=0, "", Model!O22)))))</f>
         <v>h</v>
       </c>
-      <c r="AE8" s="124" t="s">
+      <c r="AE8" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="AF8" s="124"/>
+      <c r="AF8" s="140"/>
     </row>
     <row r="9" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="93" t="s">
@@ -3769,7 +3769,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="123" t="s">
+      <c r="B10" s="139" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="64" t="s">
@@ -3785,7 +3785,7 @@
       </c>
       <c r="F10" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="G10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3797,11 +3797,11 @@
       </c>
       <c r="I10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="J10" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="K10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3821,11 +3821,11 @@
       </c>
       <c r="O10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="P10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="Q10" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="R10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="S10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3845,11 +3845,11 @@
       </c>
       <c r="U10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="V10" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="W10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3869,11 +3869,11 @@
       </c>
       <c r="AA10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="AB10" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="AC10" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3888,7 +3888,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="123"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="64" t="s">
         <v>16</v>
       </c>
@@ -3910,11 +3910,11 @@
       </c>
       <c r="H11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="I11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="J11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="K11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="L11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3934,11 +3934,11 @@
       </c>
       <c r="N11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="O11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="P11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3958,11 +3958,11 @@
       </c>
       <c r="T11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="U11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="V11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3970,7 +3970,7 @@
       </c>
       <c r="W11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="X11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -3982,11 +3982,11 @@
       </c>
       <c r="Z11" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="AA11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="AB11" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4001,11 +4001,11 @@
       </c>
       <c r="AF11" s="115" t="b">
         <f>HLOOKUP(G$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="123"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="64" t="s">
         <v>15</v>
       </c>
@@ -4019,11 +4019,11 @@
       </c>
       <c r="F12" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="G12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="H12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4043,11 +4043,11 @@
       </c>
       <c r="L12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="M12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="N12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="O12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="P12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4067,11 +4067,11 @@
       </c>
       <c r="R12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="S12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="T12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4091,11 +4091,11 @@
       </c>
       <c r="X12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="Y12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="Z12" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4103,7 +4103,7 @@
       </c>
       <c r="AA12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="AB12" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4122,7 +4122,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="123"/>
+      <c r="B13" s="139"/>
       <c r="C13" s="64" t="s">
         <v>12</v>
       </c>
@@ -4132,11 +4132,11 @@
       </c>
       <c r="E13" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="F13" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="G13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4144,7 +4144,7 @@
       </c>
       <c r="H13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="I13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4156,11 +4156,11 @@
       </c>
       <c r="K13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="L13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="M13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4180,11 +4180,11 @@
       </c>
       <c r="Q13" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="R13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="S13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4192,7 +4192,7 @@
       </c>
       <c r="T13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="U13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4204,11 +4204,11 @@
       </c>
       <c r="W13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="X13" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="Y13" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4228,7 +4228,7 @@
       </c>
       <c r="AC13" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="AE13" s="89" t="s">
         <v>6</v>
@@ -4239,7 +4239,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="123"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="64" t="s">
         <v>14</v>
       </c>
@@ -4249,7 +4249,7 @@
       </c>
       <c r="E14" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="F14" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4269,11 +4269,11 @@
       </c>
       <c r="J14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="K14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="L14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="M14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="N14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4293,11 +4293,11 @@
       </c>
       <c r="P14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="Q14" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="R14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4317,11 +4317,11 @@
       </c>
       <c r="V14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="W14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="X14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4329,7 +4329,7 @@
       </c>
       <c r="Y14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="Z14" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4341,22 +4341,22 @@
       </c>
       <c r="AB14" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="AC14" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="AE14" s="89" t="s">
         <v>7</v>
       </c>
       <c r="AF14" s="115" t="b">
         <f>HLOOKUP(J$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="63" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="133" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="64" t="s">
@@ -4372,7 +4372,7 @@
       </c>
       <c r="F15" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="G15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4384,11 +4384,11 @@
       </c>
       <c r="I15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="J15" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="K15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4408,11 +4408,11 @@
       </c>
       <c r="O15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="P15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="Q15" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="R15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="S15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4432,11 +4432,11 @@
       </c>
       <c r="U15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>G♯ : ♯5</v>
+        <v/>
       </c>
       <c r="V15" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="W15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4456,11 +4456,11 @@
       </c>
       <c r="AA15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="AB15" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
-        <v>D♯ : ♯2</v>
+        <v/>
       </c>
       <c r="AC15" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$21, 2), "")</f>
@@ -4471,11 +4471,11 @@
       </c>
       <c r="AF15" s="115" t="b">
         <f>HLOOKUP(K$1, Model!$I$41:$O$57, MATCH($B$19, Model!$H$41:$H$57, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="128"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="64" t="s">
         <v>16</v>
       </c>
@@ -4497,11 +4497,11 @@
       </c>
       <c r="H16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+H$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="I16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+I$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D♯ : 2</v>
+        <v/>
       </c>
       <c r="J16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+J$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="K16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+K$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+K$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="L16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+L$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4521,11 +4521,11 @@
       </c>
       <c r="N16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+N$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>G♯ : 6</v>
+        <v/>
       </c>
       <c r="O16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+O$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="P16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+P$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4545,11 +4545,11 @@
       </c>
       <c r="T16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+T$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="U16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+U$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D♯ : 2</v>
+        <v/>
       </c>
       <c r="V16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+V$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="W16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+W$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+W$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="X16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+X$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4569,11 +4569,11 @@
       </c>
       <c r="Z16" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+Z$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>G♯ : 6</v>
+        <v/>
       </c>
       <c r="AA16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+AA$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="AB16" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D16+AB$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4587,7 +4587,7 @@
       <c r="AF16" s="116"/>
     </row>
     <row r="17" spans="2:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="128"/>
+      <c r="B17" s="133"/>
       <c r="C17" s="64" t="s">
         <v>32</v>
       </c>
@@ -4605,11 +4605,11 @@
       </c>
       <c r="G17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+G$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>G♯ : 6</v>
+        <v/>
       </c>
       <c r="H17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+H$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="I17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+I$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4629,11 +4629,11 @@
       </c>
       <c r="M17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+M$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="N17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+N$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D♯ : 2</v>
+        <v/>
       </c>
       <c r="O17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+O$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+O$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4641,7 +4641,7 @@
       </c>
       <c r="P17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+P$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+P$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="Q17" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Q$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+Q$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4653,11 +4653,11 @@
       </c>
       <c r="S17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+S$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>G♯ : 6</v>
+        <v/>
       </c>
       <c r="T17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+T$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="U17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+U$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4677,11 +4677,11 @@
       </c>
       <c r="Y17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+Y$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="Z17" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+Z$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D♯ : 2</v>
+        <v/>
       </c>
       <c r="AA17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AA$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+AA$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="AB17" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AB$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+AB$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="AC17" s="58" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AC$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D17+AC$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4699,7 +4699,7 @@
       <c r="AF17" s="116"/>
     </row>
     <row r="18" spans="2:32" s="63" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="128"/>
+      <c r="B18" s="133"/>
       <c r="C18" s="64" t="s">
         <v>30</v>
       </c>
@@ -4713,11 +4713,11 @@
       </c>
       <c r="F18" s="114" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+F$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+F$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="G18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+G$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+G$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D♯ : 2</v>
+        <v/>
       </c>
       <c r="H18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+H$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+H$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="I18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+I$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+I$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="J18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+J$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+J$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4737,11 +4737,11 @@
       </c>
       <c r="L18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+L$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+L$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>G♯ : 6</v>
+        <v/>
       </c>
       <c r="M18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+M$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+M$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="N18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+N$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+N$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4761,11 +4761,11 @@
       </c>
       <c r="R18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+R$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+R$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>D : 2</v>
       </c>
       <c r="S18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+S$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+S$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>D♯ : 2</v>
+        <v/>
       </c>
       <c r="T18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+T$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+T$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="U18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+U$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+U$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>F : 4</v>
       </c>
       <c r="V18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+V$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+V$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4785,11 +4785,11 @@
       </c>
       <c r="X18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+X$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+X$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v>G♯ : 6</v>
+        <v/>
       </c>
       <c r="Y18" s="56" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+Y$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+Y$9, 12), Model!$I$23:$O$23, 0), "")</f>
-        <v/>
+        <v>A : 6</v>
       </c>
       <c r="Z18" s="57" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+Z$9, 12), Model!$I$23:$O$23, 0), Model!$I$20:$O$29, 5) &amp; " : " &amp; MATCH(MOD($D18+Z$9, 12), Model!$I$23:$O$23, 0), "")</f>
@@ -4812,7 +4812,7 @@
     </row>
     <row r="19" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="67" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="C19" s="65"/>
       <c r="D19" s="1"/>
@@ -5010,50 +5010,50 @@
       <c r="AF22" s="60"/>
     </row>
     <row r="23" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="129" t="str">
+      <c r="B23" s="134" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(IF(B38 = "Ionian (Major)", B29 &amp; " Major", IF(B38 = "Aolian (Minor)", B29 &amp; " Minor", B29 &amp; " " &amp; B38)), "#", "♯"), "b", "♭")</f>
         <v>E Pentatonic Minor</v>
       </c>
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
-      <c r="G23" s="129"/>
-      <c r="K23" s="126">
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="134"/>
+      <c r="K23" s="129">
         <f>IF(J27 = "", "", IF(K24 = 0, F$1, K24))</f>
         <v>1</v>
       </c>
-      <c r="L23" s="126"/>
-      <c r="M23" s="126" t="str">
+      <c r="L23" s="129"/>
+      <c r="M23" s="129" t="str">
         <f>IF(K27 = "", "", IF(M24 = 0, G$1, M24))</f>
         <v/>
       </c>
-      <c r="N23" s="126"/>
-      <c r="O23" s="126" t="str">
+      <c r="N23" s="129"/>
+      <c r="O23" s="129" t="str">
         <f>IF(L27 = "", "", IF(O24 = 0, H$1, O24))</f>
         <v>♭3</v>
       </c>
-      <c r="P23" s="126"/>
-      <c r="Q23" s="126">
+      <c r="P23" s="129"/>
+      <c r="Q23" s="129">
         <f>IF(M27 = "", "", IF(Q24 = 0, I$1, Q24))</f>
         <v>4</v>
       </c>
-      <c r="R23" s="126"/>
-      <c r="S23" s="126">
+      <c r="R23" s="129"/>
+      <c r="S23" s="129">
         <f>IF(N27 = "", "", IF(S24 = 0, J$1, S24))</f>
         <v>5</v>
       </c>
-      <c r="T23" s="126"/>
-      <c r="U23" s="126" t="str">
+      <c r="T23" s="129"/>
+      <c r="U23" s="129" t="str">
         <f>IF(O27 = "", "", IF(U24 = 0, K$1, U24))</f>
         <v/>
       </c>
-      <c r="V23" s="126"/>
-      <c r="W23" s="126" t="str">
+      <c r="V23" s="129"/>
+      <c r="W23" s="129" t="str">
         <f>IF(P27 = "", "", IF(W24 = 0, L$1, W24))</f>
         <v>♭7</v>
       </c>
-      <c r="X23" s="126"/>
+      <c r="X23" s="129"/>
       <c r="Y23" s="60"/>
       <c r="Z23" s="60"/>
       <c r="AA23" s="60"/>
@@ -5064,47 +5064,47 @@
       <c r="AF23" s="60"/>
     </row>
     <row r="24" spans="2:32" s="59" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="129"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="129"/>
-      <c r="K24" s="132">
+      <c r="B24" s="134"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
+      <c r="K24" s="130">
         <f>IFERROR(HLOOKUP(F$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), F$1)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="132"/>
-      <c r="M24" s="132">
+      <c r="L24" s="130"/>
+      <c r="M24" s="130">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), G$1)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="132"/>
-      <c r="O24" s="132" t="str">
+      <c r="N24" s="130"/>
+      <c r="O24" s="130" t="str">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), H$1)</f>
         <v>♭3</v>
       </c>
-      <c r="P24" s="132"/>
-      <c r="Q24" s="132">
+      <c r="P24" s="130"/>
+      <c r="Q24" s="130">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), I$1)</f>
         <v>0</v>
       </c>
-      <c r="R24" s="132"/>
-      <c r="S24" s="132">
+      <c r="R24" s="130"/>
+      <c r="S24" s="130">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), J$1)</f>
         <v>0</v>
       </c>
-      <c r="T24" s="132"/>
-      <c r="U24" s="132">
+      <c r="T24" s="130"/>
+      <c r="U24" s="130">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), K$1)</f>
         <v>0</v>
       </c>
-      <c r="V24" s="132"/>
-      <c r="W24" s="132" t="str">
+      <c r="V24" s="130"/>
+      <c r="W24" s="130" t="str">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$1:$W$17, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), L$1)</f>
         <v>♭7</v>
       </c>
-      <c r="X24" s="132"/>
+      <c r="X24" s="130"/>
       <c r="Y24" s="60"/>
       <c r="Z24" s="60"/>
       <c r="AA24" s="60"/>
@@ -5115,47 +5115,47 @@
       <c r="AF24" s="60"/>
     </row>
     <row r="25" spans="2:32" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="129"/>
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="129"/>
-      <c r="G25" s="129"/>
-      <c r="K25" s="133" t="str">
+      <c r="B25" s="134"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="K25" s="128" t="str">
         <f>IF(K$23="","", J$27 &amp; IFERROR(HLOOKUP(F$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), F$1))</f>
         <v>Em7</v>
       </c>
-      <c r="L25" s="133"/>
-      <c r="M25" s="133" t="str">
+      <c r="L25" s="128"/>
+      <c r="M25" s="128" t="str">
         <f>IF(M$23="","", K$27 &amp; IFERROR(HLOOKUP(G$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), G$1))</f>
         <v/>
       </c>
-      <c r="N25" s="133"/>
-      <c r="O25" s="133" t="str">
+      <c r="N25" s="128"/>
+      <c r="O25" s="128" t="str">
         <f>IF(O$23="","", L$27 &amp; IFERROR(HLOOKUP(H$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), H$1))</f>
         <v>GM</v>
       </c>
-      <c r="P25" s="133"/>
-      <c r="Q25" s="133" t="str">
+      <c r="P25" s="128"/>
+      <c r="Q25" s="128" t="str">
         <f>IF(Q$23="","", M$27 &amp; IFERROR(HLOOKUP(I$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), I$1))</f>
         <v>A5 ♭7</v>
       </c>
-      <c r="R25" s="133"/>
-      <c r="S25" s="133" t="str">
+      <c r="R25" s="128"/>
+      <c r="S25" s="128" t="str">
         <f>IF(S$23="","", N$27 &amp; IFERROR(HLOOKUP(J$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), J$1))</f>
         <v>B5</v>
       </c>
-      <c r="T25" s="133"/>
-      <c r="U25" s="133" t="str">
+      <c r="T25" s="128"/>
+      <c r="U25" s="128" t="str">
         <f>IF(U$23="","", O$27 &amp; IFERROR(HLOOKUP(K$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), K$1))</f>
         <v/>
       </c>
-      <c r="V25" s="133"/>
-      <c r="W25" s="133" t="str">
+      <c r="V25" s="128"/>
+      <c r="W25" s="128" t="str">
         <f>IF(W$23="","", P$27 &amp; IFERROR(HLOOKUP(L$1, Model!$P$20:$W$36, MATCH($B$38, Model!$P$2:$P$20, 0) + 1), L$1))</f>
         <v>D5</v>
       </c>
-      <c r="X25" s="133"/>
+      <c r="X25" s="128"/>
       <c r="Y25" s="60"/>
       <c r="Z25" s="60"/>
       <c r="AA25" s="60"/>
@@ -5166,12 +5166,12 @@
       <c r="AF25" s="60"/>
     </row>
     <row r="26" spans="2:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="129"/>
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="129"/>
-      <c r="F26" s="129"/>
-      <c r="G26" s="129"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="134"/>
       <c r="H26" s="61"/>
       <c r="I26" s="61"/>
       <c r="J26" s="94"/>
@@ -5199,16 +5199,16 @@
       <c r="AF26" s="61"/>
     </row>
     <row r="27" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="129"/>
-      <c r="C27" s="129"/>
-      <c r="D27" s="129"/>
-      <c r="E27" s="129"/>
-      <c r="F27" s="129"/>
-      <c r="G27" s="129"/>
-      <c r="H27" s="130" t="s">
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="130"/>
+      <c r="I27" s="135"/>
       <c r="J27" s="73" t="str">
         <f>Model!I29</f>
         <v>E</v>
@@ -5237,11 +5237,11 @@
         <f>IF(Model!N29=0, "", Model!O29)</f>
         <v>D</v>
       </c>
-      <c r="S27" s="131" t="s">
+      <c r="S27" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="T27" s="131"/>
-      <c r="U27" s="131"/>
+      <c r="T27" s="136"/>
+      <c r="U27" s="136"/>
       <c r="V27" s="98" t="str">
         <f>IF(Model!I27=1, "h", IF(Model!I27=2, "W", IF(Model!I27=3, "W+h", IF(Model!I27=4, "WW", IF(Model!I27=0, "", Model!I22)))))</f>
         <v/>
@@ -5270,10 +5270,10 @@
         <f>IF(Model!O27=1, "h", IF(Model!O27=2, "W", IF(Model!O27=3, "W+h", IF(Model!O27=4, "WW", IF(Model!O27=0, "", Model!O22)))))</f>
         <v>W</v>
       </c>
-      <c r="AE27" s="124" t="s">
+      <c r="AE27" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="AF27" s="124"/>
+      <c r="AF27" s="140"/>
     </row>
     <row r="28" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="93" t="s">
@@ -5391,7 +5391,7 @@
       </c>
     </row>
     <row r="29" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="123" t="s">
+      <c r="B29" s="139" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="64" t="s">
@@ -5511,7 +5511,7 @@
       </c>
     </row>
     <row r="30" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="123"/>
+      <c r="B30" s="139"/>
       <c r="C30" s="64" t="s">
         <v>16</v>
       </c>
@@ -5629,7 +5629,7 @@
       </c>
     </row>
     <row r="31" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="123"/>
+      <c r="B31" s="139"/>
       <c r="C31" s="64" t="s">
         <v>15</v>
       </c>
@@ -5747,7 +5747,7 @@
       </c>
     </row>
     <row r="32" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="123"/>
+      <c r="B32" s="139"/>
       <c r="C32" s="64" t="s">
         <v>12</v>
       </c>
@@ -5865,7 +5865,7 @@
       </c>
     </row>
     <row r="33" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="123"/>
+      <c r="B33" s="139"/>
       <c r="C33" s="64" t="s">
         <v>14</v>
       </c>
@@ -5983,7 +5983,7 @@
       </c>
     </row>
     <row r="34" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="128" t="s">
+      <c r="B34" s="133" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="64" t="s">
@@ -6103,7 +6103,7 @@
       </c>
     </row>
     <row r="35" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="128"/>
+      <c r="B35" s="133"/>
       <c r="C35" s="64" t="s">
         <v>16</v>
       </c>
@@ -6216,7 +6216,7 @@
       <c r="AF35" s="116"/>
     </row>
     <row r="36" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="128"/>
+      <c r="B36" s="133"/>
       <c r="C36" s="64" t="s">
         <v>32</v>
       </c>
@@ -6329,7 +6329,7 @@
       <c r="AF36" s="116"/>
     </row>
     <row r="37" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="128"/>
+      <c r="B37" s="133"/>
       <c r="C37" s="64" t="s">
         <v>30</v>
       </c>
@@ -6588,30 +6588,22 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Z4:AA7"/>
+    <mergeCell ref="AB4:AC7"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AE27:AF27"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B23:G27"/>
     <mergeCell ref="H27:I27"/>
@@ -6628,22 +6620,30 @@
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Z4:AA7"/>
-    <mergeCell ref="AB4:AC7"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AE27:AF27"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U25:V25"/>
   </mergeCells>
   <conditionalFormatting sqref="AB4 AF10:AF19">
     <cfRule type="expression" dxfId="126" priority="548">
@@ -7151,10 +7151,10 @@
         <v>94</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="136" t="s">
+      <c r="F1" s="143" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="137"/>
+      <c r="G1" s="144"/>
       <c r="H1" s="107" t="s">
         <v>19</v>
       </c>
@@ -7430,10 +7430,10 @@
       <c r="D3" s="11">
         <v>10</v>
       </c>
-      <c r="F3" s="134" t="s">
+      <c r="F3" s="141" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="135"/>
+      <c r="G3" s="142"/>
       <c r="H3" s="14" t="s">
         <v>59</v>
       </c>
@@ -7563,7 +7563,7 @@
       </c>
       <c r="G4" s="9" t="str">
         <f>Fretboards!B19</f>
-        <v>Augmented</v>
+        <v>Ionian (Major)</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>171</v>
@@ -7678,10 +7678,10 @@
       <c r="D5" s="11">
         <v>8</v>
       </c>
-      <c r="F5" s="134" t="s">
+      <c r="F5" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="135"/>
+      <c r="G5" s="142"/>
       <c r="H5" s="14" t="s">
         <v>172</v>
       </c>
@@ -9367,9 +9367,9 @@
         <f>IF(VLOOKUP($G$4,$P$2:$W$17, 1+I20, FALSE) = 0, I20, VLOOKUP($G$4,$P$2:$W$17, 1+I20, FALSE))</f>
         <v>1</v>
       </c>
-      <c r="J21" s="9" t="str">
+      <c r="J21" s="9">
         <f t="shared" ref="J21:O21" si="0">IF(VLOOKUP($G$4,$P$2:$W$17, 1+J20, FALSE) = 0, J20, VLOOKUP($G$4,$P$2:$W$17, 1+J20, FALSE))</f>
-        <v>♯2</v>
+        <v>2</v>
       </c>
       <c r="K21" s="9">
         <f t="shared" si="0"/>
@@ -9383,9 +9383,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="N21" s="9" t="str">
+      <c r="N21" s="9">
         <f t="shared" si="0"/>
-        <v>♯5</v>
+        <v>6</v>
       </c>
       <c r="O21" s="9">
         <f t="shared" si="0"/>
@@ -9394,25 +9394,25 @@
       <c r="P21" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="Q21" s="139" t="s">
+      <c r="Q21" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="R21" s="139" t="s">
+      <c r="R21" s="122" t="s">
         <v>194</v>
       </c>
-      <c r="S21" s="139" t="s">
+      <c r="S21" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="T21" s="138" t="s">
+      <c r="T21" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="U21" s="138" t="s">
+      <c r="U21" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="V21" s="139" t="s">
+      <c r="V21" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="W21" s="140">
+      <c r="W21" s="123">
         <v>7</v>
       </c>
     </row>
@@ -9431,27 +9431,27 @@
       </c>
       <c r="I22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!I20 + 1, FALSE)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!J20 + 1, FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!K20 + 1, FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!L20 + 1, FALSE)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!M20 + 1, FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!N20 + 1, FALSE)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O22" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$2:$O$17,  Model!O20 + 1, FALSE)</f>
@@ -9460,23 +9460,23 @@
       <c r="P22" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="Q22" s="139" t="s">
+      <c r="Q22" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="R22" s="139"/>
-      <c r="S22" s="139" t="s">
+      <c r="R22" s="122"/>
+      <c r="S22" s="122" t="s">
         <v>182</v>
       </c>
-      <c r="T22" s="139" t="s">
+      <c r="T22" s="122" t="s">
         <v>189</v>
       </c>
-      <c r="U22" s="139" t="s">
+      <c r="U22" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="V22" s="139" t="s">
+      <c r="V22" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="W22" s="140" t="s">
+      <c r="W22" s="123" t="s">
         <v>183</v>
       </c>
     </row>
@@ -9499,15 +9499,15 @@
       </c>
       <c r="J23" s="9">
         <f t="shared" ref="J23:O23" si="1">IFERROR(VLOOKUP(SUBSTITUTE(SUBSTITUTE(J24, "♭", "b"), "♯","#"), $B$2:$D$41, 3, FALSE), "")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K23" s="9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L23" s="9" t="str">
+      <c r="L23" s="9">
         <f t="shared" si="1"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="M23" s="9">
         <f t="shared" si="1"/>
@@ -9515,7 +9515,7 @@
       </c>
       <c r="N23" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O23" s="9">
         <f t="shared" si="1"/>
@@ -9524,19 +9524,19 @@
       <c r="P23" s="103" t="s">
         <v>171</v>
       </c>
-      <c r="Q23" s="139" t="s">
+      <c r="Q23" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="R23" s="139"/>
-      <c r="S23" s="138" t="s">
+      <c r="R23" s="122"/>
+      <c r="S23" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="T23" s="138"/>
-      <c r="U23" s="138">
+      <c r="T23" s="121"/>
+      <c r="U23" s="121">
         <v>7</v>
       </c>
-      <c r="V23" s="138"/>
-      <c r="W23" s="141" t="s">
+      <c r="V23" s="121"/>
+      <c r="W23" s="124" t="s">
         <v>194</v>
       </c>
     </row>
@@ -9559,7 +9559,7 @@
       </c>
       <c r="J24" s="9" t="str">
         <f>IF(I22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(J21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:I22) + 1))</f>
-        <v>D♯</v>
+        <v>D</v>
       </c>
       <c r="K24" s="9" t="str">
         <f>IF(J22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(K21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:J22) + 1))</f>
@@ -9567,7 +9567,7 @@
       </c>
       <c r="L24" s="9" t="str">
         <f>IF(K22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(L21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:K22) + 1))</f>
-        <v/>
+        <v>F</v>
       </c>
       <c r="M24" s="9" t="str">
         <f>IF(L22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(M21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:L22) + 1))</f>
@@ -9575,7 +9575,7 @@
       </c>
       <c r="N24" s="9" t="str">
         <f>IF(M22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(N21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:M22) + 1))</f>
-        <v>G♯</v>
+        <v>A</v>
       </c>
       <c r="O24" s="9" t="str">
         <f>IF(N22=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$41, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(O21, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$41, 3, FALSE) + SUM($H$22:N22) + 1))</f>
@@ -9584,19 +9584,19 @@
       <c r="P24" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="Q24" s="139" t="s">
+      <c r="Q24" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="R24" s="139"/>
-      <c r="S24" s="139" t="s">
+      <c r="R24" s="122"/>
+      <c r="S24" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="T24" s="138"/>
-      <c r="U24" s="138" t="s">
+      <c r="T24" s="121"/>
+      <c r="U24" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="V24" s="139"/>
-      <c r="W24" s="140">
+      <c r="V24" s="122"/>
+      <c r="W24" s="123">
         <v>7</v>
       </c>
     </row>
@@ -9637,19 +9637,19 @@
       <c r="P25" s="103" t="s">
         <v>173</v>
       </c>
-      <c r="Q25" s="139" t="s">
+      <c r="Q25" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="R25" s="139"/>
-      <c r="S25" s="139" t="s">
+      <c r="R25" s="122"/>
+      <c r="S25" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="T25" s="139"/>
-      <c r="U25" s="139" t="s">
+      <c r="T25" s="122"/>
+      <c r="U25" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="V25" s="139"/>
-      <c r="W25" s="140" t="s">
+      <c r="V25" s="122"/>
+      <c r="W25" s="123" t="s">
         <v>186</v>
       </c>
     </row>
@@ -9697,23 +9697,23 @@
       <c r="P26" s="103" t="s">
         <v>197</v>
       </c>
-      <c r="Q26" s="138" t="s">
+      <c r="Q26" s="121" t="s">
         <v>203</v>
       </c>
-      <c r="R26" s="139" t="s">
+      <c r="R26" s="122" t="s">
         <v>201</v>
       </c>
-      <c r="S26" s="139" t="s">
+      <c r="S26" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="T26" s="138"/>
-      <c r="U26" s="138" t="s">
+      <c r="T26" s="121"/>
+      <c r="U26" s="121" t="s">
         <v>198</v>
       </c>
-      <c r="V26" s="138" t="s">
+      <c r="V26" s="121" t="s">
         <v>202</v>
       </c>
-      <c r="W26" s="141">
+      <c r="W26" s="124">
         <v>6</v>
       </c>
     </row>
@@ -9761,25 +9761,25 @@
       <c r="P27" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="Q27" s="139" t="s">
+      <c r="Q27" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="R27" s="139" t="s">
+      <c r="R27" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="S27" s="139" t="s">
+      <c r="S27" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="T27" s="138">
+      <c r="T27" s="121">
         <v>7</v>
       </c>
-      <c r="U27" s="138" t="s">
+      <c r="U27" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="V27" s="138" t="s">
+      <c r="V27" s="121" t="s">
         <v>194</v>
       </c>
-      <c r="W27" s="140" t="s">
+      <c r="W27" s="123" t="s">
         <v>184</v>
       </c>
     </row>
@@ -9827,25 +9827,25 @@
       <c r="P28" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="Q28" s="138" t="s">
+      <c r="Q28" s="121" t="s">
         <v>193</v>
       </c>
-      <c r="R28" s="139" t="s">
+      <c r="R28" s="122" t="s">
         <v>187</v>
       </c>
-      <c r="S28" s="139" t="s">
+      <c r="S28" s="122" t="s">
         <v>188</v>
       </c>
-      <c r="T28" s="139" t="s">
+      <c r="T28" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="U28" s="139">
+      <c r="U28" s="122">
         <v>7</v>
       </c>
-      <c r="V28" s="139" t="s">
+      <c r="V28" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="W28" s="140" t="s">
+      <c r="W28" s="123" t="s">
         <v>186</v>
       </c>
     </row>
@@ -9893,25 +9893,25 @@
       <c r="P29" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="Q29" s="139" t="s">
+      <c r="Q29" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="R29" s="139" t="s">
+      <c r="R29" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="S29" s="138" t="s">
+      <c r="S29" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="T29" s="138" t="s">
+      <c r="T29" s="121" t="s">
         <v>184</v>
       </c>
-      <c r="U29" s="138">
+      <c r="U29" s="121">
         <v>7</v>
       </c>
-      <c r="V29" s="138" t="s">
+      <c r="V29" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="W29" s="141" t="s">
+      <c r="W29" s="124" t="s">
         <v>194</v>
       </c>
     </row>
@@ -9928,25 +9928,25 @@
       <c r="P30" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="Q30" s="139" t="s">
+      <c r="Q30" s="122" t="s">
         <v>194</v>
       </c>
-      <c r="R30" s="139" t="s">
+      <c r="R30" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="S30" s="138" t="s">
+      <c r="S30" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="T30" s="138" t="s">
+      <c r="T30" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="U30" s="139" t="s">
+      <c r="U30" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="V30" s="139">
+      <c r="V30" s="122">
         <v>7</v>
       </c>
-      <c r="W30" s="140" t="s">
+      <c r="W30" s="123" t="s">
         <v>183</v>
       </c>
     </row>
@@ -9971,25 +9971,25 @@
       <c r="P31" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="Q31" s="139" t="s">
+      <c r="Q31" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="R31" s="138">
+      <c r="R31" s="121">
         <v>7</v>
       </c>
-      <c r="S31" s="138" t="s">
+      <c r="S31" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="T31" s="138" t="s">
+      <c r="T31" s="121" t="s">
         <v>194</v>
       </c>
-      <c r="U31" s="139" t="s">
+      <c r="U31" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="V31" s="139" t="s">
+      <c r="V31" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="W31" s="141" t="s">
+      <c r="W31" s="124" t="s">
         <v>183</v>
       </c>
     </row>
@@ -10007,25 +10007,25 @@
       <c r="P32" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="Q32" s="138" t="s">
+      <c r="Q32" s="121" t="s">
         <v>193</v>
       </c>
-      <c r="R32" s="138" t="s">
+      <c r="R32" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="S32" s="139" t="s">
+      <c r="S32" s="122" t="s">
         <v>190</v>
       </c>
-      <c r="T32" s="138">
+      <c r="T32" s="121">
         <v>7</v>
       </c>
-      <c r="U32" s="138">
+      <c r="U32" s="121">
         <v>7</v>
       </c>
-      <c r="V32" s="138" t="s">
+      <c r="V32" s="121" t="s">
         <v>187</v>
       </c>
-      <c r="W32" s="141" t="s">
+      <c r="W32" s="124" t="s">
         <v>187</v>
       </c>
     </row>
@@ -10043,25 +10043,25 @@
       <c r="P33" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="Q33" s="138">
+      <c r="Q33" s="121">
         <v>7</v>
       </c>
-      <c r="R33" s="138" t="s">
+      <c r="R33" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="S33" s="138" t="s">
+      <c r="S33" s="121" t="s">
         <v>194</v>
       </c>
-      <c r="T33" s="139" t="s">
+      <c r="T33" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="U33" s="139" t="s">
+      <c r="U33" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="V33" s="138" t="s">
+      <c r="V33" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="W33" s="140" t="s">
+      <c r="W33" s="123" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10079,23 +10079,23 @@
       <c r="P34" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="Q34" s="138" t="s">
+      <c r="Q34" s="121" t="s">
         <v>182</v>
       </c>
-      <c r="R34" s="138" t="s">
+      <c r="R34" s="121" t="s">
         <v>185</v>
       </c>
-      <c r="S34" s="138" t="s">
+      <c r="S34" s="121" t="s">
         <v>191</v>
       </c>
-      <c r="T34" s="139"/>
-      <c r="U34" s="139">
+      <c r="T34" s="122"/>
+      <c r="U34" s="122">
         <v>5</v>
       </c>
-      <c r="V34" s="138" t="s">
+      <c r="V34" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="W34" s="140"/>
+      <c r="W34" s="123"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B35" s="9" t="s">
@@ -10111,21 +10111,21 @@
       <c r="P35" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="Q35" s="138" t="s">
+      <c r="Q35" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="R35" s="139"/>
-      <c r="S35" s="139" t="s">
+      <c r="R35" s="122"/>
+      <c r="S35" s="122" t="s">
         <v>182</v>
       </c>
-      <c r="T35" s="138" t="s">
+      <c r="T35" s="121" t="s">
         <v>192</v>
       </c>
-      <c r="U35" s="139">
+      <c r="U35" s="122">
         <v>5</v>
       </c>
-      <c r="V35" s="139"/>
-      <c r="W35" s="140">
+      <c r="V35" s="122"/>
+      <c r="W35" s="123">
         <v>5</v>
       </c>
     </row>
@@ -10143,25 +10143,25 @@
       <c r="P36" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="Q36" s="142" t="s">
+      <c r="Q36" s="125" t="s">
         <v>183</v>
       </c>
-      <c r="R36" s="142" t="s">
+      <c r="R36" s="125" t="s">
         <v>184</v>
       </c>
-      <c r="S36" s="143">
+      <c r="S36" s="126">
         <v>7</v>
       </c>
-      <c r="T36" s="143" t="s">
+      <c r="T36" s="126" t="s">
         <v>183</v>
       </c>
-      <c r="U36" s="143" t="s">
+      <c r="U36" s="126" t="s">
         <v>194</v>
       </c>
-      <c r="V36" s="142" t="s">
+      <c r="V36" s="125" t="s">
         <v>184</v>
       </c>
-      <c r="W36" s="144" t="s">
+      <c r="W36" s="127" t="s">
         <v>183</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed long standing bug with scale degree naming on the spreadsheet.
Scale degree names somehow had a terrible implementation that I'd not
noticed until recently.  It was perfect on the model page, but on the
ACTUAL fretboard, it was incorrect over 80% of the time there was an
accidental.  Whew, sorry.
</commit_message>
<xml_diff>
--- a/Shredsheets.xlsx
+++ b/Shredsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Shredsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72078827-D8E2-4BEE-8FEF-4F33265D6CA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEFB8D9-C5D6-45D6-8566-18C326242B35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1440" windowWidth="26970" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24810" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fretboards" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <definedName name="ReversedNotes">{"C","B","A#","A","G#","G","F#","F","E","D#","D","C#","C","B","A#","A","G#","G","F#","F","E","D#","D","C#","C"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1831,43 +1832,43 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3287,7 +3288,7 @@
   <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -3419,160 +3420,160 @@
       <c r="A4" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="136" t="str">
+      <c r="B4" s="138" t="str">
         <f>IF(B19 = "Ionian (Major)", B10 &amp; " Major", IF(B19 = "Aolian (Minor)", B10 &amp; " Minor", B10 &amp; " " &amp; B19))</f>
-        <v>C Major</v>
-      </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="K4" s="131">
-        <f>IF(J8 = "", "", IF(K5 = 0, F$1, K5))</f>
-        <v>1</v>
-      </c>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131">
-        <f>IF(K8 = "", "", IF(M5 = 0, G$1, M5))</f>
-        <v>2</v>
-      </c>
-      <c r="N4" s="131"/>
-      <c r="O4" s="131">
-        <f>IF(L8 = "", "", IF(O5 = 0, H$1, O5))</f>
-        <v>3</v>
-      </c>
-      <c r="P4" s="131"/>
-      <c r="Q4" s="131">
-        <f>IF(M8 = "", "", IF(Q5 = 0, I$1, Q5))</f>
+        <v>C Locrian</v>
+      </c>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="K4" s="135">
+        <f>IF(Model!I3="0","",Model!I3)</f>
+        <v>1</v>
+      </c>
+      <c r="L4" s="135"/>
+      <c r="M4" s="135" t="str">
+        <f>IF(Model!J3="0","",Model!J3)</f>
+        <v>♭2</v>
+      </c>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135" t="str">
+        <f>IF(Model!K3="0","",Model!K3)</f>
+        <v>♭3</v>
+      </c>
+      <c r="P4" s="135"/>
+      <c r="Q4" s="135">
+        <f>IF(Model!L3="0","",Model!L3)</f>
         <v>4</v>
       </c>
-      <c r="R4" s="131"/>
-      <c r="S4" s="131">
-        <f>IF(N8 = "", "", IF(S5 = 0, J$1, S5))</f>
-        <v>5</v>
-      </c>
-      <c r="T4" s="131"/>
-      <c r="U4" s="131">
-        <f>IF(O8 = "", "", IF(U5 = 0, K$1, U5))</f>
-        <v>6</v>
-      </c>
-      <c r="V4" s="131"/>
-      <c r="W4" s="131">
-        <f>IF(P8 = "", "", IF(W5 = 0, L$1, W5))</f>
-        <v>7</v>
-      </c>
-      <c r="X4" s="131"/>
-      <c r="Z4" s="139" t="s">
+      <c r="R4" s="135"/>
+      <c r="S4" s="135" t="str">
+        <f>IF(Model!M3="0","",Model!M3)</f>
+        <v>♭5</v>
+      </c>
+      <c r="T4" s="135"/>
+      <c r="U4" s="135" t="str">
+        <f>IF(Model!N3="0","",Model!N3)</f>
+        <v>♭6</v>
+      </c>
+      <c r="V4" s="135"/>
+      <c r="W4" s="135" t="str">
+        <f>IF(Model!O3="0","",Model!O3)</f>
+        <v>♭7</v>
+      </c>
+      <c r="X4" s="135"/>
+      <c r="Z4" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="AA4" s="139"/>
-      <c r="AB4" s="140" t="b">
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="131" t="b">
         <v>0</v>
       </c>
-      <c r="AC4" s="140"/>
+      <c r="AC4" s="131"/>
     </row>
     <row r="5" spans="1:32" s="50" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="K5" s="133">
-        <f>IFERROR(HLOOKUP(F$1, Model!$P$18:$W$41, MATCH($B$19, Model!$P$24:$P$43, 0) + 1), F$1)</f>
-        <v>1</v>
-      </c>
-      <c r="L5" s="133"/>
-      <c r="M5" s="133">
+      <c r="B5" s="138"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="138"/>
+      <c r="K5" s="135">
+        <f>Model!I4</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="135"/>
+      <c r="M5" s="136">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$18:$W$41, MATCH($B$19, Model!$P$24:$P$43, 0) + 1), G$1)</f>
-        <v>2</v>
-      </c>
-      <c r="N5" s="133"/>
-      <c r="O5" s="133">
+        <v>0</v>
+      </c>
+      <c r="N5" s="136"/>
+      <c r="O5" s="136" t="str">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$18:$W$41, MATCH($B$19, Model!$P$24:$P$43, 0) + 1), H$1)</f>
-        <v>3</v>
-      </c>
-      <c r="P5" s="133"/>
-      <c r="Q5" s="133">
+        <v>♭3</v>
+      </c>
+      <c r="P5" s="136"/>
+      <c r="Q5" s="136">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$18:$W$41, MATCH($B$19, Model!$P$24:$P$43, 0) + 1), I$1)</f>
-        <v>4</v>
-      </c>
-      <c r="R5" s="133"/>
-      <c r="S5" s="133">
+        <v>0</v>
+      </c>
+      <c r="R5" s="136"/>
+      <c r="S5" s="136">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$18:$W$41, MATCH($B$19, Model!$P$24:$P$43, 0) + 1), J$1)</f>
-        <v>5</v>
-      </c>
-      <c r="T5" s="133"/>
-      <c r="U5" s="133">
+        <v>0</v>
+      </c>
+      <c r="T5" s="136"/>
+      <c r="U5" s="136">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$18:$W$41, MATCH($B$19, Model!$P$24:$P$43, 0) + 1), K$1)</f>
-        <v>6</v>
-      </c>
-      <c r="V5" s="133"/>
-      <c r="W5" s="133">
+        <v>0</v>
+      </c>
+      <c r="V5" s="136"/>
+      <c r="W5" s="136" t="str">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$18:$W$41, MATCH($B$19, Model!$P$24:$P$43, 0) + 1), L$1)</f>
-        <v>7</v>
-      </c>
-      <c r="X5" s="133"/>
-      <c r="Z5" s="139"/>
-      <c r="AA5" s="139"/>
-      <c r="AB5" s="140"/>
-      <c r="AC5" s="140"/>
+        <v>♭7</v>
+      </c>
+      <c r="X5" s="136"/>
+      <c r="Z5" s="130"/>
+      <c r="AA5" s="130"/>
+      <c r="AB5" s="131"/>
+      <c r="AC5" s="131"/>
     </row>
     <row r="6" spans="1:32" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
+      <c r="G6" s="138"/>
       <c r="K6" s="134" t="str">
         <f>IF(K$4="","", J$8 &amp; IFERROR(HLOOKUP(F$1, Model!$P$43:$W$65, MATCH($B$19, Model!$P$44:$P$65, 0) + 1), F$1))</f>
-        <v>CM7</v>
+        <v>Cm7ø</v>
       </c>
       <c r="L6" s="134"/>
       <c r="M6" s="134" t="str">
         <f>IF(M$4="","", K$8 &amp; IFERROR(HLOOKUP(G$1, Model!$P$43:$W$65, MATCH($B$19, Model!$P$44:$P$65, 0) + 1), G$1))</f>
-        <v>Dm7</v>
+        <v>D♭M7</v>
       </c>
       <c r="N6" s="134"/>
       <c r="O6" s="134" t="str">
         <f>IF(O$4="","", L$8 &amp; IFERROR(HLOOKUP(H$1, Model!$P$43:$W$65, MATCH($B$19, Model!$P$44:$P$65, 0) + 1), H$1))</f>
-        <v>Em7</v>
+        <v>E♭m7</v>
       </c>
       <c r="P6" s="134"/>
       <c r="Q6" s="134" t="str">
         <f>IF(Q$4="","", M$8 &amp; IFERROR(HLOOKUP(I$1, Model!$P$43:$W$65, MATCH($B$19, Model!$P$44:$P$65, 0) + 1), I$1))</f>
-        <v>FM7</v>
+        <v>Fm7</v>
       </c>
       <c r="R6" s="134"/>
       <c r="S6" s="134" t="str">
         <f>IF(S$4="","", N$8 &amp; IFERROR(HLOOKUP(J$1, Model!$P$43:$W$65, MATCH($B$19, Model!$P$44:$P$65, 0) + 1), J$1))</f>
-        <v>G7</v>
+        <v>G♭M7</v>
       </c>
       <c r="T6" s="134"/>
       <c r="U6" s="134" t="str">
         <f>IF(U$4="","", O$8 &amp; IFERROR(HLOOKUP(K$1, Model!$P$43:$W$65, MATCH($B$19, Model!$P$44:$P$65, 0) + 1), K$1))</f>
-        <v>Am7</v>
+        <v>A♭7</v>
       </c>
       <c r="V6" s="134"/>
       <c r="W6" s="134" t="str">
         <f>IF(W$4="","", P$8 &amp; IFERROR(HLOOKUP(L$1, Model!$P$43:$W$65, MATCH($B$19, Model!$P$44:$P$65, 0) + 1), L$1))</f>
-        <v>Bm7ø</v>
+        <v>B♭m7</v>
       </c>
       <c r="X6" s="134"/>
-      <c r="Z6" s="139"/>
-      <c r="AA6" s="139"/>
-      <c r="AB6" s="140"/>
-      <c r="AC6" s="140"/>
+      <c r="Z6" s="130"/>
+      <c r="AA6" s="130"/>
+      <c r="AB6" s="131"/>
+      <c r="AC6" s="131"/>
     </row>
     <row r="7" spans="1:32" s="51" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="136"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
       <c r="J7" s="85"/>
       <c r="K7" s="85"/>
       <c r="L7" s="85"/>
@@ -3580,33 +3581,33 @@
       <c r="N7" s="85"/>
       <c r="O7" s="85"/>
       <c r="P7" s="85"/>
-      <c r="Z7" s="139"/>
-      <c r="AA7" s="139"/>
-      <c r="AB7" s="140"/>
-      <c r="AC7" s="140"/>
+      <c r="Z7" s="130"/>
+      <c r="AA7" s="130"/>
+      <c r="AB7" s="131"/>
+      <c r="AC7" s="131"/>
     </row>
     <row r="8" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="137" t="s">
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="137"/>
+      <c r="I8" s="139"/>
       <c r="J8" s="63" t="str">
         <f>Model!I6</f>
         <v>C</v>
       </c>
       <c r="K8" s="64" t="str">
         <f>IF(Model!I4=0, "", Model!J6)</f>
-        <v>D</v>
+        <v>D♭</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>IF(Model!J4=0, "", Model!K6)</f>
-        <v>E</v>
+        <v>E♭</v>
       </c>
       <c r="M8" s="66" t="str">
         <f>IF(Model!K4=0, "", Model!L6)</f>
@@ -3614,24 +3615,24 @@
       </c>
       <c r="N8" s="67" t="str">
         <f>IF(Model!L4=0, "", Model!M6)</f>
-        <v>G</v>
+        <v>G♭</v>
       </c>
       <c r="O8" s="68" t="str">
         <f>IF(Model!M4=0, "", Model!N6)</f>
-        <v>A</v>
+        <v>A♭</v>
       </c>
       <c r="P8" s="69" t="str">
         <f>IF(Model!N4=0, "", Model!O6)</f>
-        <v>B</v>
-      </c>
-      <c r="S8" s="138" t="s">
+        <v>B♭</v>
+      </c>
+      <c r="S8" s="140" t="s">
         <v>18</v>
       </c>
-      <c r="T8" s="138"/>
-      <c r="U8" s="138"/>
+      <c r="T8" s="140"/>
+      <c r="U8" s="140"/>
       <c r="V8" s="88" t="str">
         <f>IF(Model!I4=1, "h", IF(Model!I4=2, "W", IF(Model!I4=3, "W+h", IF(Model!I4=4, "WW", IF(Model!I4=0, "", Model!I4)))))</f>
-        <v>W</v>
+        <v>h</v>
       </c>
       <c r="W8" s="70" t="str">
         <f>IF(Model!J4=1, "h", IF(Model!J4=2, "W", IF(Model!J4=3, "W+h", IF(Model!J4=4, "WW", IF(Model!J4=0, "", Model!J4)))))</f>
@@ -3639,11 +3640,11 @@
       </c>
       <c r="X8" s="71" t="str">
         <f>IF(Model!K4=1, "h", IF(Model!K4=2, "W", IF(Model!K4=3, "W+h", IF(Model!K4=4, "WW", IF(Model!K4=0, "", Model!K4)))))</f>
-        <v>h</v>
+        <v>W</v>
       </c>
       <c r="Y8" s="72" t="str">
         <f>IF(Model!L4=1, "h", IF(Model!L4=2, "W", IF(Model!L4=3, "W+h",IF(Model!L4=4, "WW", IF(Model!L4=0, "", Model!L4)))))</f>
-        <v>W</v>
+        <v>h</v>
       </c>
       <c r="Z8" s="73" t="str">
         <f>IF(Model!M4=1, "h", IF(Model!M4=2, "W", IF(Model!M4=3, "W+h",IF(Model!M4=4, "WW", IF(Model!M4=0, "", Model!M4)))))</f>
@@ -3655,12 +3656,12 @@
       </c>
       <c r="AB8" s="75" t="str">
         <f>IF(Model!O4=1, "h", IF(Model!O4=2, "W", IF(Model!O4=3, "W+h",IF(Model!O4=4, "WW", IF(Model!O4=0, "", Model!O4)))))</f>
-        <v>h</v>
-      </c>
-      <c r="AE8" s="142" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="142"/>
+        <v>W</v>
+      </c>
+      <c r="AE8" s="133" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="133"/>
     </row>
     <row r="9" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="83" t="s">
@@ -3778,7 +3779,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="141" t="s">
+      <c r="B10" s="132" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="54" t="s">
@@ -3790,7 +3791,7 @@
       </c>
       <c r="E10" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="F10" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3798,27 +3799,27 @@
       </c>
       <c r="G10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="H10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="I10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="J10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="K10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="L10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="M10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3826,19 +3827,19 @@
       </c>
       <c r="N10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="O10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="P10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="Q10" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="R10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3846,27 +3847,27 @@
       </c>
       <c r="S10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="T10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="U10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="V10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="W10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="X10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="Y10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3874,19 +3875,19 @@
       </c>
       <c r="Z10" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="AA10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="AB10" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="AC10" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="AE10" s="78" t="s">
         <v>2</v>
@@ -3897,7 +3898,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="141"/>
+      <c r="B11" s="132"/>
       <c r="C11" s="54" t="s">
         <v>15</v>
       </c>
@@ -3907,7 +3908,7 @@
       </c>
       <c r="E11" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="F11" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3915,19 +3916,19 @@
       </c>
       <c r="G11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="H11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="I11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="J11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="K11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3935,27 +3936,27 @@
       </c>
       <c r="L11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="M11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="N11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="O11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="P11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="Q11" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="R11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3963,19 +3964,19 @@
       </c>
       <c r="S11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="T11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="U11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="V11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="W11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -3983,38 +3984,38 @@
       </c>
       <c r="X11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="Y11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="Z11" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="AA11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="AB11" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="AC11" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="AE11" s="79" t="s">
         <v>3</v>
       </c>
       <c r="AF11" s="92" t="b">
         <f>HLOOKUP(G$1, Model!$I$43:$O$65, MATCH($B$19, Model!$H$43:$H$65, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:32" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="141"/>
+      <c r="B12" s="132"/>
       <c r="C12" s="54" t="s">
         <v>14</v>
       </c>
@@ -4024,23 +4025,23 @@
       </c>
       <c r="E12" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="F12" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="G12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="H12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="I12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="J12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4048,19 +4049,19 @@
       </c>
       <c r="K12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="L12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="M12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="N12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="O12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4068,27 +4069,27 @@
       </c>
       <c r="P12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="Q12" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="R12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="S12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="T12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="U12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="V12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4096,19 +4097,19 @@
       </c>
       <c r="W12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="X12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="Y12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="Z12" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="AA12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4116,11 +4117,11 @@
       </c>
       <c r="AB12" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="AC12" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="AE12" s="79" t="s">
         <v>4</v>
@@ -4131,7 +4132,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="141"/>
+      <c r="B13" s="132"/>
       <c r="C13" s="54" t="s">
         <v>11</v>
       </c>
@@ -4141,15 +4142,15 @@
       </c>
       <c r="E13" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="F13" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="G13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="H13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4157,27 +4158,27 @@
       </c>
       <c r="I13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="J13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="K13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="L13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="M13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="N13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="O13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4185,19 +4186,19 @@
       </c>
       <c r="P13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="Q13" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="R13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="S13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="T13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4205,27 +4206,27 @@
       </c>
       <c r="U13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="V13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="W13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="X13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="Y13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="Z13" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="AA13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4233,11 +4234,11 @@
       </c>
       <c r="AB13" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="AC13" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="AE13" s="79" t="s">
         <v>5</v>
@@ -4248,7 +4249,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="141"/>
+      <c r="B14" s="132"/>
       <c r="C14" s="54" t="s">
         <v>13</v>
       </c>
@@ -4258,15 +4259,15 @@
       </c>
       <c r="E14" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="F14" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="G14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="H14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4274,19 +4275,19 @@
       </c>
       <c r="I14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="J14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="K14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="L14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="M14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4294,27 +4295,27 @@
       </c>
       <c r="N14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="O14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="P14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="Q14" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="R14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="S14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="T14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4322,19 +4323,19 @@
       </c>
       <c r="U14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="V14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="W14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="X14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="Y14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4342,30 +4343,30 @@
       </c>
       <c r="Z14" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="AA14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="AB14" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="AC14" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="AE14" s="79" t="s">
         <v>6</v>
       </c>
       <c r="AF14" s="92" t="b">
         <f>HLOOKUP(J$1, Model!$I$43:$O$65, MATCH($B$19, Model!$H$43:$H$65, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="137" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="54" t="s">
@@ -4377,7 +4378,7 @@
       </c>
       <c r="E15" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="F15" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4385,27 +4386,27 @@
       </c>
       <c r="G15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="H15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="I15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="J15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="K15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="L15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="M15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4413,19 +4414,19 @@
       </c>
       <c r="N15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="O15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="P15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="Q15" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="R15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4433,27 +4434,27 @@
       </c>
       <c r="S15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="T15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="U15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="V15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="W15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="X15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="Y15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4461,30 +4462,30 @@
       </c>
       <c r="Z15" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="AA15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="AB15" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="AC15" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="AE15" s="79" t="s">
         <v>7</v>
       </c>
       <c r="AF15" s="92" t="b">
         <f>HLOOKUP(K$1, Model!$I$43:$O$65, MATCH($B$19, Model!$H$43:$H$65, 0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:32" s="53" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="135"/>
+      <c r="B16" s="137"/>
       <c r="C16" s="54" t="s">
         <v>15</v>
       </c>
@@ -4494,7 +4495,7 @@
       </c>
       <c r="E16" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="F16" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4502,19 +4503,19 @@
       </c>
       <c r="G16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="H16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="I16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="J16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="K16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4522,27 +4523,27 @@
       </c>
       <c r="L16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="M16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="N16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="O16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="P16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="Q16" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="R16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4550,19 +4551,19 @@
       </c>
       <c r="S16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="T16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="U16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="V16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="W16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4570,33 +4571,33 @@
       </c>
       <c r="X16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="Y16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="Z16" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="AA16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="AB16" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="AC16" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="AE16" s="80"/>
       <c r="AF16" s="93"/>
     </row>
     <row r="17" spans="2:32" s="53" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="135"/>
+      <c r="B17" s="137"/>
       <c r="C17" s="54" t="s">
         <v>66</v>
       </c>
@@ -4606,27 +4607,27 @@
       </c>
       <c r="E17" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="F17" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="G17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="H17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="I17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="J17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="K17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4634,19 +4635,19 @@
       </c>
       <c r="L17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="M17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="N17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="O17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="P17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4654,27 +4655,27 @@
       </c>
       <c r="Q17" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="R17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="S17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="T17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="U17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="V17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="W17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4682,19 +4683,19 @@
       </c>
       <c r="X17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="Y17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="Z17" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="AA17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="AB17" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4702,13 +4703,13 @@
       </c>
       <c r="AC17" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D17+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D17+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="AE17" s="81"/>
       <c r="AF17" s="93"/>
     </row>
     <row r="18" spans="2:32" s="53" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="135"/>
+      <c r="B18" s="137"/>
       <c r="C18" s="54" t="s">
         <v>60</v>
       </c>
@@ -4718,19 +4719,19 @@
       </c>
       <c r="E18" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+E$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="F18" s="91" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+F$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="G18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+G$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="H18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+H$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="I18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+I$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4738,27 +4739,27 @@
       </c>
       <c r="J18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+J$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="K18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+K$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="L18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+L$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="M18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+M$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="N18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+N$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="O18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+O$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="P18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+P$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4766,19 +4767,19 @@
       </c>
       <c r="Q18" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+Q$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="R18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+R$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>D : 2</v>
+        <v/>
       </c>
       <c r="S18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+S$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>E♭ : ♭3</v>
       </c>
       <c r="T18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+T$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>E : 3</v>
+        <v/>
       </c>
       <c r="U18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+U$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4786,27 +4787,27 @@
       </c>
       <c r="V18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+V$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>G♭ : ♭5</v>
       </c>
       <c r="W18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+W$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>G : 5</v>
+        <v/>
       </c>
       <c r="X18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+X$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>A♭ : ♭6</v>
       </c>
       <c r="Y18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+Y$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>A : 6</v>
+        <v/>
       </c>
       <c r="Z18" s="47" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+Z$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>B♭ : ♭7</v>
       </c>
       <c r="AA18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+AA$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v>B : 7</v>
+        <v/>
       </c>
       <c r="AB18" s="46" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+AB$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
@@ -4814,14 +4815,14 @@
       </c>
       <c r="AC18" s="48" t="str">
         <f>IFERROR(HLOOKUP(MATCH(MOD($D18+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D18+AC$9, 12), Model!$I$5:$O$5, 0), Model!$I$2:$O$3, 2), "")</f>
-        <v/>
+        <v>D♭ : ♭2</v>
       </c>
       <c r="AE18" s="82"/>
       <c r="AF18" s="93"/>
     </row>
     <row r="19" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="57" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="C19" s="55"/>
       <c r="D19" s="1"/>
@@ -5007,62 +5008,61 @@
     <row r="22" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="56"/>
       <c r="E22" s="60"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="Y22" s="50"/>
-      <c r="Z22" s="50"/>
-      <c r="AA22" s="50"/>
-      <c r="AB22" s="50"/>
-      <c r="AC22" s="50"/>
-      <c r="AD22" s="50"/>
-      <c r="AE22" s="62"/>
-      <c r="AF22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="62"/>
+      <c r="R22" s="50"/>
+      <c r="AE22" s="52"/>
     </row>
     <row r="23" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="136" t="str">
+      <c r="B23" s="138" t="str">
         <f>IF(B38 = "Ionian (Major)", B29 &amp; " Major", IF(B38 = "Aolian (Minor)", B29 &amp; " Minor", B29 &amp; " " &amp; B38))</f>
         <v>C Pentatonic Minor</v>
       </c>
-      <c r="C23" s="136"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="136"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="136"/>
-      <c r="K23" s="131">
-        <f>IF(J27 = "", "", IF(K24 = 0, F$1, K24))</f>
-        <v>1</v>
-      </c>
-      <c r="L23" s="131"/>
-      <c r="M23" s="131" t="str">
-        <f>IF(K27 = "", "", IF(M24 = 0, G$1, M24))</f>
-        <v/>
-      </c>
-      <c r="N23" s="131"/>
-      <c r="O23" s="131">
-        <f>IF(L27 = "", "", IF(O24 = 0, H$1, O24))</f>
-        <v>3</v>
-      </c>
-      <c r="P23" s="131"/>
-      <c r="Q23" s="131" t="str">
-        <f>IF(M27 = "", "", IF(Q24 = 0, I$1, Q24))</f>
-        <v>♯4</v>
-      </c>
-      <c r="R23" s="131"/>
-      <c r="S23" s="131">
-        <f>IF(N27 = "", "", IF(S24 = 0, J$1, S24))</f>
+      <c r="C23" s="138"/>
+      <c r="D23" s="138"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="138"/>
+      <c r="G23" s="138"/>
+      <c r="K23" s="135">
+        <f>IF(Model!I10="0","",Model!I10)</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="135"/>
+      <c r="M23" s="135" t="str">
+        <f>IF(Model!J10="0","",Model!J10)</f>
+        <v/>
+      </c>
+      <c r="N23" s="135"/>
+      <c r="O23" s="135" t="str">
+        <f>IF(Model!K10="0","",Model!K10)</f>
+        <v>♭3</v>
+      </c>
+      <c r="P23" s="135"/>
+      <c r="Q23" s="135">
+        <f>IF(Model!L10="0","",Model!L10)</f>
+        <v>4</v>
+      </c>
+      <c r="R23" s="135"/>
+      <c r="S23" s="135">
+        <f>IF(Model!M10="0","",Model!M10)</f>
         <v>5</v>
       </c>
-      <c r="T23" s="131"/>
-      <c r="U23" s="131" t="str">
-        <f>IF(O27 = "", "", IF(U24 = 0, K$1, U24))</f>
-        <v/>
-      </c>
-      <c r="V23" s="131"/>
-      <c r="W23" s="131">
-        <f>IF(P27 = "", "", IF(W24 = 0, L$1, W24))</f>
-        <v>7</v>
-      </c>
-      <c r="X23" s="131"/>
+      <c r="T23" s="135"/>
+      <c r="U23" s="135" t="str">
+        <f>IF(Model!N10="0","",Model!N10)</f>
+        <v/>
+      </c>
+      <c r="V23" s="135"/>
+      <c r="W23" s="135" t="str">
+        <f>IF(Model!O10="0","",Model!O10)</f>
+        <v>♭7</v>
+      </c>
+      <c r="X23" s="135"/>
       <c r="Y23" s="50"/>
       <c r="Z23" s="50"/>
       <c r="AA23" s="50"/>
@@ -5073,47 +5073,47 @@
       <c r="AF23" s="50"/>
     </row>
     <row r="24" spans="2:32" s="49" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="136"/>
-      <c r="C24" s="136"/>
-      <c r="D24" s="136"/>
-      <c r="E24" s="136"/>
-      <c r="F24" s="136"/>
-      <c r="G24" s="136"/>
-      <c r="K24" s="132">
+      <c r="B24" s="138"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="K24" s="141">
         <f>IFERROR(HLOOKUP(F$1, Model!$P$18:$W$41, MATCH($B$38, Model!$P$24:$P$43, 0) + 1), F$1)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="132"/>
-      <c r="M24" s="132">
+      <c r="L24" s="141"/>
+      <c r="M24" s="141">
         <f>IFERROR(HLOOKUP(G$1, Model!$P$18:$W$41, MATCH($B$38, Model!$P$24:$P$43, 0) + 1), G$1)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="132"/>
-      <c r="O24" s="132">
+      <c r="N24" s="141"/>
+      <c r="O24" s="141">
         <f>IFERROR(HLOOKUP(H$1, Model!$P$18:$W$41, MATCH($B$38, Model!$P$24:$P$43, 0) + 1), H$1)</f>
         <v>0</v>
       </c>
-      <c r="P24" s="132"/>
-      <c r="Q24" s="132" t="str">
+      <c r="P24" s="141"/>
+      <c r="Q24" s="141" t="str">
         <f>IFERROR(HLOOKUP(I$1, Model!$P$18:$W$41, MATCH($B$38, Model!$P$24:$P$43, 0) + 1), I$1)</f>
         <v>♯4</v>
       </c>
-      <c r="R24" s="132"/>
-      <c r="S24" s="132">
+      <c r="R24" s="141"/>
+      <c r="S24" s="141">
         <f>IFERROR(HLOOKUP(J$1, Model!$P$18:$W$41, MATCH($B$38, Model!$P$24:$P$43, 0) + 1), J$1)</f>
         <v>0</v>
       </c>
-      <c r="T24" s="132"/>
-      <c r="U24" s="132">
+      <c r="T24" s="141"/>
+      <c r="U24" s="141">
         <f>IFERROR(HLOOKUP(K$1, Model!$P$18:$W$41, MATCH($B$38, Model!$P$24:$P$43, 0) + 1), K$1)</f>
         <v>0</v>
       </c>
-      <c r="V24" s="132"/>
-      <c r="W24" s="132">
+      <c r="V24" s="141"/>
+      <c r="W24" s="141">
         <f>IFERROR(HLOOKUP(L$1, Model!$P$18:$W$41, MATCH($B$38, Model!$P$24:$P$43, 0) + 1), L$1)</f>
         <v>0</v>
       </c>
-      <c r="X24" s="132"/>
+      <c r="X24" s="141"/>
       <c r="Y24" s="50"/>
       <c r="Z24" s="50"/>
       <c r="AA24" s="50"/>
@@ -5124,47 +5124,47 @@
       <c r="AF24" s="50"/>
     </row>
     <row r="25" spans="2:32" s="49" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="136"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="136"/>
-      <c r="E25" s="136"/>
-      <c r="F25" s="136"/>
-      <c r="G25" s="136"/>
-      <c r="K25" s="130" t="str">
+      <c r="B25" s="138"/>
+      <c r="C25" s="138"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="138"/>
+      <c r="K25" s="142" t="str">
         <f>IF(K$23="","", J$27 &amp; IFERROR(HLOOKUP(F$1, Model!$P$43:$W$65, MATCH($B$38, Model!$P$44:$P$65, 0) + 1), F$1))</f>
         <v>Cm7</v>
       </c>
-      <c r="L25" s="130"/>
-      <c r="M25" s="130" t="str">
+      <c r="L25" s="142"/>
+      <c r="M25" s="142" t="str">
         <f>IF(M$23="","", K$27 &amp; IFERROR(HLOOKUP(G$1, Model!$P$43:$W$65, MATCH($B$38, Model!$P$44:$P$65, 0) + 1), G$1))</f>
         <v/>
       </c>
-      <c r="N25" s="130"/>
-      <c r="O25" s="130" t="str">
+      <c r="N25" s="142"/>
+      <c r="O25" s="142" t="str">
         <f>IF(O$23="","", L$27 &amp; IFERROR(HLOOKUP(H$1, Model!$P$43:$W$65, MATCH($B$38, Model!$P$44:$P$65, 0) + 1), H$1))</f>
         <v>E♭M</v>
       </c>
-      <c r="P25" s="130"/>
-      <c r="Q25" s="130" t="str">
+      <c r="P25" s="142"/>
+      <c r="Q25" s="142" t="str">
         <f>IF(Q$23="","", M$27 &amp; IFERROR(HLOOKUP(I$1, Model!$P$43:$W$65, MATCH($B$38, Model!$P$44:$P$65, 0) + 1), I$1))</f>
         <v>F5 ♭7</v>
       </c>
-      <c r="R25" s="130"/>
-      <c r="S25" s="130" t="str">
+      <c r="R25" s="142"/>
+      <c r="S25" s="142" t="str">
         <f>IF(S$23="","", N$27 &amp; IFERROR(HLOOKUP(J$1, Model!$P$43:$W$65, MATCH($B$38, Model!$P$44:$P$65, 0) + 1), J$1))</f>
         <v>G♭3 ♭7</v>
       </c>
-      <c r="T25" s="130"/>
-      <c r="U25" s="130" t="str">
+      <c r="T25" s="142"/>
+      <c r="U25" s="142" t="str">
         <f>IF(U$23="","", O$27 &amp; IFERROR(HLOOKUP(K$1, Model!$P$43:$W$65, MATCH($B$38, Model!$P$44:$P$65, 0) + 1), K$1))</f>
         <v/>
       </c>
-      <c r="V25" s="130"/>
-      <c r="W25" s="130" t="str">
+      <c r="V25" s="142"/>
+      <c r="W25" s="142" t="str">
         <f>IF(W$23="","", P$27 &amp; IFERROR(HLOOKUP(L$1, Model!$P$43:$W$65, MATCH($B$38, Model!$P$44:$P$65, 0) + 1), L$1))</f>
         <v>B♭5</v>
       </c>
-      <c r="X25" s="130"/>
+      <c r="X25" s="142"/>
       <c r="Y25" s="50"/>
       <c r="Z25" s="50"/>
       <c r="AA25" s="50"/>
@@ -5175,12 +5175,12 @@
       <c r="AF25" s="50"/>
     </row>
     <row r="26" spans="2:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="136"/>
-      <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
-      <c r="E26" s="136"/>
-      <c r="F26" s="136"/>
-      <c r="G26" s="136"/>
+      <c r="B26" s="138"/>
+      <c r="C26" s="138"/>
+      <c r="D26" s="138"/>
+      <c r="E26" s="138"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="138"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
       <c r="J26" s="84"/>
@@ -5208,16 +5208,16 @@
       <c r="AF26" s="51"/>
     </row>
     <row r="27" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="136"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="136"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="136"/>
-      <c r="G27" s="136"/>
-      <c r="H27" s="137" t="s">
+      <c r="B27" s="138"/>
+      <c r="C27" s="138"/>
+      <c r="D27" s="138"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="138"/>
+      <c r="G27" s="138"/>
+      <c r="H27" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="137"/>
+      <c r="I27" s="139"/>
       <c r="J27" s="63" t="str">
         <f>Model!I13</f>
         <v>C</v>
@@ -5246,11 +5246,11 @@
         <f>IF(Model!N13=0, "", Model!O13)</f>
         <v>B♭</v>
       </c>
-      <c r="S27" s="138" t="s">
+      <c r="S27" s="140" t="s">
         <v>18</v>
       </c>
-      <c r="T27" s="138"/>
-      <c r="U27" s="138"/>
+      <c r="T27" s="140"/>
+      <c r="U27" s="140"/>
       <c r="V27" s="88" t="str">
         <f>IF(Model!I11=1, "h", IF(Model!I11=2, "W", IF(Model!I11=3, "W+h", IF(Model!I11=4, "WW", IF(Model!I11=0, "", Model!I4)))))</f>
         <v/>
@@ -5279,10 +5279,10 @@
         <f>IF(Model!O11=1, "h", IF(Model!O11=2, "W", IF(Model!O11=3, "W+h", IF(Model!O11=4, "WW", IF(Model!O11=0, "", Model!O4)))))</f>
         <v>W</v>
       </c>
-      <c r="AE27" s="142" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF27" s="142"/>
+      <c r="AE27" s="133" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="133"/>
     </row>
     <row r="28" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="83" t="s">
@@ -5400,7 +5400,7 @@
       </c>
     </row>
     <row r="29" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="141" t="s">
+      <c r="B29" s="132" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="54" t="s">
@@ -5520,7 +5520,7 @@
       </c>
     </row>
     <row r="30" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="141"/>
+      <c r="B30" s="132"/>
       <c r="C30" s="54" t="s">
         <v>15</v>
       </c>
@@ -5638,7 +5638,7 @@
       </c>
     </row>
     <row r="31" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="141"/>
+      <c r="B31" s="132"/>
       <c r="C31" s="54" t="s">
         <v>14</v>
       </c>
@@ -5756,7 +5756,7 @@
       </c>
     </row>
     <row r="32" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="141"/>
+      <c r="B32" s="132"/>
       <c r="C32" s="54" t="s">
         <v>11</v>
       </c>
@@ -5874,7 +5874,7 @@
       </c>
     </row>
     <row r="33" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="141"/>
+      <c r="B33" s="132"/>
       <c r="C33" s="54" t="s">
         <v>13</v>
       </c>
@@ -5992,7 +5992,7 @@
       </c>
     </row>
     <row r="34" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="135" t="s">
+      <c r="B34" s="137" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="54" t="s">
@@ -6112,7 +6112,7 @@
       </c>
     </row>
     <row r="35" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="135"/>
+      <c r="B35" s="137"/>
       <c r="C35" s="54" t="s">
         <v>15</v>
       </c>
@@ -6225,7 +6225,7 @@
       <c r="AF35" s="93"/>
     </row>
     <row r="36" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="135"/>
+      <c r="B36" s="137"/>
       <c r="C36" s="54" t="s">
         <v>66</v>
       </c>
@@ -6338,7 +6338,7 @@
       <c r="AF36" s="93"/>
     </row>
     <row r="37" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="135"/>
+      <c r="B37" s="137"/>
       <c r="C37" s="54" t="s">
         <v>60</v>
       </c>
@@ -6597,6 +6597,46 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B23:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B4:G8"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
     <mergeCell ref="Z4:AA7"/>
     <mergeCell ref="AB4:AC7"/>
     <mergeCell ref="B10:B14"/>
@@ -6613,46 +6653,6 @@
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="U5:V5"/>
     <mergeCell ref="U6:V6"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B23:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B4:G8"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U25:V25"/>
   </mergeCells>
   <conditionalFormatting sqref="AB4 AF10:AF19">
     <cfRule type="expression" dxfId="126" priority="548">
@@ -7097,7 +7097,7 @@
       <formula>AND($AF$19, SEARCH("7", E10))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB4" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -7106,7 +7106,7 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Model!$A$2:$A$23</xm:f>
@@ -7130,8 +7130,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BN68"/>
   <sheetViews>
-    <sheetView topLeftCell="E22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -7424,29 +7424,29 @@
         <f>IF(VLOOKUP($G$4,$P$19:$W$40, 1+I2, FALSE) = 0, I2, VLOOKUP($G$4,$P$19:$W$40, 1+I2, FALSE))</f>
         <v>1</v>
       </c>
-      <c r="J3" s="9">
-        <f t="shared" ref="J3:O3" si="0">IF(VLOOKUP($G$4,$P$19:$W$40, 1+J2, FALSE) = 0, J2, VLOOKUP($G$4,$P$19:$W$40, 1+J2, FALSE))</f>
-        <v>2</v>
-      </c>
-      <c r="K3" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+      <c r="J3" s="9" t="str">
+        <f>IF(I4=0,"",IF(VLOOKUP($G$4,$P$19:$W$40,1+J2,FALSE)=0,J2,VLOOKUP($G$4,$P$19:$W$40,1+J2,FALSE)))</f>
+        <v>♭2</v>
+      </c>
+      <c r="K3" s="9" t="str">
+        <f t="shared" ref="K3:O3" si="0">IF(J4=0,"",IF(VLOOKUP($G$4,$P$19:$W$40,1+K2,FALSE)=0,K2,VLOOKUP($G$4,$P$19:$W$40,1+K2,FALSE)))</f>
+        <v>♭3</v>
       </c>
       <c r="L3" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N3" s="9">
+        <v>♭5</v>
+      </c>
+      <c r="N3" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="O3" s="105">
+        <v>♭6</v>
+      </c>
+      <c r="O3" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>♭7</v>
       </c>
       <c r="X3" s="100">
         <v>2</v>
@@ -7533,14 +7533,14 @@
       </c>
       <c r="G4" s="9" t="str">
         <f>Fretboards!B19</f>
-        <v>Ionian (Major)</v>
+        <v>Locrian</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$19:$O$40,  Model!I2 + 1, FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$19:$O$40,  Model!J2 + 1, FALSE)</f>
@@ -7548,11 +7548,11 @@
       </c>
       <c r="K4" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$19:$O$40,  Model!K2 + 1, FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$19:$O$40,  Model!L2 + 1, FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="9">
         <f>VLOOKUP(Model!$G$4, Model!$H$19:$O$40,  Model!M2 + 1, FALSE)</f>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="O4" s="105">
         <f>VLOOKUP(Model!$G$4, Model!$H$19:$O$40,  Model!O2 + 1, FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X4" s="100">
         <v>3</v>
@@ -7658,11 +7658,11 @@
       </c>
       <c r="J5" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" si="1"/>
@@ -7670,15 +7670,15 @@
       </c>
       <c r="M5" s="9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N5" s="9">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O5" s="105">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X5" s="100">
         <v>4</v>
@@ -7774,11 +7774,11 @@
       </c>
       <c r="J6" s="21" t="str">
         <f>IF(I4=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$34, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(J3, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$34, 3, FALSE) + SUM($H$4:I4) + 1))</f>
-        <v>D</v>
+        <v>D♭</v>
       </c>
       <c r="K6" s="21" t="str">
         <f>IF(J4=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$34, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(K3, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$34, 3, FALSE) + SUM($H$4:J4) + 1))</f>
-        <v>E</v>
+        <v>E♭</v>
       </c>
       <c r="L6" s="21" t="str">
         <f>IF(K4=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$34, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(L3, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$34, 3, FALSE) + SUM($H$4:K4) + 1))</f>
@@ -7786,15 +7786,15 @@
       </c>
       <c r="M6" s="21" t="str">
         <f>IF(L4=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$34, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(M3, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$34, 3, FALSE) + SUM($H$4:L4) + 1))</f>
-        <v>G</v>
+        <v>G♭</v>
       </c>
       <c r="N6" s="21" t="str">
         <f>IF(M4=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$34, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(N3, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$34, 3, FALSE) + SUM($H$4:M4) + 1))</f>
-        <v>A</v>
+        <v>A♭</v>
       </c>
       <c r="O6" s="107" t="str">
         <f>IF(N4=0, "", INDEX($Y$2:$AX$15,VLOOKUP($F$4, $B$2:$D$34, 2, FALSE) + SUBSTITUTE(SUBSTITUTE(O3, "♯", ""),"♭","") - 1, VLOOKUP($F$4, $B$2:$D$34, 3, FALSE) + SUM($H$4:N4) + 1))</f>
-        <v>B</v>
+        <v>B♭</v>
       </c>
       <c r="X6" s="100">
         <v>5</v>
@@ -8205,12 +8205,12 @@
         <f>IF(VLOOKUP($G$6,$P$19:$W$40, 1+I2, FALSE) = 0, I2, VLOOKUP($G$6,$P$19:$W$40, 1+I2, FALSE))</f>
         <v>1</v>
       </c>
-      <c r="J10" s="9">
-        <f t="shared" ref="J10:O10" si="2">IF(VLOOKUP($G$6,$P$19:$W$40, 1+J2, FALSE) = 0, J2, VLOOKUP($G$6,$P$19:$W$40, 1+J2, FALSE))</f>
-        <v>2</v>
+      <c r="J10" s="9" t="str">
+        <f>IF(I11=0,"",IF(VLOOKUP($G$6,$P$19:$W$40,1+J2,FALSE)=0,J2,VLOOKUP($G$6,$P$19:$W$40,1+J2,FALSE)))</f>
+        <v/>
       </c>
       <c r="K10" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K10:O10" si="2">IF(J11=0,"",IF(VLOOKUP($G$6,$P$19:$W$40,1+K2,FALSE)=0,K2,VLOOKUP($G$6,$P$19:$W$40,1+K2,FALSE)))</f>
         <v>♭3</v>
       </c>
       <c r="L10" s="9">
@@ -8221,11 +8221,11 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="O10" s="105" t="str">
+        <v/>
+      </c>
+      <c r="O10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>♭7</v>
       </c>
@@ -11270,7 +11270,7 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:O1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I44:O65" xr:uid="{9E77CF2C-8DC6-4DA2-8C23-71D2EAF5B912}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Fixed coloring errors of the notes within the upper scale
</commit_message>
<xml_diff>
--- a/Shredsheets.xlsx
+++ b/Shredsheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Shredsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79F7A23-C88D-4B6D-AB6F-76F1AAF6433D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F011CBE9-CBB2-4D5C-9C62-3B4C2850D788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2164,6 +2164,33 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2188,18 +2215,21 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2222,43 +2252,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="238">
+  <dxfs count="126">
     <dxf>
       <font>
         <color theme="0" tint="-4.9989318521683403E-2"/>
@@ -2271,23 +2271,13 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <color theme="0" tint="-4.9989318521683403E-2"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF813997"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2297,7 +2287,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFB567F5"/>
+          <bgColor rgb="FF8CC068"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2307,7 +2297,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
+          <bgColor rgb="FF81B2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2317,7 +2307,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
+          <bgColor rgb="FFC6E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2325,11 +2315,21 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="0"/>
+        <color theme="1" tint="0.14996795556505021"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF3788CB"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2705,7 +2705,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF2992D9"/>
+        <color rgb="FF3788CB"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -2715,17 +2715,17 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC07DE2"/>
+        <color rgb="FFE4D2F2"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF70C3FC"/>
+        <color rgb="FFF4DA3E"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFB7EE00"/>
+        <color rgb="FFB567F5"/>
       </font>
     </dxf>
     <dxf>
@@ -2735,13 +2735,161 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFA63AB8"/>
+        <color rgb="FF642C76"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FFFF66FF"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF813997"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8CFF19"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB567F5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4DA3E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3788CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8CC068"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF81B2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1" tint="0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3117,1026 +3265,20 @@
         <i val="0"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF813997"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CC068"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81B2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF642C76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CFF19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB567F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4DA3E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3788CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CC068"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81B2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF2992D9"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC07DE2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF70C3FC"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB7EE00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF63D218"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFA63AB8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF3788CB"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD3B5E9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF4DA3E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB567F5"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF75E604"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF642C76"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF66FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF372F2D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CC068"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81B2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8CC068"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81B2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3788CB"/>
+      <color rgb="FF642C76"/>
+      <color rgb="FFE4D2F2"/>
+      <color rgb="FFF4DA3E"/>
+      <color rgb="FFB567F5"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FFA63AB8"/>
       <color rgb="FF63D218"/>
       <color rgb="FFB7EE00"/>
       <color rgb="FF70C3FC"/>
-      <color rgb="FFC07DE2"/>
-      <color rgb="FF2992D9"/>
-      <color rgb="FF75F00F"/>
-      <color rgb="FFC07DF7"/>
-      <color rgb="FFB567F5"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4453,7 +3595,7 @@
   <dimension ref="A1:AF38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="AF18" sqref="AF18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4549,113 +3691,113 @@
       <c r="A3" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="163" t="str">
+      <c r="B3" s="172" t="str">
         <f>IF(B17 = "Ionian (Major)", B8 &amp; " Major", IF(B17 = "Aolian (Minor)", B8 &amp; " Minor", B8 &amp; " " &amp; B17))</f>
         <v>E Pentatonic Minor</v>
       </c>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="K3" s="162">
+      <c r="C3" s="172"/>
+      <c r="D3" s="172"/>
+      <c r="E3" s="172"/>
+      <c r="F3" s="172"/>
+      <c r="G3" s="172"/>
+      <c r="K3" s="171">
         <f>IF(Model!J3="0","",Model!J3)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="162"/>
-      <c r="M3" s="162" t="str">
+      <c r="L3" s="171"/>
+      <c r="M3" s="171" t="str">
         <f>IF(Model!K3="0","",Model!K3)</f>
         <v/>
       </c>
-      <c r="N3" s="162"/>
-      <c r="O3" s="162" t="str">
+      <c r="N3" s="171"/>
+      <c r="O3" s="171" t="str">
         <f>IF(Model!L3="0","",Model!L3)</f>
         <v>♭3</v>
       </c>
-      <c r="P3" s="162"/>
-      <c r="Q3" s="162">
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171">
         <f>IF(Model!M3="0","",Model!M3)</f>
         <v>4</v>
       </c>
-      <c r="R3" s="162"/>
-      <c r="S3" s="162">
+      <c r="R3" s="171"/>
+      <c r="S3" s="171">
         <f>IF(Model!N3="0","",Model!N3)</f>
         <v>5</v>
       </c>
-      <c r="T3" s="162"/>
-      <c r="U3" s="162" t="str">
+      <c r="T3" s="171"/>
+      <c r="U3" s="171" t="str">
         <f>IF(Model!O3="0","",Model!O3)</f>
         <v/>
       </c>
-      <c r="V3" s="162"/>
-      <c r="W3" s="162" t="str">
+      <c r="V3" s="171"/>
+      <c r="W3" s="171" t="str">
         <f>IF(Model!P3="0","",Model!P3)</f>
         <v>♭7</v>
       </c>
-      <c r="X3" s="162"/>
-      <c r="Z3" s="158" t="s">
+      <c r="X3" s="171"/>
+      <c r="Z3" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" s="158"/>
-      <c r="AB3" s="159" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="159"/>
+      <c r="AA3" s="167"/>
+      <c r="AB3" s="168" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="168"/>
     </row>
     <row r="4" spans="1:32" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="K4" s="161" t="str">
+      <c r="B4" s="172"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="K4" s="170" t="str">
         <f>Model!J7</f>
         <v>Em7</v>
       </c>
-      <c r="L4" s="161"/>
-      <c r="M4" s="161" t="str">
+      <c r="L4" s="170"/>
+      <c r="M4" s="170" t="str">
         <f>Model!K7</f>
         <v/>
       </c>
-      <c r="N4" s="161"/>
-      <c r="O4" s="161" t="str">
+      <c r="N4" s="170"/>
+      <c r="O4" s="170" t="str">
         <f>Model!L7</f>
         <v>GM</v>
       </c>
-      <c r="P4" s="161"/>
-      <c r="Q4" s="161" t="str">
+      <c r="P4" s="170"/>
+      <c r="Q4" s="170" t="str">
         <f>Model!M7</f>
         <v>A5 ♭7</v>
       </c>
-      <c r="R4" s="161"/>
-      <c r="S4" s="161" t="str">
+      <c r="R4" s="170"/>
+      <c r="S4" s="170" t="str">
         <f>Model!N7</f>
         <v>B♭3 ♭7</v>
       </c>
-      <c r="T4" s="161"/>
-      <c r="U4" s="161" t="str">
+      <c r="T4" s="170"/>
+      <c r="U4" s="170" t="str">
         <f>Model!O7</f>
         <v/>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161" t="str">
+      <c r="V4" s="170"/>
+      <c r="W4" s="170" t="str">
         <f>Model!P7</f>
         <v>D5</v>
       </c>
-      <c r="X4" s="161"/>
-      <c r="Z4" s="158"/>
-      <c r="AA4" s="158"/>
-      <c r="AB4" s="159"/>
-      <c r="AC4" s="159"/>
+      <c r="X4" s="170"/>
+      <c r="Z4" s="167"/>
+      <c r="AA4" s="167"/>
+      <c r="AB4" s="168"/>
+      <c r="AC4" s="168"/>
     </row>
     <row r="5" spans="1:32" s="49" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="163"/>
+      <c r="B5" s="172"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="172"/>
       <c r="J5" s="74"/>
       <c r="K5" s="58"/>
       <c r="L5" s="74"/>
@@ -4663,22 +3805,22 @@
       <c r="N5" s="74"/>
       <c r="O5" s="74"/>
       <c r="P5" s="74"/>
-      <c r="Z5" s="158"/>
-      <c r="AA5" s="158"/>
-      <c r="AB5" s="159"/>
-      <c r="AC5" s="159"/>
+      <c r="Z5" s="167"/>
+      <c r="AA5" s="167"/>
+      <c r="AB5" s="168"/>
+      <c r="AC5" s="168"/>
     </row>
     <row r="6" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="163"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="164" t="s">
+      <c r="B6" s="172"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="172"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="172"/>
+      <c r="H6" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="164"/>
+      <c r="I6" s="173"/>
       <c r="J6" s="57" t="str">
         <f>IF(Model!J6=0,"", Model!J6)</f>
         <v>E</v>
@@ -4707,11 +3849,11 @@
         <f>IF(Model!P6=0,"", Model!P6)</f>
         <v>D</v>
       </c>
-      <c r="S6" s="165" t="s">
+      <c r="S6" s="174" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="165"/>
-      <c r="U6" s="165"/>
+      <c r="T6" s="174"/>
+      <c r="U6" s="174"/>
       <c r="V6" s="75" t="str">
         <f>IF(Model!J4=1, "h", IF(Model!J4=2, "W", IF(Model!J4=3, "W+h", IF(Model!J4=4, "WW", IF(Model!J4=0, "", Model!J4)))))</f>
         <v/>
@@ -4740,10 +3882,10 @@
         <f>IF(Model!P4=1, "h", IF(Model!P4=2, "W", IF(Model!P4=3, "W+h",IF(Model!P4=4, "WW", IF(Model!P4=0, "", Model!P4)))))</f>
         <v>W</v>
       </c>
-      <c r="AE6" s="178" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="178"/>
+      <c r="AE6" s="175" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="175"/>
     </row>
     <row r="7" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="72" t="s">
@@ -4853,15 +3995,15 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AE7" s="179" t="s">
+      <c r="AE7" s="158" t="s">
         <v>207</v>
       </c>
-      <c r="AF7" s="180" t="s">
+      <c r="AF7" s="159" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="51" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="169" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="52" t="s">
@@ -4971,15 +4113,15 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D8+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D8+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v>E : 1</v>
       </c>
-      <c r="AE8" s="181" t="s">
+      <c r="AE8" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="AF8" s="182" t="b">
+      <c r="AF8" s="161" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:32" s="51" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="160"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="52" t="s">
         <v>14</v>
       </c>
@@ -5087,15 +4229,15 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D9+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D9+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v>B : 5</v>
       </c>
-      <c r="AE9" s="183" t="s">
+      <c r="AE9" s="162" t="s">
         <v>3</v>
       </c>
-      <c r="AF9" s="182" t="b">
+      <c r="AF9" s="161" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="51" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="160"/>
+      <c r="B10" s="169"/>
       <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
@@ -5203,15 +4345,15 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D10+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D10+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v>G : ♭3</v>
       </c>
-      <c r="AE10" s="183" t="s">
+      <c r="AE10" s="162" t="s">
         <v>4</v>
       </c>
-      <c r="AF10" s="182" t="b">
-        <v>1</v>
+      <c r="AF10" s="161" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="51" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="160"/>
+      <c r="B11" s="169"/>
       <c r="C11" s="52" t="s">
         <v>10</v>
       </c>
@@ -5319,15 +4461,15 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D11+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D11+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v>D : ♭7</v>
       </c>
-      <c r="AE11" s="183" t="s">
+      <c r="AE11" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="AF11" s="182" t="b">
+      <c r="AF11" s="161" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:32" s="51" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="160"/>
+      <c r="B12" s="169"/>
       <c r="C12" s="52" t="s">
         <v>12</v>
       </c>
@@ -5435,15 +4577,15 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D12+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D12+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v>A : 4</v>
       </c>
-      <c r="AE12" s="183" t="s">
+      <c r="AE12" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="AF12" s="182" t="b">
+      <c r="AF12" s="161" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:32" s="51" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="179" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="52" t="s">
@@ -5553,15 +4695,15 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D13+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D13+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v>E : 1</v>
       </c>
-      <c r="AE13" s="183" t="s">
+      <c r="AE13" s="162" t="s">
         <v>7</v>
       </c>
-      <c r="AF13" s="182" t="b">
+      <c r="AF13" s="161" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:32" s="51" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="166"/>
+      <c r="B14" s="179"/>
       <c r="C14" s="52" t="s">
         <v>14</v>
       </c>
@@ -5669,11 +4811,11 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D14+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D14+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v>B : 5</v>
       </c>
-      <c r="AE14" s="184"/>
-      <c r="AF14" s="185"/>
+      <c r="AE14" s="163"/>
+      <c r="AF14" s="164"/>
     </row>
     <row r="15" spans="1:32" s="51" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="166"/>
+      <c r="B15" s="179"/>
       <c r="C15" s="52" t="s">
         <v>57</v>
       </c>
@@ -5781,11 +4923,11 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D15+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D15+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v/>
       </c>
-      <c r="AE15" s="186"/>
-      <c r="AF15" s="185"/>
+      <c r="AE15" s="165"/>
+      <c r="AF15" s="164"/>
     </row>
     <row r="16" spans="1:32" s="51" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="166"/>
+      <c r="B16" s="179"/>
       <c r="C16" s="52" t="s">
         <v>51</v>
       </c>
@@ -5893,8 +5035,8 @@
         <f>IFERROR(HLOOKUP(MATCH(MOD($D16+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$6, 5) &amp; " : " &amp; HLOOKUP(MATCH(MOD($D16+AC$7, 12), Model!$J$5:$P$5, 0), Model!$J$2:$P$3, 2), "")</f>
         <v/>
       </c>
-      <c r="AE16" s="187"/>
-      <c r="AF16" s="185"/>
+      <c r="AE16" s="166"/>
+      <c r="AF16" s="164"/>
     </row>
     <row r="17" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="55" t="s">
@@ -6002,10 +5144,10 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AE17" s="181" t="s">
+      <c r="AE17" s="160" t="s">
         <v>8</v>
       </c>
-      <c r="AF17" s="182" t="b">
+      <c r="AF17" s="161" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6061,50 +5203,50 @@
       <c r="AC19" s="114"/>
     </row>
     <row r="20" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="163" t="str">
+      <c r="B20" s="172" t="str">
         <f>IF(B34 = "Ionian (Major)", B25 &amp; " Major", IF(B34 = "Aolian (Minor)", B25 &amp; " Minor", B25 &amp; " " &amp; B34))</f>
         <v>E Aeolian (Minor)</v>
       </c>
-      <c r="C20" s="163"/>
-      <c r="D20" s="163"/>
-      <c r="E20" s="163"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="163"/>
-      <c r="K20" s="162">
+      <c r="C20" s="172"/>
+      <c r="D20" s="172"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="172"/>
+      <c r="G20" s="172"/>
+      <c r="K20" s="171">
         <f>IF(Model!J12="0","",Model!J12)</f>
         <v>1</v>
       </c>
-      <c r="L20" s="162"/>
-      <c r="M20" s="162">
+      <c r="L20" s="171"/>
+      <c r="M20" s="171">
         <f>IF(Model!K12="0","",Model!K12)</f>
         <v>2</v>
       </c>
-      <c r="N20" s="162"/>
-      <c r="O20" s="162" t="str">
+      <c r="N20" s="171"/>
+      <c r="O20" s="171" t="str">
         <f>IF(Model!L12="0","",Model!L12)</f>
         <v>♭3</v>
       </c>
-      <c r="P20" s="162"/>
-      <c r="Q20" s="162">
+      <c r="P20" s="171"/>
+      <c r="Q20" s="171">
         <f>IF(Model!M12="0","",Model!M12)</f>
         <v>4</v>
       </c>
-      <c r="R20" s="162"/>
-      <c r="S20" s="162">
+      <c r="R20" s="171"/>
+      <c r="S20" s="171">
         <f>IF(Model!N12="0","",Model!N12)</f>
         <v>5</v>
       </c>
-      <c r="T20" s="162"/>
-      <c r="U20" s="162" t="str">
+      <c r="T20" s="171"/>
+      <c r="U20" s="171" t="str">
         <f>IF(Model!O12="0","",Model!O12)</f>
         <v>♭6</v>
       </c>
-      <c r="V20" s="162"/>
-      <c r="W20" s="162" t="str">
+      <c r="V20" s="171"/>
+      <c r="W20" s="171" t="str">
         <f>IF(Model!P12="0","",Model!P12)</f>
         <v>♭7</v>
       </c>
-      <c r="X20" s="162"/>
+      <c r="X20" s="171"/>
       <c r="Y20" s="48"/>
       <c r="Z20" s="48"/>
       <c r="AA20" s="48"/>
@@ -6113,53 +5255,53 @@
       <c r="AD20" s="48"/>
     </row>
     <row r="21" spans="2:32" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="163"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="163"/>
-      <c r="E21" s="163"/>
-      <c r="F21" s="163"/>
-      <c r="G21" s="163"/>
-      <c r="K21" s="169" t="str">
+      <c r="B21" s="172"/>
+      <c r="C21" s="172"/>
+      <c r="D21" s="172"/>
+      <c r="E21" s="172"/>
+      <c r="F21" s="172"/>
+      <c r="G21" s="172"/>
+      <c r="K21" s="178" t="str">
         <f>Model!J$16</f>
         <v>Em7</v>
       </c>
-      <c r="L21" s="169" t="str">
+      <c r="L21" s="178" t="str">
         <f>Model!K$16</f>
         <v>F♯m7ø</v>
       </c>
-      <c r="M21" s="169" t="str">
+      <c r="M21" s="178" t="str">
         <f>Model!K$16</f>
         <v>F♯m7ø</v>
       </c>
-      <c r="N21" s="169" t="str">
+      <c r="N21" s="178" t="str">
         <f>Model!M$16</f>
         <v>Am7</v>
       </c>
-      <c r="O21" s="169" t="str">
+      <c r="O21" s="178" t="str">
         <f>Model!L$16</f>
         <v>GM7</v>
       </c>
-      <c r="P21" s="169"/>
-      <c r="Q21" s="169" t="str">
+      <c r="P21" s="178"/>
+      <c r="Q21" s="178" t="str">
         <f>Model!M$16</f>
         <v>Am7</v>
       </c>
-      <c r="R21" s="169"/>
-      <c r="S21" s="169" t="str">
+      <c r="R21" s="178"/>
+      <c r="S21" s="178" t="str">
         <f>Model!N$16</f>
         <v>Bm7</v>
       </c>
-      <c r="T21" s="169"/>
-      <c r="U21" s="169" t="str">
+      <c r="T21" s="178"/>
+      <c r="U21" s="178" t="str">
         <f>Model!O$16</f>
         <v>CM7</v>
       </c>
-      <c r="V21" s="169"/>
-      <c r="W21" s="169" t="str">
+      <c r="V21" s="178"/>
+      <c r="W21" s="178" t="str">
         <f>Model!P$16</f>
         <v>D7</v>
       </c>
-      <c r="X21" s="169"/>
+      <c r="X21" s="178"/>
       <c r="Y21" s="48"/>
       <c r="Z21" s="48"/>
       <c r="AA21" s="48"/>
@@ -6168,12 +5310,12 @@
       <c r="AD21" s="48"/>
     </row>
     <row r="22" spans="2:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="163"/>
-      <c r="C22" s="163"/>
-      <c r="D22" s="163"/>
-      <c r="E22" s="163"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="163"/>
+      <c r="B22" s="172"/>
+      <c r="C22" s="172"/>
+      <c r="D22" s="172"/>
+      <c r="E22" s="172"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="172"/>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
       <c r="J22" s="73"/>
@@ -6199,16 +5341,16 @@
       <c r="AD22" s="49"/>
     </row>
     <row r="23" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="163"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="163"/>
-      <c r="E23" s="163"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="163"/>
-      <c r="H23" s="164" t="s">
+      <c r="B23" s="172"/>
+      <c r="C23" s="172"/>
+      <c r="D23" s="172"/>
+      <c r="E23" s="172"/>
+      <c r="F23" s="172"/>
+      <c r="G23" s="172"/>
+      <c r="H23" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="164"/>
+      <c r="I23" s="173"/>
       <c r="J23" s="57" t="str">
         <f>Model!J15</f>
         <v>E</v>
@@ -6237,11 +5379,11 @@
         <f>IF(Model!P15=0, "", Model!P15)</f>
         <v>D</v>
       </c>
-      <c r="S23" s="165" t="s">
+      <c r="S23" s="174" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="165"/>
-      <c r="U23" s="165"/>
+      <c r="T23" s="174"/>
+      <c r="U23" s="174"/>
       <c r="V23" s="75" t="str">
         <f>IF(Model!J13=1, "h", IF(Model!J13=2, "W", IF(Model!J13=3, "W+h", IF(Model!J13=4, "WW", IF(Model!J13=0, "", Model!J4)))))</f>
         <v>W</v>
@@ -6381,7 +5523,7 @@
       </c>
     </row>
     <row r="25" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="160" t="s">
+      <c r="B25" s="169" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="52" t="s">
@@ -6494,7 +5636,7 @@
       <c r="AD25" s="51"/>
     </row>
     <row r="26" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="160"/>
+      <c r="B26" s="169"/>
       <c r="C26" s="52" t="s">
         <v>14</v>
       </c>
@@ -6605,7 +5747,7 @@
       <c r="AD26" s="51"/>
     </row>
     <row r="27" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="160"/>
+      <c r="B27" s="169"/>
       <c r="C27" s="52" t="s">
         <v>13</v>
       </c>
@@ -6716,7 +5858,7 @@
       <c r="AD27" s="51"/>
     </row>
     <row r="28" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="160"/>
+      <c r="B28" s="169"/>
       <c r="C28" s="52" t="s">
         <v>10</v>
       </c>
@@ -6827,7 +5969,7 @@
       <c r="AD28" s="51"/>
     </row>
     <row r="29" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="160"/>
+      <c r="B29" s="169"/>
       <c r="C29" s="52" t="s">
         <v>12</v>
       </c>
@@ -6938,7 +6080,7 @@
       <c r="AD29" s="51"/>
     </row>
     <row r="30" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="166" t="s">
+      <c r="B30" s="179" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="52" t="s">
@@ -7051,7 +6193,7 @@
       <c r="AD30" s="51"/>
     </row>
     <row r="31" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="166"/>
+      <c r="B31" s="179"/>
       <c r="C31" s="52" t="s">
         <v>14</v>
       </c>
@@ -7162,7 +6304,7 @@
       <c r="AD31" s="51"/>
     </row>
     <row r="32" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="166"/>
+      <c r="B32" s="179"/>
       <c r="C32" s="52" t="s">
         <v>57</v>
       </c>
@@ -7273,7 +6415,7 @@
       <c r="AD32" s="51"/>
     </row>
     <row r="33" spans="2:30" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="166"/>
+      <c r="B33" s="179"/>
       <c r="C33" s="52" t="s">
         <v>51</v>
       </c>
@@ -7519,10 +6661,10 @@
       <c r="AC35" s="56"/>
     </row>
     <row r="36" spans="2:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="168" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="168"/>
+      <c r="B36" s="177" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="177"/>
       <c r="E36" s="70" t="s">
         <v>2</v>
       </c>
@@ -7546,17 +6688,17 @@
       </c>
     </row>
     <row r="37" spans="2:30" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B37" s="168"/>
-      <c r="C37" s="168"/>
-      <c r="E37" s="167" t="s">
+      <c r="B37" s="177"/>
+      <c r="C37" s="177"/>
+      <c r="E37" s="176" t="s">
         <v>192</v>
       </c>
-      <c r="F37" s="167"/>
-      <c r="G37" s="167"/>
-      <c r="H37" s="167"/>
-      <c r="I37" s="167"/>
-      <c r="J37" s="167"/>
-      <c r="K37" s="167"/>
+      <c r="F37" s="176"/>
+      <c r="G37" s="176"/>
+      <c r="H37" s="176"/>
+      <c r="I37" s="176"/>
+      <c r="J37" s="176"/>
+      <c r="K37" s="176"/>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B38" s="76"/>
@@ -7578,13 +6720,13 @@
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B13:B16"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="W3:X3"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="W20:X20"/>
-    <mergeCell ref="B13:B16"/>
     <mergeCell ref="B3:G6"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
@@ -7608,279 +6750,279 @@
     <mergeCell ref="S6:U6"/>
   </mergeCells>
   <conditionalFormatting sqref="W6:AA6">
-    <cfRule type="containsText" dxfId="223" priority="199" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="125" priority="199" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",W6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V6">
-    <cfRule type="containsText" dxfId="222" priority="82" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="124" priority="82" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",V6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6">
-    <cfRule type="containsText" dxfId="221" priority="81" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="123" priority="81" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AB6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V23">
-    <cfRule type="containsText" dxfId="220" priority="73" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="122" priority="73" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",V23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W23">
-    <cfRule type="containsText" dxfId="219" priority="72" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="121" priority="72" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",W23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23">
-    <cfRule type="containsText" dxfId="218" priority="71" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="120" priority="71" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",X23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y23">
-    <cfRule type="containsText" dxfId="217" priority="70" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="119" priority="70" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Y23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23">
-    <cfRule type="containsText" dxfId="216" priority="69" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="118" priority="69" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Z23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23">
-    <cfRule type="containsText" dxfId="215" priority="68" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="117" priority="68" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AA23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB23">
-    <cfRule type="containsText" dxfId="214" priority="67" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="116" priority="67" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AB23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:P33">
-    <cfRule type="containsBlanks" dxfId="213" priority="587">
+    <cfRule type="containsBlanks" dxfId="115" priority="587">
       <formula>LEN(TRIM(F25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AB16">
-    <cfRule type="containsBlanks" dxfId="212" priority="588">
+    <cfRule type="containsBlanks" dxfId="114" priority="588">
       <formula>LEN(TRIM(R8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R25:AB33">
-    <cfRule type="containsBlanks" dxfId="211" priority="51">
+    <cfRule type="containsBlanks" dxfId="113" priority="51">
       <formula>LEN(TRIM(R25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="expression" dxfId="210" priority="624">
+    <cfRule type="expression" dxfId="112" priority="624">
       <formula>FIND(7,Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="625">
+    <cfRule type="expression" dxfId="111" priority="625">
       <formula>FIND(6, Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="626">
+    <cfRule type="expression" dxfId="110" priority="626">
       <formula>FIND(5,Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="207" priority="627">
+    <cfRule type="expression" dxfId="109" priority="627">
       <formula>FIND(4,Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="628">
+    <cfRule type="expression" dxfId="108" priority="628">
       <formula>FIND(3, Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="629">
+    <cfRule type="expression" dxfId="107" priority="629">
       <formula>FIND(2, Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="630">
+    <cfRule type="expression" dxfId="106" priority="630">
       <formula>FIND(1, Q20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="expression" dxfId="203" priority="638">
+    <cfRule type="expression" dxfId="105" priority="638">
       <formula>FIND(7,O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="639">
+    <cfRule type="expression" dxfId="104" priority="639">
       <formula>FIND(6, O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="640">
+    <cfRule type="expression" dxfId="103" priority="640">
       <formula>FIND(5,O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="641">
+    <cfRule type="expression" dxfId="102" priority="641">
       <formula>FIND(4,O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="642">
+    <cfRule type="expression" dxfId="101" priority="642">
       <formula>FIND(3, O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="643">
+    <cfRule type="expression" dxfId="100" priority="643">
       <formula>FIND(2, O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="644">
+    <cfRule type="expression" dxfId="99" priority="644">
       <formula>FIND(1, O20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="expression" dxfId="196" priority="652">
+    <cfRule type="expression" dxfId="98" priority="652">
       <formula>FIND(7,M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="653">
+    <cfRule type="expression" dxfId="97" priority="653">
       <formula>FIND(6, M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="654">
+    <cfRule type="expression" dxfId="96" priority="654">
       <formula>FIND(5,M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="655">
+    <cfRule type="expression" dxfId="95" priority="655">
       <formula>FIND(4,M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="656">
+    <cfRule type="expression" dxfId="94" priority="656">
       <formula>FIND(3, M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="657">
+    <cfRule type="expression" dxfId="93" priority="657">
       <formula>FIND(2, M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="658">
+    <cfRule type="expression" dxfId="92" priority="658">
       <formula>FIND(1, M20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="expression" dxfId="189" priority="666">
+    <cfRule type="expression" dxfId="91" priority="666">
       <formula>FIND(7,K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="667">
+    <cfRule type="expression" dxfId="90" priority="667">
       <formula>FIND(6, K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="668">
+    <cfRule type="expression" dxfId="89" priority="668">
       <formula>FIND(5,K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="669">
+    <cfRule type="expression" dxfId="88" priority="669">
       <formula>FIND(4,K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="670">
+    <cfRule type="expression" dxfId="87" priority="670">
       <formula>FIND(3, K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="671">
+    <cfRule type="expression" dxfId="86" priority="671">
       <formula>FIND(2, K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="672">
+    <cfRule type="expression" dxfId="85" priority="672">
       <formula>FIND(1, K20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23">
-    <cfRule type="expression" dxfId="182" priority="673">
+    <cfRule type="expression" dxfId="84" priority="673">
       <formula>FIND(7,W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="674">
+    <cfRule type="expression" dxfId="83" priority="674">
       <formula>FIND(6, W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="675">
+    <cfRule type="expression" dxfId="82" priority="675">
       <formula>FIND(5,W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="676">
+    <cfRule type="expression" dxfId="81" priority="676">
       <formula>FIND(4,W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="677">
+    <cfRule type="expression" dxfId="80" priority="677">
       <formula>FIND(3, W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="678">
+    <cfRule type="expression" dxfId="79" priority="678">
       <formula>FIND(2, W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="679">
+    <cfRule type="expression" dxfId="78" priority="679">
       <formula>FIND(1, W20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="175" priority="680">
+    <cfRule type="expression" dxfId="77" priority="680">
       <formula>FIND(7,U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="681">
+    <cfRule type="expression" dxfId="76" priority="681">
       <formula>FIND(6, U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="682">
+    <cfRule type="expression" dxfId="75" priority="682">
       <formula>FIND(5,U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="683">
+    <cfRule type="expression" dxfId="74" priority="683">
       <formula>FIND(4,U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="684">
+    <cfRule type="expression" dxfId="73" priority="684">
       <formula>FIND(3, U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="685">
+    <cfRule type="expression" dxfId="72" priority="685">
       <formula>FIND(2, U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="686">
+    <cfRule type="expression" dxfId="71" priority="686">
       <formula>FIND(1, U20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="expression" dxfId="168" priority="687">
+    <cfRule type="expression" dxfId="70" priority="687">
       <formula>FIND(7,S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="688">
+    <cfRule type="expression" dxfId="69" priority="688">
       <formula>FIND(6, S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="689">
+    <cfRule type="expression" dxfId="68" priority="689">
       <formula>FIND(5,S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="690">
+    <cfRule type="expression" dxfId="67" priority="690">
       <formula>FIND(4,S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="691">
+    <cfRule type="expression" dxfId="66" priority="691">
       <formula>FIND(3, S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="692">
+    <cfRule type="expression" dxfId="65" priority="692">
       <formula>FIND(2, S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="693">
+    <cfRule type="expression" dxfId="64" priority="693">
       <formula>FIND(1, S20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:P16">
-    <cfRule type="containsBlanks" dxfId="161" priority="43">
+    <cfRule type="containsBlanks" dxfId="63" priority="43">
       <formula>LEN(TRIM(F8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF8:AF17">
-    <cfRule type="expression" dxfId="125" priority="1730">
+    <cfRule type="expression" dxfId="62" priority="1730">
       <formula>AND($AF$15=TRUE, SEARCH("6", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="1731">
+    <cfRule type="expression" dxfId="61" priority="1731">
       <formula>AND($AF$10=TRUE, SEARCH("1", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="1732">
+    <cfRule type="expression" dxfId="60" priority="1732">
       <formula>AND($AF$11=TRUE, SEARCH("2", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="1733">
+    <cfRule type="expression" dxfId="59" priority="1733">
       <formula>AND($AF$12=TRUE, SEARCH("3", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="1734">
+    <cfRule type="expression" dxfId="58" priority="1734">
       <formula>AND($AF$13=TRUE, SEARCH("4", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="1735">
+    <cfRule type="expression" dxfId="57" priority="1735">
       <formula>AND($AF$14=TRUE, SEARCH("5", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="1736">
+    <cfRule type="expression" dxfId="56" priority="1736">
       <formula>AND(#REF!=TRUE, SEARCH("7", AF8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AE13 AE17">
-    <cfRule type="expression" dxfId="118" priority="1737">
+    <cfRule type="expression" dxfId="55" priority="1737">
       <formula>AND($AF$8, SEARCH("1", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="1738">
+    <cfRule type="expression" dxfId="54" priority="1738">
       <formula>AND($AF$9, SEARCH("2", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="1739">
+    <cfRule type="expression" dxfId="53" priority="1739">
       <formula>AND($AF$10, SEARCH("3", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="1740">
+    <cfRule type="expression" dxfId="52" priority="1740">
       <formula>AND($AF$11, SEARCH("4", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="1741">
+    <cfRule type="expression" dxfId="51" priority="1741">
       <formula>AND($AF$12, SEARCH("5", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="1742">
+    <cfRule type="expression" dxfId="50" priority="1742">
       <formula>AND($AF$13, SEARCH("6", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="1743">
+    <cfRule type="expression" dxfId="49" priority="1743">
       <formula>AND($AF$17, SEARCH("7", AE8))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7910,7 +7052,7 @@
             <xm:f>SEARCH("6", Model!J$3)</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FFA63AB8"/>
+                <color rgb="FF642C76"/>
               </font>
             </x14:dxf>
           </x14:cfRule>
@@ -7926,7 +7068,7 @@
             <xm:f>SEARCH("4", Model!J$3)</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FFB7EE00"/>
+                <color rgb="FFB567F5"/>
               </font>
             </x14:dxf>
           </x14:cfRule>
@@ -7934,7 +7076,7 @@
             <xm:f>SEARCH("3", Model!J$3)</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF70C3FC"/>
+                <color rgb="FFF4DA3E"/>
               </font>
             </x14:dxf>
           </x14:cfRule>
@@ -7942,7 +7084,7 @@
             <xm:f>SEARCH("2", Model!J$3)</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FFC07DE2"/>
+                <color rgb="FFE4D2F2"/>
               </font>
             </x14:dxf>
           </x14:cfRule>
@@ -7950,7 +7092,7 @@
             <xm:f>SEARCH("1", Model!J$3)</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF2992D9"/>
+                <color rgb="FF3788CB"/>
               </font>
               <fill>
                 <patternFill patternType="none">
@@ -8422,21 +7564,21 @@
         <v>68</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="175" t="s">
+      <c r="F1" s="185" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="176"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="171" t="s">
+      <c r="G1" s="186"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="181" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="171"/>
-      <c r="K1" s="171"/>
-      <c r="L1" s="171"/>
-      <c r="M1" s="171"/>
-      <c r="N1" s="171"/>
-      <c r="O1" s="171"/>
-      <c r="P1" s="171"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
       <c r="Q1"/>
       <c r="R1"/>
       <c r="S1"/>
@@ -8673,11 +7815,11 @@
       <c r="D3" s="11">
         <v>10</v>
       </c>
-      <c r="F3" s="172" t="s">
+      <c r="F3" s="182" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="173"/>
-      <c r="H3" s="174"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="184"/>
       <c r="I3" s="85" t="s">
         <v>34</v>
       </c>
@@ -8910,11 +8052,11 @@
       <c r="D5" s="11">
         <v>8</v>
       </c>
-      <c r="F5" s="172" t="s">
+      <c r="F5" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="173"/>
-      <c r="H5" s="174"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="184"/>
       <c r="I5" s="113" t="s">
         <v>31</v>
       </c>
@@ -9284,7 +8426,7 @@
       </c>
       <c r="L8" s="116" t="b">
         <f>Fretboards!AF10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="116" t="b">
         <f>Fretboards!AF11</f>
@@ -9385,16 +8527,16 @@
       <c r="D9" s="11">
         <v>13</v>
       </c>
-      <c r="I9" s="170" t="s">
+      <c r="I9" s="180" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="170"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="170"/>
-      <c r="M9" s="170"/>
-      <c r="N9" s="170"/>
-      <c r="O9" s="170"/>
-      <c r="P9" s="170"/>
+      <c r="J9" s="180"/>
+      <c r="K9" s="180"/>
+      <c r="L9" s="180"/>
+      <c r="M9" s="180"/>
+      <c r="N9" s="180"/>
+      <c r="O9" s="180"/>
+      <c r="P9" s="180"/>
       <c r="Y9" s="85">
         <v>8</v>
       </c>
@@ -9498,14 +8640,14 @@
       <c r="D10" s="9">
         <v>10</v>
       </c>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
-      <c r="K10" s="171"/>
-      <c r="L10" s="171"/>
-      <c r="M10" s="171"/>
-      <c r="N10" s="171"/>
-      <c r="O10" s="171"/>
-      <c r="P10" s="171"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="181"/>
+      <c r="M10" s="181"/>
+      <c r="N10" s="181"/>
+      <c r="O10" s="181"/>
+      <c r="P10" s="181"/>
       <c r="Y10" s="85">
         <v>9</v>
       </c>
@@ -13325,48 +12467,48 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="J17:P17">
-    <cfRule type="expression" dxfId="237" priority="57">
+    <cfRule type="expression" dxfId="13" priority="57">
       <formula>AND($O$8=TRUE, SEARCH("6", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="58">
+    <cfRule type="expression" dxfId="12" priority="58">
       <formula>AND($J$8=TRUE, SEARCH("1", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="59">
+    <cfRule type="expression" dxfId="11" priority="59">
       <formula>AND($K$8=TRUE, SEARCH("2", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="60">
+    <cfRule type="expression" dxfId="10" priority="60">
       <formula>AND($L$8=TRUE, SEARCH("3", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="61">
+    <cfRule type="expression" dxfId="9" priority="61">
       <formula>AND($M$8=TRUE, SEARCH("4", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="62">
+    <cfRule type="expression" dxfId="8" priority="62">
       <formula>AND($N$8=TRUE, SEARCH("5", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="63">
+    <cfRule type="expression" dxfId="7" priority="63">
       <formula>AND($P$8=TRUE, SEARCH("7", J17))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="expression" dxfId="230" priority="1709">
+    <cfRule type="expression" dxfId="6" priority="1709">
       <formula>AND($K$23=TRUE, SEARCH("6", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="1710">
+    <cfRule type="expression" dxfId="5" priority="1710">
       <formula>AND($E$21=TRUE, SEARCH("1", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="1711">
+    <cfRule type="expression" dxfId="4" priority="1711">
       <formula>AND($F$21=TRUE, SEARCH("2", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="1712">
+    <cfRule type="expression" dxfId="3" priority="1712">
       <formula>AND($G$21=TRUE, SEARCH("3", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="1713">
+    <cfRule type="expression" dxfId="2" priority="1713">
       <formula>AND($I$23=TRUE, SEARCH("4", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="1714">
+    <cfRule type="expression" dxfId="1" priority="1714">
       <formula>AND($J$23=TRUE, SEARCH("5", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="1715">
+    <cfRule type="expression" dxfId="0" priority="1715">
       <formula>AND($L$23=TRUE, SEARCH("7", J8))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added basic Circle of Fifths to Spreadsheet
</commit_message>
<xml_diff>
--- a/Shredsheets.xlsx
+++ b/Shredsheets.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Shredsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DEA5C2-551D-485F-BB61-1EAADB1C5C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F280A81D-50AD-449B-9864-9A0CB33585EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fretboards" sheetId="1" r:id="rId1"/>
-    <sheet name="Model" sheetId="2" r:id="rId2"/>
+    <sheet name="Circle of Fifths" sheetId="4" r:id="rId2"/>
+    <sheet name="Model" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Model!#REF!</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">Model!#REF!</definedName>
     <definedName name="IntervalCharacters">{"W","W","h","W","W","W","h","W","W","h","W","W","W","h"}</definedName>
     <definedName name="IntervalOffset">MATCH(ModalRootNote, ReversedNotes, 0) - 1</definedName>
     <definedName name="IntervalOffset2">MATCH(ModalRootNote2, ReversedNotes, 0) - 1</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="222">
   <si>
     <t>C</t>
   </si>
@@ -438,12 +439,6 @@
     <t>Ionian (Major)</t>
   </si>
   <si>
-    <t>Major Chord Tones</t>
-  </si>
-  <si>
-    <t>Minor Chord Tones</t>
-  </si>
-  <si>
     <t>Diminished</t>
   </si>
   <si>
@@ -676,13 +671,55 @@
   </si>
   <si>
     <t>Minor Triads</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>f♯</t>
+  </si>
+  <si>
+    <t>e♭</t>
+  </si>
+  <si>
+    <t>b♭</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>c♯</t>
+  </si>
+  <si>
+    <t>g♯</t>
+  </si>
+  <si>
+    <t>d♯</t>
+  </si>
+  <si>
+    <t>M7 Chord Tones</t>
+  </si>
+  <si>
+    <t>m7 Chord Tones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1025,6 +1062,20 @@
       <sz val="12"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="72"/>
+      <color theme="1"/>
+      <name val="Segoe UI Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Segoe UI Black"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1772,7 +1823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2151,6 +2202,28 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2160,28 +2233,22 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2208,93 +2275,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="138">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="130">
     <dxf>
       <font>
         <color theme="0" tint="-4.9989318521683403E-2"/>
@@ -2781,6 +2766,78 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0" tint="-4.9989318521683403E-2"/>
       </font>
       <fill>
@@ -3253,48 +3310,6 @@
         <i val="0"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3320,6 +3335,421 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>108376</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>403221</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>375271</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Group 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1F2486D-E9B3-49F2-ACB1-1040D5AD99FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm rot="20688759">
+          <a:off x="2489626" y="1562284"/>
+          <a:ext cx="6009845" cy="5956737"/>
+          <a:chOff x="4197163" y="2454088"/>
+          <a:chExt cx="7813862" cy="7867650"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="Oval 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09157681-1A33-F979-F2AC-30BD53DC21C4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4197163" y="2454088"/>
+            <a:ext cx="7813862" cy="7867650"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="50800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="29" name="Group 28">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3693FAC8-6729-BCA1-887F-402E236D3715}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="4340194" y="2454088"/>
+            <a:ext cx="7540958" cy="7867650"/>
+            <a:chOff x="3827093" y="1557617"/>
+            <a:chExt cx="7598633" cy="7867650"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="36" name="Straight Connector 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{893503EC-5D58-CB2B-D159-066E21F3C64A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="911241" flipV="1">
+              <a:off x="3827093" y="4427101"/>
+              <a:ext cx="7598633" cy="2079454"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="37" name="Straight Connector 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C64E2C8-CE54-6680-9905-A25A27A014BD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="28" idx="0"/>
+              <a:endCxn id="28" idx="4"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7619782" y="1557617"/>
+              <a:ext cx="0" cy="7867650"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="30" name="Group 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99CB1428-3D51-FDA3-B5AC-8DB24CFB4E8E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm rot="19794269">
+            <a:off x="5366848" y="3019402"/>
+            <a:ext cx="5497513" cy="6745942"/>
+            <a:chOff x="4799353" y="2051945"/>
+            <a:chExt cx="5539559" cy="6745942"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="34" name="Straight Connector 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D955B14B-3D80-F1B6-1CD1-594C63931279}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="2716972" flipV="1">
+              <a:off x="4738854" y="2623804"/>
+              <a:ext cx="5660558" cy="5539559"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="35" name="Straight Connector 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A28E1107-89B0-C88B-22F2-C308A2B51309}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="1805731">
+              <a:off x="5558025" y="2051945"/>
+              <a:ext cx="4042389" cy="6745942"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="31" name="Group 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1218B1E4-BD58-B281-226B-148BBF566FA8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm rot="17994305">
+            <a:off x="4287482" y="2623488"/>
+            <a:ext cx="7596076" cy="7538915"/>
+            <a:chOff x="3896861" y="1347949"/>
+            <a:chExt cx="7553699" cy="7634135"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="32" name="Straight Connector 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D4A026C-FD98-9DC8-D986-EF6744C9305C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="4516936" flipV="1">
+              <a:off x="6650492" y="1396356"/>
+              <a:ext cx="2046437" cy="7553699"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="33" name="Straight Connector 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8B4F27A-3CE9-B3E7-69A6-E853739CBCB6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr/>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="4516936">
+              <a:off x="3892901" y="4183651"/>
+              <a:ext cx="7634135" cy="1962731"/>
+            </a:xfrm>
+            <a:prstGeom prst="line">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3624,8 +4054,8 @@
   </sheetPr>
   <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3718,17 +4148,17 @@
     <row r="2" spans="1:32" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="153" t="str">
+        <v>147</v>
+      </c>
+      <c r="B3" s="155" t="str">
         <f>IF(B17 = "Ionian (Major)", B8 &amp; " Major", IF(B17 = "Aolian (Minor)", B8 &amp; " Minor", B8 &amp; " " &amp; B17))</f>
         <v>C Major Triads</v>
       </c>
-      <c r="C3" s="153"/>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
       <c r="K3" s="152">
         <f>IF(Model!J3="0","",Model!J3)</f>
         <v>1</v>
@@ -3764,69 +4194,69 @@
         <v/>
       </c>
       <c r="X3" s="152"/>
-      <c r="Z3" s="148" t="s">
+      <c r="Z3" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" s="148"/>
-      <c r="AB3" s="149" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="149"/>
+      <c r="AA3" s="156"/>
+      <c r="AB3" s="157" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="157"/>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="K4" s="151" t="str">
+      <c r="B4" s="155"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="K4" s="154" t="str">
         <f>Model!J7</f>
         <v>CM7</v>
       </c>
-      <c r="L4" s="151"/>
-      <c r="M4" s="151" t="str">
+      <c r="L4" s="154"/>
+      <c r="M4" s="154" t="str">
         <f>Model!K7</f>
         <v/>
       </c>
-      <c r="N4" s="151"/>
-      <c r="O4" s="151" t="str">
+      <c r="N4" s="154"/>
+      <c r="O4" s="154" t="str">
         <f>Model!L7</f>
         <v>Em7</v>
       </c>
-      <c r="P4" s="151"/>
-      <c r="Q4" s="151" t="str">
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154" t="str">
         <f>Model!M7</f>
         <v/>
       </c>
-      <c r="R4" s="151"/>
-      <c r="S4" s="151" t="str">
+      <c r="R4" s="154"/>
+      <c r="S4" s="154" t="str">
         <f>Model!N7</f>
         <v>G7</v>
       </c>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151" t="str">
+      <c r="T4" s="154"/>
+      <c r="U4" s="154" t="str">
         <f>Model!O7</f>
         <v/>
       </c>
-      <c r="V4" s="151"/>
-      <c r="W4" s="151" t="str">
+      <c r="V4" s="154"/>
+      <c r="W4" s="154" t="str">
         <f>Model!P7</f>
         <v/>
       </c>
-      <c r="X4" s="151"/>
-      <c r="Z4" s="148"/>
-      <c r="AA4" s="148"/>
-      <c r="AB4" s="149"/>
-      <c r="AC4" s="149"/>
+      <c r="X4" s="154"/>
+      <c r="Z4" s="156"/>
+      <c r="AA4" s="156"/>
+      <c r="AB4" s="157"/>
+      <c r="AC4" s="157"/>
     </row>
     <row r="5" spans="1:32" s="42" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="153"/>
-      <c r="C5" s="153"/>
-      <c r="D5" s="153"/>
-      <c r="E5" s="153"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="153"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
       <c r="J5" s="64"/>
       <c r="K5" s="48"/>
       <c r="L5" s="64"/>
@@ -3834,22 +4264,22 @@
       <c r="N5" s="64"/>
       <c r="O5" s="64"/>
       <c r="P5" s="64"/>
-      <c r="Z5" s="148"/>
-      <c r="AA5" s="148"/>
-      <c r="AB5" s="149"/>
-      <c r="AC5" s="149"/>
+      <c r="Z5" s="156"/>
+      <c r="AA5" s="156"/>
+      <c r="AB5" s="157"/>
+      <c r="AC5" s="157"/>
     </row>
     <row r="6" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="153"/>
-      <c r="C6" s="153"/>
-      <c r="D6" s="153"/>
-      <c r="E6" s="153"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="154" t="s">
+      <c r="B6" s="155"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="155"/>
+      <c r="G6" s="155"/>
+      <c r="H6" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="154"/>
+      <c r="I6" s="159"/>
       <c r="J6" s="47" t="str">
         <f>IF(Model!J6=0,"", Model!J6)</f>
         <v>C</v>
@@ -3878,11 +4308,11 @@
         <f>IF(Model!P6=0,"", Model!P6)</f>
         <v/>
       </c>
-      <c r="S6" s="154" t="s">
+      <c r="S6" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="154"/>
-      <c r="U6" s="154"/>
+      <c r="T6" s="159"/>
+      <c r="U6" s="159"/>
       <c r="V6" s="65" t="str">
         <f>IF(Model!J4=1, "h", IF(Model!J4=2, "W", IF(Model!J4=3, "W+h", IF(Model!J4=4, "WW", IF(Model!J4=0, "", IF(Model!J4=5, "WWh", Model!J4))))))</f>
         <v/>
@@ -3911,10 +4341,10 @@
         <f>IF(Model!P4=1, "h", IF(Model!P4=2, "W", IF(Model!P4=3, "W+h", IF(Model!P4=4, "WW", IF(Model!P4=0, "", IF(Model!P4=5, "WWh", Model!P4))))))</f>
         <v>WWh</v>
       </c>
-      <c r="AE6" s="155" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="155"/>
+      <c r="AE6" s="149" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="149"/>
     </row>
     <row r="7" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="62" t="s">
@@ -4025,14 +4455,14 @@
         <v>24</v>
       </c>
       <c r="AE7" s="141" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AF7" s="142" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="150" t="s">
+      <c r="B8" s="158" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="43" t="s">
@@ -4150,7 +4580,7 @@
       </c>
     </row>
     <row r="9" spans="1:32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="150"/>
+      <c r="B9" s="158"/>
       <c r="C9" s="43" t="s">
         <v>14</v>
       </c>
@@ -4266,7 +4696,7 @@
       </c>
     </row>
     <row r="10" spans="1:32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="150"/>
+      <c r="B10" s="158"/>
       <c r="C10" s="43" t="s">
         <v>13</v>
       </c>
@@ -4382,7 +4812,7 @@
       </c>
     </row>
     <row r="11" spans="1:32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="150"/>
+      <c r="B11" s="158"/>
       <c r="C11" s="43" t="s">
         <v>10</v>
       </c>
@@ -4498,7 +4928,7 @@
       </c>
     </row>
     <row r="12" spans="1:32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="150"/>
+      <c r="B12" s="158"/>
       <c r="C12" s="43" t="s">
         <v>12</v>
       </c>
@@ -4614,7 +5044,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="153" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="43" t="s">
@@ -4732,7 +5162,7 @@
       </c>
     </row>
     <row r="14" spans="1:32" s="2" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="158"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="43" t="s">
         <v>14</v>
       </c>
@@ -4844,7 +5274,7 @@
       <c r="AF14" s="145"/>
     </row>
     <row r="15" spans="1:32" s="2" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="158"/>
+      <c r="B15" s="153"/>
       <c r="C15" s="43" t="s">
         <v>57</v>
       </c>
@@ -4956,7 +5386,7 @@
       <c r="AF15" s="145"/>
     </row>
     <row r="16" spans="1:32" s="2" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="158"/>
+      <c r="B16" s="153"/>
       <c r="C16" s="43" t="s">
         <v>51</v>
       </c>
@@ -5069,7 +5499,7 @@
     </row>
     <row r="17" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="45" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -5232,15 +5662,15 @@
       <c r="AC19" s="99"/>
     </row>
     <row r="20" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="153" t="str">
+      <c r="B20" s="155" t="str">
         <f>IF(B34 = "Ionian (Major)", B25 &amp; " Major", IF(B34 = "Aolian (Minor)", B25 &amp; " Minor", B25 &amp; " " &amp; B34))</f>
         <v>E Aeolian (Minor)</v>
       </c>
-      <c r="C20" s="153"/>
-      <c r="D20" s="153"/>
-      <c r="E20" s="153"/>
-      <c r="F20" s="153"/>
-      <c r="G20" s="153"/>
+      <c r="C20" s="155"/>
+      <c r="D20" s="155"/>
+      <c r="E20" s="155"/>
+      <c r="F20" s="155"/>
+      <c r="G20" s="155"/>
       <c r="K20" s="152">
         <f>IF(Model!J12="0","",Model!J12)</f>
         <v>1</v>
@@ -5278,53 +5708,53 @@
       <c r="X20" s="152"/>
     </row>
     <row r="21" spans="2:32" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="153"/>
-      <c r="C21" s="153"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="153"/>
-      <c r="F21" s="153"/>
-      <c r="G21" s="153"/>
-      <c r="K21" s="157" t="str">
+      <c r="B21" s="155"/>
+      <c r="C21" s="155"/>
+      <c r="D21" s="155"/>
+      <c r="E21" s="155"/>
+      <c r="F21" s="155"/>
+      <c r="G21" s="155"/>
+      <c r="K21" s="151" t="str">
         <f>Model!J$16</f>
         <v>Em7</v>
       </c>
-      <c r="L21" s="157" t="str">
+      <c r="L21" s="151" t="str">
         <f>Model!K$16</f>
         <v>F♯m7ø</v>
       </c>
-      <c r="M21" s="157" t="str">
+      <c r="M21" s="151" t="str">
         <f>Model!K$16</f>
         <v>F♯m7ø</v>
       </c>
-      <c r="N21" s="157" t="str">
+      <c r="N21" s="151" t="str">
         <f>Model!M$16</f>
         <v>Am7</v>
       </c>
-      <c r="O21" s="157" t="str">
+      <c r="O21" s="151" t="str">
         <f>Model!L$16</f>
         <v>GM7</v>
       </c>
-      <c r="P21" s="157"/>
-      <c r="Q21" s="157" t="str">
+      <c r="P21" s="151"/>
+      <c r="Q21" s="151" t="str">
         <f>Model!M$16</f>
         <v>Am7</v>
       </c>
-      <c r="R21" s="157"/>
-      <c r="S21" s="157" t="str">
+      <c r="R21" s="151"/>
+      <c r="S21" s="151" t="str">
         <f>Model!N$16</f>
         <v>Bm7</v>
       </c>
-      <c r="T21" s="157"/>
-      <c r="U21" s="157" t="str">
+      <c r="T21" s="151"/>
+      <c r="U21" s="151" t="str">
         <f>Model!O$16</f>
         <v>CM7</v>
       </c>
-      <c r="V21" s="157"/>
-      <c r="W21" s="157" t="str">
+      <c r="V21" s="151"/>
+      <c r="W21" s="151" t="str">
         <f>Model!P$16</f>
         <v>D7</v>
       </c>
-      <c r="X21" s="157"/>
+      <c r="X21" s="151"/>
       <c r="Y21"/>
       <c r="Z21"/>
       <c r="AA21"/>
@@ -5333,12 +5763,12 @@
       <c r="AD21"/>
     </row>
     <row r="22" spans="2:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="153"/>
-      <c r="C22" s="153"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="153"/>
-      <c r="F22" s="153"/>
-      <c r="G22" s="153"/>
+      <c r="B22" s="155"/>
+      <c r="C22" s="155"/>
+      <c r="D22" s="155"/>
+      <c r="E22" s="155"/>
+      <c r="F22" s="155"/>
+      <c r="G22" s="155"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="63"/>
@@ -5364,16 +5794,16 @@
       <c r="AD22" s="42"/>
     </row>
     <row r="23" spans="2:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="153"/>
-      <c r="C23" s="153"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="153"/>
-      <c r="F23" s="153"/>
-      <c r="G23" s="153"/>
-      <c r="H23" s="154" t="s">
+      <c r="B23" s="155"/>
+      <c r="C23" s="155"/>
+      <c r="D23" s="155"/>
+      <c r="E23" s="155"/>
+      <c r="F23" s="155"/>
+      <c r="G23" s="155"/>
+      <c r="H23" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="154"/>
+      <c r="I23" s="159"/>
       <c r="J23" s="47" t="str">
         <f>Model!J15</f>
         <v>E</v>
@@ -5402,11 +5832,11 @@
         <f>IF(Model!P15=0, "", Model!P15)</f>
         <v>D</v>
       </c>
-      <c r="S23" s="154" t="s">
+      <c r="S23" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="T23" s="154"/>
-      <c r="U23" s="154"/>
+      <c r="T23" s="159"/>
+      <c r="U23" s="159"/>
       <c r="V23" s="65" t="str">
         <f>IF(Model!J13=1, "h", IF(Model!J13=2, "W", IF(Model!J13=3, "W+h", IF(Model!J13=4, "WW", IF(Model!J13=0, "", IF(Model!J13=5, "WWh", Model!J4))))))</f>
         <v>W</v>
@@ -5546,7 +5976,7 @@
       </c>
     </row>
     <row r="25" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="150" t="s">
+      <c r="B25" s="158" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="43" t="s">
@@ -5659,7 +6089,7 @@
       <c r="AD25" s="2"/>
     </row>
     <row r="26" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="150"/>
+      <c r="B26" s="158"/>
       <c r="C26" s="43" t="s">
         <v>14</v>
       </c>
@@ -5770,7 +6200,7 @@
       <c r="AD26" s="2"/>
     </row>
     <row r="27" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="150"/>
+      <c r="B27" s="158"/>
       <c r="C27" s="43" t="s">
         <v>13</v>
       </c>
@@ -5881,7 +6311,7 @@
       <c r="AD27" s="2"/>
     </row>
     <row r="28" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="150"/>
+      <c r="B28" s="158"/>
       <c r="C28" s="43" t="s">
         <v>10</v>
       </c>
@@ -5992,7 +6422,7 @@
       <c r="AD28" s="2"/>
     </row>
     <row r="29" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="150"/>
+      <c r="B29" s="158"/>
       <c r="C29" s="43" t="s">
         <v>12</v>
       </c>
@@ -6103,7 +6533,7 @@
       <c r="AD29" s="2"/>
     </row>
     <row r="30" spans="2:32" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="158" t="s">
+      <c r="B30" s="153" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="43" t="s">
@@ -6216,7 +6646,7 @@
       <c r="AD30" s="2"/>
     </row>
     <row r="31" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="158"/>
+      <c r="B31" s="153"/>
       <c r="C31" s="43" t="s">
         <v>14</v>
       </c>
@@ -6327,7 +6757,7 @@
       <c r="AD31" s="2"/>
     </row>
     <row r="32" spans="2:32" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="158"/>
+      <c r="B32" s="153"/>
       <c r="C32" s="43" t="s">
         <v>57</v>
       </c>
@@ -6438,7 +6868,7 @@
       <c r="AD32" s="2"/>
     </row>
     <row r="33" spans="2:30" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="158"/>
+      <c r="B33" s="153"/>
       <c r="C33" s="43" t="s">
         <v>51</v>
       </c>
@@ -6550,7 +6980,7 @@
     </row>
     <row r="34" spans="2:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -6684,10 +7114,10 @@
       <c r="AC35" s="46"/>
     </row>
     <row r="36" spans="2:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="155" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="155"/>
+      <c r="B36" s="149" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="149"/>
       <c r="E36" s="60" t="s">
         <v>2</v>
       </c>
@@ -6711,23 +7141,50 @@
       </c>
     </row>
     <row r="37" spans="2:30" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B37" s="155"/>
-      <c r="C37" s="155"/>
-      <c r="E37" s="156" t="s">
-        <v>191</v>
-      </c>
-      <c r="F37" s="156"/>
-      <c r="G37" s="156"/>
-      <c r="H37" s="156"/>
-      <c r="I37" s="156"/>
-      <c r="J37" s="156"/>
-      <c r="K37" s="156"/>
+      <c r="B37" s="149"/>
+      <c r="C37" s="149"/>
+      <c r="E37" s="150" t="s">
+        <v>189</v>
+      </c>
+      <c r="F37" s="150"/>
+      <c r="G37" s="150"/>
+      <c r="H37" s="150"/>
+      <c r="I37" s="150"/>
+      <c r="J37" s="150"/>
+      <c r="K37" s="150"/>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B38" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="Z3:AA5"/>
+    <mergeCell ref="AB3:AC5"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="B20:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="W20:X20"/>
     <mergeCell ref="AE6:AF6"/>
     <mergeCell ref="E37:K37"/>
     <mergeCell ref="B36:C37"/>
@@ -6744,328 +7201,301 @@
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="B13:B16"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="Z3:AA5"/>
-    <mergeCell ref="AB3:AC5"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="B20:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="S6:U6"/>
   </mergeCells>
   <conditionalFormatting sqref="V6">
-    <cfRule type="containsText" dxfId="12" priority="94" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="129" priority="94" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",V6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V23">
-    <cfRule type="containsText" dxfId="135" priority="85" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="128" priority="85" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",V23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:P33">
-    <cfRule type="containsBlanks" dxfId="128" priority="599">
+    <cfRule type="containsBlanks" dxfId="127" priority="599">
       <formula>LEN(TRIM(F25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AB16">
-    <cfRule type="containsBlanks" dxfId="127" priority="600">
+    <cfRule type="containsBlanks" dxfId="126" priority="600">
       <formula>LEN(TRIM(R8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R25:AB33">
-    <cfRule type="containsBlanks" dxfId="126" priority="63">
+    <cfRule type="containsBlanks" dxfId="125" priority="63">
       <formula>LEN(TRIM(R25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="expression" dxfId="125" priority="636">
+    <cfRule type="expression" dxfId="124" priority="636">
       <formula>FIND(7,Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="637">
+    <cfRule type="expression" dxfId="123" priority="637">
       <formula>FIND(6, Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="638">
+    <cfRule type="expression" dxfId="122" priority="638">
       <formula>FIND(5,Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="639">
+    <cfRule type="expression" dxfId="121" priority="639">
       <formula>FIND(4,Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="640">
+    <cfRule type="expression" dxfId="120" priority="640">
       <formula>FIND(3, Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="641">
+    <cfRule type="expression" dxfId="119" priority="641">
       <formula>FIND(2, Q20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="642">
+    <cfRule type="expression" dxfId="118" priority="642">
       <formula>FIND(1, Q20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="expression" dxfId="118" priority="650">
+    <cfRule type="expression" dxfId="117" priority="650">
       <formula>FIND(7,O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="651">
+    <cfRule type="expression" dxfId="116" priority="651">
       <formula>FIND(6, O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="652">
+    <cfRule type="expression" dxfId="115" priority="652">
       <formula>FIND(5,O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="653">
+    <cfRule type="expression" dxfId="114" priority="653">
       <formula>FIND(4,O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="654">
+    <cfRule type="expression" dxfId="113" priority="654">
       <formula>FIND(3, O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="655">
+    <cfRule type="expression" dxfId="112" priority="655">
       <formula>FIND(2, O20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="656">
+    <cfRule type="expression" dxfId="111" priority="656">
       <formula>FIND(1, O20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="expression" dxfId="111" priority="664">
+    <cfRule type="expression" dxfId="110" priority="664">
       <formula>FIND(7,M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="665">
+    <cfRule type="expression" dxfId="109" priority="665">
       <formula>FIND(6, M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="666">
+    <cfRule type="expression" dxfId="108" priority="666">
       <formula>FIND(5,M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="667">
+    <cfRule type="expression" dxfId="107" priority="667">
       <formula>FIND(4,M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="668">
+    <cfRule type="expression" dxfId="106" priority="668">
       <formula>FIND(3, M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="669">
+    <cfRule type="expression" dxfId="105" priority="669">
       <formula>FIND(2, M20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="670">
+    <cfRule type="expression" dxfId="104" priority="670">
       <formula>FIND(1, M20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="expression" dxfId="104" priority="678">
+    <cfRule type="expression" dxfId="103" priority="678">
       <formula>FIND(7,K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="679">
+    <cfRule type="expression" dxfId="102" priority="679">
       <formula>FIND(6, K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="680">
+    <cfRule type="expression" dxfId="101" priority="680">
       <formula>FIND(5,K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="681">
+    <cfRule type="expression" dxfId="100" priority="681">
       <formula>FIND(4,K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="682">
+    <cfRule type="expression" dxfId="99" priority="682">
       <formula>FIND(3, K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="683">
+    <cfRule type="expression" dxfId="98" priority="683">
       <formula>FIND(2, K20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="684">
+    <cfRule type="expression" dxfId="97" priority="684">
       <formula>FIND(1, K20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23">
-    <cfRule type="expression" dxfId="97" priority="685">
+    <cfRule type="expression" dxfId="96" priority="685">
       <formula>FIND(7,W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="686">
+    <cfRule type="expression" dxfId="95" priority="686">
       <formula>FIND(6, W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="687">
+    <cfRule type="expression" dxfId="94" priority="687">
       <formula>FIND(5,W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="688">
+    <cfRule type="expression" dxfId="93" priority="688">
       <formula>FIND(4,W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="689">
+    <cfRule type="expression" dxfId="92" priority="689">
       <formula>FIND(3, W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="690">
+    <cfRule type="expression" dxfId="91" priority="690">
       <formula>FIND(2, W20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="691">
+    <cfRule type="expression" dxfId="90" priority="691">
       <formula>FIND(1, W20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="90" priority="692">
+    <cfRule type="expression" dxfId="89" priority="692">
       <formula>FIND(7,U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="693">
+    <cfRule type="expression" dxfId="88" priority="693">
       <formula>FIND(6, U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="694">
+    <cfRule type="expression" dxfId="87" priority="694">
       <formula>FIND(5,U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="695">
+    <cfRule type="expression" dxfId="86" priority="695">
       <formula>FIND(4,U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="696">
+    <cfRule type="expression" dxfId="85" priority="696">
       <formula>FIND(3, U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="697">
+    <cfRule type="expression" dxfId="84" priority="697">
       <formula>FIND(2, U20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="698">
+    <cfRule type="expression" dxfId="83" priority="698">
       <formula>FIND(1, U20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="expression" dxfId="83" priority="699">
+    <cfRule type="expression" dxfId="82" priority="699">
       <formula>FIND(7,S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="700">
+    <cfRule type="expression" dxfId="81" priority="700">
       <formula>FIND(6, S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="701">
+    <cfRule type="expression" dxfId="80" priority="701">
       <formula>FIND(5,S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="702">
+    <cfRule type="expression" dxfId="79" priority="702">
       <formula>FIND(4,S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="703">
+    <cfRule type="expression" dxfId="78" priority="703">
       <formula>FIND(3, S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="704">
+    <cfRule type="expression" dxfId="77" priority="704">
       <formula>FIND(2, S20)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="705">
+    <cfRule type="expression" dxfId="76" priority="705">
       <formula>FIND(1, S20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:P16">
-    <cfRule type="containsBlanks" dxfId="76" priority="55">
+    <cfRule type="containsBlanks" dxfId="75" priority="55">
       <formula>LEN(TRIM(F8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF8:AF17">
-    <cfRule type="expression" dxfId="75" priority="1742">
+    <cfRule type="expression" dxfId="74" priority="1742">
       <formula>AND($AF$15=TRUE, SEARCH("6", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="1743">
+    <cfRule type="expression" dxfId="73" priority="1743">
       <formula>AND($AF$10=TRUE, SEARCH("1", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="1744">
+    <cfRule type="expression" dxfId="72" priority="1744">
       <formula>AND($AF$11=TRUE, SEARCH("2", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="1745">
+    <cfRule type="expression" dxfId="71" priority="1745">
       <formula>AND($AF$12=TRUE, SEARCH("3", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="1746">
+    <cfRule type="expression" dxfId="70" priority="1746">
       <formula>AND($AF$13=TRUE, SEARCH("4", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="1747">
+    <cfRule type="expression" dxfId="69" priority="1747">
       <formula>AND($AF$14=TRUE, SEARCH("5", AF8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="1748">
+    <cfRule type="expression" dxfId="68" priority="1748">
       <formula>AND(#REF!=TRUE, SEARCH("7", AF8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AE13 AE17">
-    <cfRule type="expression" dxfId="68" priority="1749">
+    <cfRule type="expression" dxfId="67" priority="1749">
       <formula>AND($AF$8, SEARCH("1", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="1750">
+    <cfRule type="expression" dxfId="66" priority="1750">
       <formula>AND($AF$9, SEARCH("2", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="1751">
+    <cfRule type="expression" dxfId="65" priority="1751">
       <formula>AND($AF$10, SEARCH("3", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="1752">
+    <cfRule type="expression" dxfId="64" priority="1752">
       <formula>AND($AF$11, SEARCH("4", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="1753">
+    <cfRule type="expression" dxfId="63" priority="1753">
       <formula>AND($AF$12, SEARCH("5", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="1754">
+    <cfRule type="expression" dxfId="62" priority="1754">
       <formula>AND($AF$13, SEARCH("6", AE8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="1755">
+    <cfRule type="expression" dxfId="61" priority="1755">
       <formula>AND($AF$17, SEARCH("7", AE8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W6">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="60" priority="12" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",W6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="59" priority="11" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",X6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="58" priority="10" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Y6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z6">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Z6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA6">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="56" priority="8" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AA6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="55" priority="7" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AB6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W23">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="54" priority="6" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",W23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",X23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y23">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="52" priority="4" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Y23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",Z23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="50" priority="2" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AA23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB23">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="W">
+    <cfRule type="containsText" dxfId="49" priority="1" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH("W",AB23)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7567,12 +7997,342 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2CC882-300F-4F9A-9DBD-6F108027CABC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="C2:U20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="1.7"/>
+  <cols>
+    <col min="1" max="16384" width="7.140625" style="148"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="G2" s="162" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="K2" s="162" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="162"/>
+      <c r="M2" s="162"/>
+      <c r="O2" s="162" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="162"/>
+      <c r="Q2" s="162"/>
+    </row>
+    <row r="3" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="162"/>
+      <c r="M3" s="162"/>
+      <c r="O3" s="162"/>
+      <c r="P3" s="162"/>
+      <c r="Q3" s="162"/>
+    </row>
+    <row r="4" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="G4" s="162"/>
+      <c r="H4" s="162"/>
+      <c r="I4" s="162"/>
+      <c r="K4" s="160" t="s">
+        <v>208</v>
+      </c>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="O4" s="162"/>
+      <c r="P4" s="162"/>
+      <c r="Q4" s="162"/>
+    </row>
+    <row r="5" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D5" s="162" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="I5" s="163" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5" s="163"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="163" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="163"/>
+      <c r="R5" s="162" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="162"/>
+      <c r="T5" s="162"/>
+    </row>
+    <row r="6" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
+      <c r="K6" s="160"/>
+      <c r="L6" s="160"/>
+      <c r="M6" s="160"/>
+      <c r="N6" s="163"/>
+      <c r="O6" s="163"/>
+      <c r="R6" s="162"/>
+      <c r="S6" s="162"/>
+      <c r="T6" s="162"/>
+    </row>
+    <row r="7" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163" t="s">
+        <v>215</v>
+      </c>
+      <c r="H7" s="163"/>
+      <c r="P7" s="163" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q7" s="163"/>
+      <c r="R7" s="162"/>
+      <c r="S7" s="162"/>
+      <c r="T7" s="162"/>
+    </row>
+    <row r="8" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
+      <c r="H8" s="163"/>
+      <c r="P8" s="163"/>
+      <c r="Q8" s="163"/>
+      <c r="R8" s="162"/>
+      <c r="S8" s="162"/>
+      <c r="T8" s="162"/>
+    </row>
+    <row r="9" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="C9" s="164" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="164"/>
+      <c r="E9" s="164"/>
+      <c r="F9" s="160" t="s">
+        <v>214</v>
+      </c>
+      <c r="G9" s="160"/>
+      <c r="H9" s="160"/>
+      <c r="P9" s="160" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q9" s="160"/>
+      <c r="R9" s="160"/>
+      <c r="S9" s="164" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9" s="164"/>
+      <c r="U9" s="164"/>
+    </row>
+    <row r="10" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="C10" s="164"/>
+      <c r="D10" s="164"/>
+      <c r="E10" s="164"/>
+      <c r="F10" s="160"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="160"/>
+      <c r="P10" s="160"/>
+      <c r="Q10" s="160"/>
+      <c r="R10" s="160"/>
+      <c r="S10" s="164"/>
+      <c r="T10" s="164"/>
+      <c r="U10" s="164"/>
+    </row>
+    <row r="11" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="C11" s="164"/>
+      <c r="D11" s="164"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="P11" s="160"/>
+      <c r="Q11" s="160"/>
+      <c r="R11" s="160"/>
+      <c r="S11" s="164"/>
+      <c r="T11" s="164"/>
+      <c r="U11" s="164"/>
+    </row>
+    <row r="12" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D12" s="162" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="162"/>
+      <c r="F12" s="162"/>
+      <c r="G12" s="160" t="s">
+        <v>213</v>
+      </c>
+      <c r="H12" s="160"/>
+      <c r="P12" s="160" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q12" s="160"/>
+      <c r="R12" s="162" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" s="162"/>
+      <c r="T12" s="162"/>
+    </row>
+    <row r="13" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D13" s="162"/>
+      <c r="E13" s="162"/>
+      <c r="F13" s="162"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="K13" s="160" t="s">
+        <v>219</v>
+      </c>
+      <c r="L13" s="160"/>
+      <c r="M13" s="160"/>
+      <c r="P13" s="160"/>
+      <c r="Q13" s="160"/>
+      <c r="R13" s="162"/>
+      <c r="S13" s="162"/>
+      <c r="T13" s="162"/>
+    </row>
+    <row r="14" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D14" s="162"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
+      <c r="I14" s="160" t="s">
+        <v>212</v>
+      </c>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
+      <c r="L14" s="160"/>
+      <c r="M14" s="160"/>
+      <c r="N14" s="160" t="s">
+        <v>218</v>
+      </c>
+      <c r="O14" s="160"/>
+      <c r="R14" s="162"/>
+      <c r="S14" s="162"/>
+      <c r="T14" s="162"/>
+    </row>
+    <row r="15" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="D15" s="162"/>
+      <c r="E15" s="162"/>
+      <c r="F15" s="162"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="161" t="s">
+        <v>211</v>
+      </c>
+      <c r="L15" s="161"/>
+      <c r="M15" s="161"/>
+      <c r="N15" s="160"/>
+      <c r="O15" s="160"/>
+      <c r="R15" s="162"/>
+      <c r="S15" s="162"/>
+      <c r="T15" s="162"/>
+    </row>
+    <row r="16" spans="3:21" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="G16" s="162" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="162"/>
+      <c r="I16" s="162"/>
+      <c r="K16" s="161"/>
+      <c r="L16" s="161"/>
+      <c r="M16" s="161"/>
+      <c r="O16" s="162" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" s="162"/>
+      <c r="Q16" s="162"/>
+    </row>
+    <row r="17" spans="7:17" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="G17" s="162"/>
+      <c r="H17" s="162"/>
+      <c r="I17" s="162"/>
+      <c r="K17" s="162" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" s="162"/>
+      <c r="M17" s="162"/>
+      <c r="O17" s="162"/>
+      <c r="P17" s="162"/>
+      <c r="Q17" s="162"/>
+    </row>
+    <row r="18" spans="7:17" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="G18" s="162"/>
+      <c r="H18" s="162"/>
+      <c r="I18" s="162"/>
+      <c r="K18" s="162"/>
+      <c r="L18" s="162"/>
+      <c r="M18" s="162"/>
+      <c r="O18" s="162"/>
+      <c r="P18" s="162"/>
+      <c r="Q18" s="162"/>
+    </row>
+    <row r="19" spans="7:17" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="K19" s="162" t="s">
+        <v>44</v>
+      </c>
+      <c r="L19" s="162"/>
+      <c r="M19" s="162"/>
+    </row>
+    <row r="20" spans="7:17" ht="37.5" customHeight="1" x14ac:dyDescent="1.7">
+      <c r="K20" s="162"/>
+      <c r="L20" s="162"/>
+      <c r="M20" s="162"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="K2:M3"/>
+    <mergeCell ref="O2:Q4"/>
+    <mergeCell ref="G2:I4"/>
+    <mergeCell ref="R5:T8"/>
+    <mergeCell ref="D5:F8"/>
+    <mergeCell ref="S9:U11"/>
+    <mergeCell ref="C9:E11"/>
+    <mergeCell ref="R12:T15"/>
+    <mergeCell ref="D12:F15"/>
+    <mergeCell ref="O16:Q18"/>
+    <mergeCell ref="G16:I18"/>
+    <mergeCell ref="K17:M18"/>
+    <mergeCell ref="P12:Q13"/>
+    <mergeCell ref="G12:H13"/>
+    <mergeCell ref="N14:O15"/>
+    <mergeCell ref="N5:O6"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="P9:R11"/>
+    <mergeCell ref="F9:H11"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="K15:M16"/>
+    <mergeCell ref="K13:M14"/>
+    <mergeCell ref="K19:M20"/>
+    <mergeCell ref="K4:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="42" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BO94"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -7595,7 +8355,7 @@
   <sheetData>
     <row r="1" spans="1:67" s="3" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>20</v>
@@ -7607,21 +8367,21 @@
         <v>68</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="164" t="s">
+      <c r="F1" s="170" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="165"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="160" t="s">
+      <c r="G1" s="171"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="160"/>
-      <c r="K1" s="160"/>
-      <c r="L1" s="160"/>
-      <c r="M1" s="160"/>
-      <c r="N1" s="160"/>
-      <c r="O1" s="160"/>
-      <c r="P1" s="160"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
       <c r="Q1"/>
       <c r="R1"/>
       <c r="S1"/>
@@ -7738,7 +8498,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="113" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I2" s="112" t="s">
         <v>65</v>
@@ -7858,11 +8618,11 @@
       <c r="D3" s="9">
         <v>10</v>
       </c>
-      <c r="F3" s="161" t="s">
+      <c r="F3" s="167" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="162"/>
-      <c r="H3" s="163"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="169"/>
       <c r="I3" s="74" t="s">
         <v>34</v>
       </c>
@@ -7871,27 +8631,27 @@
         <v>1</v>
       </c>
       <c r="K3" s="5" t="str">
-        <f>IF(J4=0,"",IF(VLOOKUP($G$4,$Q$22:$X$45,1+K2,FALSE)=0,K2,VLOOKUP($G$4,$Q$22:$X$45,1+K2,FALSE)))</f>
+        <f t="shared" ref="K3:P3" si="0">IF(J4=0,"",IF(VLOOKUP($G$4,$Q$22:$X$45,1+K2,FALSE)=0,K2,VLOOKUP($G$4,$Q$22:$X$45,1+K2,FALSE)))</f>
         <v/>
       </c>
       <c r="L3" s="5">
-        <f>IF(K4=0,"",IF(VLOOKUP($G$4,$Q$22:$X$45,1+L2,FALSE)=0,L2,VLOOKUP($G$4,$Q$22:$X$45,1+L2,FALSE)))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="M3" s="5" t="str">
-        <f>IF(L4=0,"",IF(VLOOKUP($G$4,$Q$22:$X$45,1+M2,FALSE)=0,M2,VLOOKUP($G$4,$Q$22:$X$45,1+M2,FALSE)))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N3" s="5">
-        <f>IF(M4=0,"",IF(VLOOKUP($G$4,$Q$22:$X$45,1+N2,FALSE)=0,N2,VLOOKUP($G$4,$Q$22:$X$45,1+N2,FALSE)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="O3" s="5" t="str">
-        <f>IF(N4=0,"",IF(VLOOKUP($G$4,$Q$22:$X$45,1+O2,FALSE)=0,O2,VLOOKUP($G$4,$Q$22:$X$45,1+O2,FALSE)))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="P3" s="79" t="str">
-        <f>IF(O4=0,"",IF(VLOOKUP($G$4,$Q$22:$X$45,1+P2,FALSE)=0,P2,VLOOKUP($G$4,$Q$22:$X$45,1+P2,FALSE)))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="Y3" s="74">
@@ -8095,40 +8855,40 @@
       <c r="D5" s="9">
         <v>8</v>
       </c>
-      <c r="F5" s="161" t="s">
+      <c r="F5" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="162"/>
-      <c r="H5" s="163"/>
+      <c r="G5" s="168"/>
+      <c r="H5" s="169"/>
       <c r="I5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" ref="J5:P5" si="0">IFERROR(VLOOKUP(J6, $B$2:$D$37, 3, FALSE), "")</f>
+        <f t="shared" ref="J5:P5" si="1">IFERROR(VLOOKUP(J6, $B$2:$D$37, 3, FALSE), "")</f>
         <v>0</v>
       </c>
       <c r="K5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L5" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="M5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N5" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="O5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="P5" s="79" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Y5" s="74">
@@ -8180,7 +8940,7 @@
         <v>91</v>
       </c>
       <c r="BD5" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BE5" s="6" t="s">
         <v>82</v>
@@ -8312,13 +9072,13 @@
         <v>96</v>
       </c>
       <c r="BH6" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BI6" s="6" t="s">
         <v>97</v>
       </c>
       <c r="BJ6" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BK6" s="6" t="s">
         <v>91</v>
@@ -8347,7 +9107,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J7" s="5" t="str">
         <f>Model!J6 &amp; HLOOKUP(Model!J2, Model!$Q$48:$X$72, MATCH(Model!$G$4, Model!$Q$49:$Q$72, 0) + 1)</f>
@@ -8457,7 +9217,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J8" s="101" t="b">
         <f>Fretboards!AF8</f>
@@ -8570,16 +9330,16 @@
       <c r="D9" s="9">
         <v>13</v>
       </c>
-      <c r="I9" s="159" t="s">
+      <c r="I9" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
+      <c r="J9" s="165"/>
+      <c r="K9" s="165"/>
+      <c r="L9" s="165"/>
+      <c r="M9" s="165"/>
+      <c r="N9" s="165"/>
+      <c r="O9" s="165"/>
+      <c r="P9" s="165"/>
       <c r="Y9" s="74">
         <v>8</v>
       </c>
@@ -8683,14 +9443,14 @@
       <c r="D10" s="5">
         <v>10</v>
       </c>
-      <c r="I10" s="160"/>
-      <c r="J10" s="160"/>
-      <c r="K10" s="160"/>
-      <c r="L10" s="160"/>
-      <c r="M10" s="160"/>
-      <c r="N10" s="160"/>
-      <c r="O10" s="160"/>
-      <c r="P10" s="160"/>
+      <c r="I10" s="166"/>
+      <c r="J10" s="166"/>
+      <c r="K10" s="166"/>
+      <c r="L10" s="166"/>
+      <c r="M10" s="166"/>
+      <c r="N10" s="166"/>
+      <c r="O10" s="166"/>
+      <c r="P10" s="166"/>
       <c r="Y10" s="74">
         <v>9</v>
       </c>
@@ -8909,27 +9669,27 @@
         <v>1</v>
       </c>
       <c r="K12" s="5">
-        <f>IF(J13=0,"",IF(VLOOKUP($G$6,$Q$22:$X$45,1+K2,FALSE)=0,K2,VLOOKUP($G$6,$Q$22:$X$45,1+K2,FALSE)))</f>
+        <f t="shared" ref="K12:P12" si="2">IF(J13=0,"",IF(VLOOKUP($G$6,$Q$22:$X$45,1+K2,FALSE)=0,K2,VLOOKUP($G$6,$Q$22:$X$45,1+K2,FALSE)))</f>
         <v>2</v>
       </c>
       <c r="L12" s="5" t="str">
-        <f>IF(K13=0,"",IF(VLOOKUP($G$6,$Q$22:$X$45,1+L2,FALSE)=0,L2,VLOOKUP($G$6,$Q$22:$X$45,1+L2,FALSE)))</f>
+        <f t="shared" si="2"/>
         <v>♭3</v>
       </c>
       <c r="M12" s="5">
-        <f>IF(L13=0,"",IF(VLOOKUP($G$6,$Q$22:$X$45,1+M2,FALSE)=0,M2,VLOOKUP($G$6,$Q$22:$X$45,1+M2,FALSE)))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="N12" s="5">
-        <f>IF(M13=0,"",IF(VLOOKUP($G$6,$Q$22:$X$45,1+N2,FALSE)=0,N2,VLOOKUP($G$6,$Q$22:$X$45,1+N2,FALSE)))</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O12" s="5" t="str">
-        <f>IF(N13=0,"",IF(VLOOKUP($G$6,$Q$22:$X$45,1+O2,FALSE)=0,O2,VLOOKUP($G$6,$Q$22:$X$45,1+O2,FALSE)))</f>
+        <f t="shared" si="2"/>
         <v>♭6</v>
       </c>
       <c r="P12" s="79" t="str">
-        <f>IF(O13=0,"",IF(VLOOKUP($G$6,$Q$22:$X$45,1+P2,FALSE)=0,P2,VLOOKUP($G$6,$Q$22:$X$45,1+P2,FALSE)))</f>
+        <f t="shared" si="2"/>
         <v>♭7</v>
       </c>
       <c r="Y12" s="74">
@@ -9134,22 +9894,22 @@
         <v>97</v>
       </c>
       <c r="BI13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="BJ13" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="BL13" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="BJ13" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="BK13" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="BL13" s="6" t="s">
-        <v>137</v>
       </c>
       <c r="BM13" s="6" t="s">
         <v>120</v>
       </c>
       <c r="BN13" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="BO13" s="6" t="s">
         <v>93</v>
@@ -9172,31 +9932,31 @@
         <v>67</v>
       </c>
       <c r="J14" s="72">
-        <f t="shared" ref="J14:P14" si="1">IFERROR(VLOOKUP(J15, $B$2:$D$37, 3, FALSE), "")</f>
+        <f t="shared" ref="J14:P14" si="3">IFERROR(VLOOKUP(J15, $B$2:$D$37, 3, FALSE), "")</f>
         <v>4</v>
       </c>
       <c r="K14" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L14" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="M14" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="N14" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="O14" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P14" s="80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Y14" s="74">
@@ -9427,7 +10187,7 @@
         <v>10</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J16" s="5" t="str">
         <f>Model!J15 &amp; HLOOKUP(Model!J11, Model!$Q$48:$X$72, MATCH(Model!$G$6, Model!$Q$49:$Q$72, 0) + 1)</f>
@@ -9513,7 +10273,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J17" s="101" t="b">
         <f>HLOOKUP(Fretboards!F$1, $R$75:$X$85, MATCH($H$6, $Q$75:$Q$85, 0))</f>
@@ -9642,25 +10402,25 @@
         <v>17</v>
       </c>
       <c r="J21" s="95" t="s">
+        <v>180</v>
+      </c>
+      <c r="K21" s="95" t="s">
+        <v>181</v>
+      </c>
+      <c r="L21" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="K21" s="95" t="s">
+      <c r="M21" s="95" t="s">
         <v>183</v>
       </c>
-      <c r="L21" s="95" t="s">
+      <c r="N21" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="M21" s="95" t="s">
+      <c r="O21" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="N21" s="95" t="s">
+      <c r="P21" s="98" t="s">
         <v>186</v>
-      </c>
-      <c r="O21" s="95" t="s">
-        <v>187</v>
-      </c>
-      <c r="P21" s="98" t="s">
-        <v>188</v>
       </c>
       <c r="Q21" s="91" t="s">
         <v>34</v>
@@ -9920,7 +10680,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="81" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J27" s="5">
         <v>2</v>
@@ -9944,7 +10704,7 @@
         <v>2</v>
       </c>
       <c r="Q27" s="81" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T27" t="s">
         <v>70</v>
@@ -10198,7 +10958,7 @@
         <v>7</v>
       </c>
       <c r="I33" s="81" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J33" s="5">
         <v>2</v>
@@ -10222,7 +10982,7 @@
         <v>1</v>
       </c>
       <c r="Q33" s="81" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="W33" t="s">
         <v>73</v>
@@ -10282,7 +11042,7 @@
         <v>5</v>
       </c>
       <c r="I35" s="81" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J35" s="5">
         <v>1</v>
@@ -10306,7 +11066,7 @@
         <v>1</v>
       </c>
       <c r="Q35" s="81" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="S35" t="s">
         <v>74</v>
@@ -10327,7 +11087,7 @@
         <v>8</v>
       </c>
       <c r="I36" s="81" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J36" s="5">
         <v>3</v>
@@ -10351,10 +11111,10 @@
         <v>2</v>
       </c>
       <c r="Q36" s="81" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="S36" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U36" t="s">
         <v>75</v>
@@ -10374,7 +11134,7 @@
         <v>9</v>
       </c>
       <c r="I37" s="81" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J37" s="5">
         <v>1</v>
@@ -10398,7 +11158,7 @@
         <v>1</v>
       </c>
       <c r="Q37" s="81" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S37" t="s">
         <v>74</v>
@@ -10413,7 +11173,7 @@
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I38" s="81" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J38" s="5">
         <v>1</v>
@@ -10437,7 +11197,7 @@
         <v>1</v>
       </c>
       <c r="Q38" s="81" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="S38" t="s">
         <v>74</v>
@@ -10449,7 +11209,7 @@
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I39" s="81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J39" s="5">
         <v>1</v>
@@ -10473,7 +11233,7 @@
         <v>1</v>
       </c>
       <c r="Q39" s="81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="S39" t="s">
         <v>74</v>
@@ -10488,7 +11248,7 @@
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I40" s="81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J40" s="5">
         <v>0</v>
@@ -10512,7 +11272,7 @@
         <v>2</v>
       </c>
       <c r="Q40" s="81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="T40" t="s">
         <v>70</v>
@@ -10521,12 +11281,12 @@
         <v>71</v>
       </c>
       <c r="X40" s="87" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I41" s="81" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J41" s="5">
         <v>3</v>
@@ -10550,19 +11310,19 @@
         <v>1</v>
       </c>
       <c r="Q41" s="81" t="s">
+        <v>148</v>
+      </c>
+      <c r="S41" t="s">
+        <v>151</v>
+      </c>
+      <c r="W41" t="s">
         <v>150</v>
-      </c>
-      <c r="S41" t="s">
-        <v>153</v>
-      </c>
-      <c r="W41" t="s">
-        <v>152</v>
       </c>
       <c r="X41" s="87"/>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I42" s="81" t="s">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="J42" s="5">
         <v>0</v>
@@ -10586,13 +11346,13 @@
         <v>1</v>
       </c>
       <c r="Q42" s="81" t="s">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="X42" s="87"/>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I43" s="81" t="s">
-        <v>131</v>
+        <v>221</v>
       </c>
       <c r="J43" s="5">
         <v>0</v>
@@ -10616,7 +11376,7 @@
         <v>2</v>
       </c>
       <c r="Q43" s="81" t="s">
-        <v>131</v>
+        <v>221</v>
       </c>
       <c r="T43" t="s">
         <v>70</v>
@@ -10627,7 +11387,7 @@
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I44" s="81" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J44" s="5">
         <v>0</v>
@@ -10651,13 +11411,13 @@
         <v>5</v>
       </c>
       <c r="Q44" s="81" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="X44" s="87"/>
     </row>
     <row r="45" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I45" s="83" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J45" s="84">
         <v>0</v>
@@ -10681,7 +11441,7 @@
         <v>5</v>
       </c>
       <c r="Q45" s="83" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R45" s="96"/>
       <c r="S45" s="96"/>
@@ -10697,7 +11457,7 @@
     <row r="47" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="2:24" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I48" s="91" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J48" s="92">
         <v>1</v>
@@ -10721,7 +11481,7 @@
         <v>7</v>
       </c>
       <c r="Q48" s="91" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R48" s="92">
         <v>1</v>
@@ -10774,25 +11534,25 @@
         <v>129</v>
       </c>
       <c r="R49" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S49" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T49" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U49" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V49" s="73">
         <v>7</v>
       </c>
       <c r="W49" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="X49" s="86" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="9:24" x14ac:dyDescent="0.25">
@@ -10824,25 +11584,25 @@
         <v>23</v>
       </c>
       <c r="R50" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S50" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T50" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U50" s="73">
         <v>7</v>
       </c>
       <c r="V50" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W50" s="73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="X50" s="86" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="9:24" x14ac:dyDescent="0.25">
@@ -10874,25 +11634,25 @@
         <v>24</v>
       </c>
       <c r="R51" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S51" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="T51" s="73">
         <v>7</v>
       </c>
       <c r="U51" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V51" s="73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="W51" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="X51" s="86" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="9:24" x14ac:dyDescent="0.25">
@@ -10924,25 +11684,25 @@
         <v>22</v>
       </c>
       <c r="R52" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S52" s="73">
         <v>7</v>
       </c>
       <c r="T52" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U52" s="73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="V52" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="W52" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="X52" s="86" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="9:24" x14ac:dyDescent="0.25">
@@ -10977,27 +11737,27 @@
         <v>7</v>
       </c>
       <c r="S53" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T53" s="73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="U53" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V53" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W53" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="X53" s="86" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I54" s="81" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J54" s="5" t="b">
         <v>1</v>
@@ -11021,25 +11781,25 @@
         <v>1</v>
       </c>
       <c r="Q54" s="81" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="R54" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S54" s="73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="T54" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U54" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V54" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W54" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="X54" s="86">
         <v>7</v>
@@ -11074,25 +11834,25 @@
         <v>25</v>
       </c>
       <c r="R55" s="73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="S55" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="T55" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U55" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V55" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="W55" s="73">
         <v>7</v>
       </c>
       <c r="X55" s="86" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="9:24" x14ac:dyDescent="0.25">
@@ -11124,23 +11884,23 @@
         <v>33</v>
       </c>
       <c r="R56" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S56" s="73"/>
       <c r="T56" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="U56" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="V56" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="W56" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="U56" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="V56" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="W56" s="73" t="s">
-        <v>142</v>
-      </c>
       <c r="X56" s="86" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="9:24" x14ac:dyDescent="0.25">
@@ -11172,17 +11932,17 @@
         <v>77</v>
       </c>
       <c r="R57" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S57" s="73"/>
       <c r="T57" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="U57" s="73" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="V57" s="73" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="W57" s="73"/>
       <c r="X57" s="86">
@@ -11218,20 +11978,20 @@
         <v>76</v>
       </c>
       <c r="R58" s="73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S58" s="73" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="T58" s="73" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="U58" s="73"/>
       <c r="V58" s="73">
         <v>5</v>
       </c>
       <c r="W58" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="X58" s="86"/>
     </row>
@@ -11264,75 +12024,75 @@
         <v>30</v>
       </c>
       <c r="R59" s="73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S59" s="73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T59" s="73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="U59" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="V59" s="73">
         <v>7</v>
       </c>
       <c r="W59" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="X59" s="86" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I60" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="J60" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L60" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O60" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P60" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="R60" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="S60" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="T60" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="U60" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="V60" s="73" t="s">
+        <v>170</v>
+      </c>
+      <c r="W60" s="73" t="s">
+        <v>163</v>
+      </c>
+      <c r="X60" s="86" t="s">
         <v>171</v>
-      </c>
-      <c r="J60" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L60" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O60" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P60" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q60" s="81" t="s">
-        <v>171</v>
-      </c>
-      <c r="R60" s="73" t="s">
-        <v>142</v>
-      </c>
-      <c r="S60" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="T60" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="U60" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="V60" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="W60" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="X60" s="86" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="61" spans="9:24" x14ac:dyDescent="0.25">
@@ -11364,13 +12124,13 @@
         <v>29</v>
       </c>
       <c r="R61" s="73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S61" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="T61" s="73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U61" s="73">
         <v>7</v>
@@ -11379,215 +12139,215 @@
         <v>7</v>
       </c>
       <c r="W61" s="73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="X61" s="86" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I62" s="81" t="s">
+        <v>177</v>
+      </c>
+      <c r="J62" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K62" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L62" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M62" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N62" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O62" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P62" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="81" t="s">
+        <v>177</v>
+      </c>
+      <c r="R62" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="S62" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="T62" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="U62" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="V62" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="J62" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K62" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L62" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M62" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N62" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O62" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P62" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q62" s="81" t="s">
-        <v>179</v>
-      </c>
-      <c r="R62" s="73" t="s">
-        <v>142</v>
-      </c>
-      <c r="S62" s="73" t="s">
-        <v>142</v>
-      </c>
-      <c r="T62" s="73" t="s">
-        <v>180</v>
-      </c>
-      <c r="U62" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="V62" s="73" t="s">
-        <v>181</v>
-      </c>
       <c r="W62" s="73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="X62" s="86" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I63" s="81" t="s">
+        <v>172</v>
+      </c>
+      <c r="J63" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K63" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L63" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M63" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N63" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O63" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P63" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="81" t="s">
+        <v>172</v>
+      </c>
+      <c r="R63" s="73" t="s">
+        <v>170</v>
+      </c>
+      <c r="S63" s="73" t="s">
+        <v>171</v>
+      </c>
+      <c r="T63" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="U63" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="V63" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="J63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N63" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O63" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P63" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q63" s="81" t="s">
-        <v>174</v>
-      </c>
-      <c r="R63" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="S63" s="73" t="s">
-        <v>173</v>
-      </c>
-      <c r="T63" s="73" t="s">
+      <c r="W63" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="X63" s="86" t="s">
         <v>175</v>
-      </c>
-      <c r="U63" s="73" t="s">
-        <v>147</v>
-      </c>
-      <c r="V63" s="73" t="s">
-        <v>176</v>
-      </c>
-      <c r="W63" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="X63" s="86" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="64" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I64" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="J64" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K64" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L64" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M64" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N64" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O64" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P64" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="R64" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="S64" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="T64" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="U64" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="V64" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="J64" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K64" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L64" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M64" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N64" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O64" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P64" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q64" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="R64" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="S64" s="73" t="s">
-        <v>142</v>
-      </c>
-      <c r="T64" s="73" t="s">
+      <c r="W64" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="X64" s="86" t="s">
         <v>160</v>
-      </c>
-      <c r="U64" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="V64" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="W64" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="X64" s="86" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="65" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I65" s="81" t="s">
+        <v>161</v>
+      </c>
+      <c r="J65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M65" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N65" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P65" s="82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="81" t="s">
+        <v>161</v>
+      </c>
+      <c r="R65" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="S65" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="J65" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K65" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L65" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M65" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N65" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O65" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P65" s="82" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="81" t="s">
-        <v>163</v>
-      </c>
-      <c r="R65" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="S65" s="73" t="s">
+      <c r="T65" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="U65" s="73" t="s">
+        <v>159</v>
+      </c>
+      <c r="V65" s="73" t="s">
         <v>165</v>
       </c>
-      <c r="T65" s="73" t="s">
+      <c r="W65" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="X65" s="86" t="s">
         <v>166</v>
-      </c>
-      <c r="U65" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="V65" s="73" t="s">
-        <v>167</v>
-      </c>
-      <c r="W65" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="X65" s="86" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="66" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I66" s="81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J66" s="5" t="b">
         <v>1</v>
@@ -11611,33 +12371,33 @@
         <v>1</v>
       </c>
       <c r="Q66" s="81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="R66" s="73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="S66" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="T66" s="73" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U66" s="73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="V66" s="73" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="W66" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="X66" s="86" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I67" s="81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J67" s="5" t="b">
         <v>1</v>
@@ -11661,27 +12421,27 @@
         <v>1</v>
       </c>
       <c r="Q67" s="81" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R67" s="73" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S67" s="73"/>
       <c r="T67" s="73" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="U67" s="73"/>
       <c r="V67" s="73" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="W67" s="73"/>
       <c r="X67" s="86" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I68" s="81" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J68" s="5" t="b">
         <v>1</v>
@@ -11705,23 +12465,23 @@
         <v>1</v>
       </c>
       <c r="Q68" s="81" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="R68" s="73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="S68" s="73" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="T68" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U68" s="73"/>
       <c r="V68" s="73" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="W68" s="73" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="X68" s="86">
         <v>6</v>
@@ -11729,7 +12489,7 @@
     </row>
     <row r="69" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I69" s="81" t="s">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="J69" s="5" t="b">
         <v>1</v>
@@ -11753,14 +12513,14 @@
         <v>1</v>
       </c>
       <c r="Q69" s="81" t="s">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="R69" s="73" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S69" s="73"/>
       <c r="T69" s="73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U69" s="73"/>
       <c r="V69" s="73">
@@ -11768,98 +12528,98 @@
       </c>
       <c r="W69" s="73"/>
       <c r="X69" s="86" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I70" s="81" t="s">
-        <v>131</v>
-      </c>
-      <c r="J70" s="167" t="b">
-        <v>1</v>
-      </c>
-      <c r="K70" s="167" t="b">
-        <v>0</v>
-      </c>
-      <c r="L70" s="167" t="b">
-        <v>1</v>
-      </c>
-      <c r="M70" s="167" t="b">
-        <v>0</v>
-      </c>
-      <c r="N70" s="167" t="b">
-        <v>1</v>
-      </c>
-      <c r="O70" s="167" t="b">
+        <v>221</v>
+      </c>
+      <c r="J70" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L70" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N70" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O70" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P70" s="82" t="b">
         <v>1</v>
       </c>
       <c r="Q70" s="81" t="s">
-        <v>131</v>
-      </c>
-      <c r="R70" s="168" t="s">
-        <v>141</v>
-      </c>
-      <c r="S70" s="168"/>
-      <c r="T70" s="168" t="s">
-        <v>142</v>
-      </c>
-      <c r="U70" s="168"/>
-      <c r="V70" s="168" t="s">
-        <v>141</v>
-      </c>
-      <c r="W70" s="168"/>
+        <v>221</v>
+      </c>
+      <c r="R70" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="S70" s="73"/>
+      <c r="T70" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="U70" s="73"/>
+      <c r="V70" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="W70" s="73"/>
       <c r="X70" s="86">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="9:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I71" s="81" t="s">
-        <v>208</v>
-      </c>
-      <c r="J71" s="167" t="b">
-        <v>1</v>
-      </c>
-      <c r="K71" s="167" t="b">
-        <v>0</v>
-      </c>
-      <c r="L71" s="167" t="b">
-        <v>1</v>
-      </c>
-      <c r="M71" s="167" t="b">
-        <v>0</v>
-      </c>
-      <c r="N71" s="167" t="b">
-        <v>1</v>
-      </c>
-      <c r="O71" s="167" t="b">
+        <v>206</v>
+      </c>
+      <c r="J71" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K71" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L71" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M71" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N71" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O71" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P71" s="82" t="b">
         <v>0</v>
       </c>
       <c r="Q71" s="81" t="s">
-        <v>208</v>
-      </c>
-      <c r="R71" s="168" t="s">
-        <v>142</v>
-      </c>
-      <c r="S71" s="168"/>
-      <c r="T71" s="168" t="s">
-        <v>141</v>
-      </c>
-      <c r="U71" s="168"/>
-      <c r="V71" s="168">
+        <v>206</v>
+      </c>
+      <c r="R71" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="S71" s="73"/>
+      <c r="T71" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="U71" s="73"/>
+      <c r="V71" s="73">
         <v>7</v>
       </c>
-      <c r="W71" s="168"/>
+      <c r="W71" s="73"/>
       <c r="X71" s="86"/>
     </row>
     <row r="72" spans="9:24" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I72" s="83" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J72" s="84" t="b">
         <v>1</v>
@@ -11883,18 +12643,18 @@
         <v>0</v>
       </c>
       <c r="Q72" s="83" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R72" s="88" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S72" s="88"/>
       <c r="T72" s="88" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U72" s="88"/>
       <c r="V72" s="88" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W72" s="88"/>
       <c r="X72" s="94"/>
@@ -11903,7 +12663,7 @@
     <row r="74" spans="9:24" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="9:24" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I75" s="104" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J75" s="105">
         <v>1</v>
@@ -11927,7 +12687,7 @@
         <v>7</v>
       </c>
       <c r="Q75" s="104" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R75" s="105">
         <v>1</v>
@@ -11953,7 +12713,7 @@
     </row>
     <row r="76" spans="9:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I76" s="110" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J76" s="6" t="b">
         <f>HLOOKUP(Fretboards!F$1, Model!$J$48:$P$72, MATCH($G$4, Model!$I$48:$I$72, 0))</f>
@@ -11984,7 +12744,7 @@
         <v>0</v>
       </c>
       <c r="Q76" s="110" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R76" s="6" t="b">
         <f>HLOOKUP(R75, Model!$J$48:$P$72, MATCH($G$6, Model!$I$48:$I$72, 0))</f>
@@ -12017,7 +12777,7 @@
     </row>
     <row r="77" spans="9:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I77" s="110" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J77" s="6" t="b">
         <v>1</v>
@@ -12041,7 +12801,7 @@
         <v>1</v>
       </c>
       <c r="Q77" s="110" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="R77" s="6" t="b">
         <v>1</v>
@@ -12067,7 +12827,7 @@
     </row>
     <row r="78" spans="9:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I78" s="110" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J78" s="6" t="b">
         <v>1</v>
@@ -12091,7 +12851,7 @@
         <v>0</v>
       </c>
       <c r="Q78" s="110" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R78" s="6" t="b">
         <v>1</v>
@@ -12117,7 +12877,7 @@
     </row>
     <row r="79" spans="9:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I79" s="110" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J79" s="6" t="b">
         <v>0</v>
@@ -12141,7 +12901,7 @@
         <v>1</v>
       </c>
       <c r="Q79" s="110" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="R79" s="6" t="b">
         <v>0</v>
@@ -12167,7 +12927,7 @@
     </row>
     <row r="80" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I80" s="110" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J80" s="6" t="b">
         <v>1</v>
@@ -12191,7 +12951,7 @@
         <v>0</v>
       </c>
       <c r="Q80" s="110" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="R80" s="6" t="b">
         <v>1</v>
@@ -12217,7 +12977,7 @@
     </row>
     <row r="81" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I81" s="110" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J81" s="6" t="b">
         <v>0</v>
@@ -12241,7 +13001,7 @@
         <v>1</v>
       </c>
       <c r="Q81" s="110" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="R81" s="6" t="b">
         <v>0</v>
@@ -12267,7 +13027,7 @@
     </row>
     <row r="82" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I82" s="110" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J82" s="6" t="b">
         <v>1</v>
@@ -12291,7 +13051,7 @@
         <v>0</v>
       </c>
       <c r="Q82" s="110" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R82" s="6" t="b">
         <v>1</v>
@@ -12317,7 +13077,7 @@
     </row>
     <row r="83" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I83" s="110" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J83" s="6" t="b">
         <v>0</v>
@@ -12341,7 +13101,7 @@
         <v>1</v>
       </c>
       <c r="Q83" s="110" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R83" s="6" t="b">
         <v>0</v>
@@ -12367,7 +13127,7 @@
     </row>
     <row r="84" spans="9:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I84" s="110" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J84" s="6" t="b">
         <v>1</v>
@@ -12391,7 +13151,7 @@
         <v>1</v>
       </c>
       <c r="Q84" s="110" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R84" s="6" t="b">
         <v>1</v>
@@ -12417,7 +13177,7 @@
     </row>
     <row r="85" spans="9:24" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I85" s="111" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J85" s="108" t="b">
         <v>0</v>
@@ -12441,7 +13201,7 @@
         <v>0</v>
       </c>
       <c r="Q85" s="111" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R85" s="108" t="b">
         <v>0</v>
@@ -12495,7 +13255,7 @@
     </row>
     <row r="89" spans="9:24" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I89" s="129" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J89" s="116"/>
       <c r="K89" s="117"/>
@@ -12511,7 +13271,7 @@
     </row>
     <row r="91" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I91" s="129" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J91" s="116"/>
       <c r="K91" s="125"/>
@@ -12527,7 +13287,7 @@
     </row>
     <row r="93" spans="9:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I93" s="133" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J93" s="134"/>
       <c r="K93" s="135"/>
@@ -12547,48 +13307,48 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="J17:P17">
-    <cfRule type="expression" dxfId="26" priority="57">
+    <cfRule type="expression" dxfId="13" priority="57">
       <formula>AND($O$8=TRUE, SEARCH("6", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="58">
+    <cfRule type="expression" dxfId="12" priority="58">
       <formula>AND($J$8=TRUE, SEARCH("1", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="59">
+    <cfRule type="expression" dxfId="11" priority="59">
       <formula>AND($K$8=TRUE, SEARCH("2", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="60">
+    <cfRule type="expression" dxfId="10" priority="60">
       <formula>AND($L$8=TRUE, SEARCH("3", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="61">
+    <cfRule type="expression" dxfId="9" priority="61">
       <formula>AND($M$8=TRUE, SEARCH("4", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="62">
+    <cfRule type="expression" dxfId="8" priority="62">
       <formula>AND($N$8=TRUE, SEARCH("5", J17))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="63">
+    <cfRule type="expression" dxfId="7" priority="63">
       <formula>AND($P$8=TRUE, SEARCH("7", J17))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="expression" dxfId="19" priority="1709">
+    <cfRule type="expression" dxfId="6" priority="1709">
       <formula>AND($K$23=TRUE, SEARCH("6", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="1710">
+    <cfRule type="expression" dxfId="5" priority="1710">
       <formula>AND($E$21=TRUE, SEARCH("1", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="1711">
+    <cfRule type="expression" dxfId="4" priority="1711">
       <formula>AND($F$21=TRUE, SEARCH("2", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="1712">
+    <cfRule type="expression" dxfId="3" priority="1712">
       <formula>AND($G$21=TRUE, SEARCH("3", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="1713">
+    <cfRule type="expression" dxfId="2" priority="1713">
       <formula>AND($I$23=TRUE, SEARCH("4", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="1714">
+    <cfRule type="expression" dxfId="1" priority="1714">
       <formula>AND($J$23=TRUE, SEARCH("5", J8))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="1715">
+    <cfRule type="expression" dxfId="0" priority="1715">
       <formula>AND($L$23=TRUE, SEARCH("7", J8))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>